<commit_message>
initialized variables and equations for a more accurate projectile model
</commit_message>
<xml_diff>
--- a/models.xlsx
+++ b/models.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssb\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CD74023-5D52-4720-A112-3CC962FB7968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B44BE0-0253-4828-AD19-D5E54D73E2E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6422CA17-FA72-4B85-908A-20157EF2E374}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{6422CA17-FA72-4B85-908A-20157EF2E374}"/>
   </bookViews>
   <sheets>
     <sheet name="model 1" sheetId="1" r:id="rId1"/>
+    <sheet name="model 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <r>
       <t>launch angle/</t>
@@ -186,6 +187,45 @@
       </rPr>
       <t>-1</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <t>launch elevation/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>°</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t>θ)</t>
+    </r>
+  </si>
+  <si>
+    <t>launch elevation/c(θ)</t>
+  </si>
+  <si>
+    <t>range/m(R)</t>
   </si>
 </sst>
 </file>
@@ -342,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -354,6 +394,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5902,8 +5944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A0679C-E006-47C6-B970-B6CA34D7885D}">
   <dimension ref="B2:J315"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14106,4 +14148,462 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CCE5E17-412F-4B65-BE92-5E427918CCA8}">
+  <dimension ref="B2:G79"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1">
+        <v>42</v>
+      </c>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3">
+        <f>($C2*PI()/180)</f>
+        <v>0.73303828583761843</v>
+      </c>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="2:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>10</v>
+      </c>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="2:7" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>9.81</v>
+      </c>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="3">
+        <f>(($C$4*$C$4)/$C$6)*(SIN($C$3)*COS($C$3)+COS($C$3)*SQRT((SIN($C$3)*SIN($C$3)+((2*$C$6*$C$5)/($C$4*$C$4)))))</f>
+        <v>11.147829102248627</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B10" s="11"/>
+      <c r="C10" s="12"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="11"/>
+      <c r="C11" s="12"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="11"/>
+      <c r="C12" s="12"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+    </row>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+    </row>
+    <row r="18" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+    </row>
+    <row r="19" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+    </row>
+    <row r="20" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+    </row>
+    <row r="21" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+    </row>
+    <row r="22" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+    </row>
+    <row r="23" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E23" s="11"/>
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+    </row>
+    <row r="24" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E24" s="11"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="11"/>
+    </row>
+    <row r="25" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="11"/>
+    </row>
+    <row r="26" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+    </row>
+    <row r="27" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E27" s="11"/>
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+    </row>
+    <row r="28" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+    </row>
+    <row r="29" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+    </row>
+    <row r="30" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+      <c r="G30" s="11"/>
+    </row>
+    <row r="31" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+    </row>
+    <row r="32" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E32" s="11"/>
+      <c r="F32" s="11"/>
+      <c r="G32" s="11"/>
+    </row>
+    <row r="33" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+    </row>
+    <row r="34" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E34" s="11"/>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11"/>
+    </row>
+    <row r="35" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+    </row>
+    <row r="36" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E36" s="11"/>
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E37" s="11"/>
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+    </row>
+    <row r="38" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="11"/>
+    </row>
+    <row r="39" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+    </row>
+    <row r="40" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E40" s="11"/>
+      <c r="F40" s="11"/>
+      <c r="G40" s="11"/>
+    </row>
+    <row r="41" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+    </row>
+    <row r="42" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E42" s="11"/>
+      <c r="F42" s="11"/>
+      <c r="G42" s="11"/>
+    </row>
+    <row r="43" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+    </row>
+    <row r="44" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E44" s="11"/>
+      <c r="F44" s="11"/>
+      <c r="G44" s="11"/>
+    </row>
+    <row r="45" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E45" s="11"/>
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+    </row>
+    <row r="46" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+    </row>
+    <row r="47" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+    </row>
+    <row r="48" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E48" s="11"/>
+      <c r="F48" s="11"/>
+      <c r="G48" s="11"/>
+    </row>
+    <row r="49" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E49" s="11"/>
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+    </row>
+    <row r="50" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E50" s="11"/>
+      <c r="F50" s="11"/>
+      <c r="G50" s="11"/>
+    </row>
+    <row r="51" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E51" s="11"/>
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+    </row>
+    <row r="52" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E52" s="11"/>
+      <c r="F52" s="11"/>
+      <c r="G52" s="11"/>
+    </row>
+    <row r="53" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E53" s="11"/>
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+    </row>
+    <row r="54" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E54" s="11"/>
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+    </row>
+    <row r="55" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E55" s="11"/>
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+    </row>
+    <row r="56" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E56" s="11"/>
+      <c r="F56" s="11"/>
+      <c r="G56" s="11"/>
+    </row>
+    <row r="57" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E57" s="11"/>
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+    </row>
+    <row r="58" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E58" s="11"/>
+      <c r="F58" s="11"/>
+      <c r="G58" s="11"/>
+    </row>
+    <row r="59" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E59" s="11"/>
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+    </row>
+    <row r="60" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E60" s="11"/>
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+    </row>
+    <row r="61" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E61" s="11"/>
+      <c r="F61" s="11"/>
+      <c r="G61" s="11"/>
+    </row>
+    <row r="62" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E62" s="11"/>
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+    </row>
+    <row r="63" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E63" s="11"/>
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+    </row>
+    <row r="64" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E64" s="11"/>
+      <c r="F64" s="11"/>
+      <c r="G64" s="11"/>
+    </row>
+    <row r="65" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E65" s="11"/>
+      <c r="F65" s="11"/>
+      <c r="G65" s="11"/>
+    </row>
+    <row r="66" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E66" s="11"/>
+      <c r="F66" s="11"/>
+      <c r="G66" s="11"/>
+    </row>
+    <row r="67" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E67" s="11"/>
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+    </row>
+    <row r="68" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E68" s="11"/>
+      <c r="F68" s="11"/>
+      <c r="G68" s="11"/>
+    </row>
+    <row r="69" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E69" s="11"/>
+      <c r="F69" s="11"/>
+      <c r="G69" s="11"/>
+    </row>
+    <row r="70" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E70" s="11"/>
+      <c r="F70" s="11"/>
+      <c r="G70" s="11"/>
+    </row>
+    <row r="71" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E71" s="11"/>
+      <c r="F71" s="11"/>
+      <c r="G71" s="11"/>
+    </row>
+    <row r="72" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E72" s="11"/>
+      <c r="F72" s="11"/>
+      <c r="G72" s="11"/>
+    </row>
+    <row r="73" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E73" s="11"/>
+      <c r="F73" s="11"/>
+      <c r="G73" s="11"/>
+    </row>
+    <row r="74" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E74" s="11"/>
+      <c r="F74" s="11"/>
+      <c r="G74" s="11"/>
+    </row>
+    <row r="75" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E75" s="11"/>
+      <c r="F75" s="11"/>
+      <c r="G75" s="11"/>
+    </row>
+    <row r="76" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E76" s="11"/>
+      <c r="F76" s="11"/>
+      <c r="G76" s="11"/>
+    </row>
+    <row r="77" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E77" s="11"/>
+      <c r="F77" s="11"/>
+      <c r="G77" s="11"/>
+    </row>
+    <row r="78" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E78" s="11"/>
+      <c r="F78" s="11"/>
+      <c r="G78" s="11"/>
+    </row>
+    <row r="79" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E79" s="11"/>
+      <c r="F79" s="11"/>
+      <c r="G79" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added more variables + started x column and time period
</commit_message>
<xml_diff>
--- a/models.xlsx
+++ b/models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssb\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B44BE0-0253-4828-AD19-D5E54D73E2E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D0495D-5562-4FE7-B438-C23A8FB14D08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{6422CA17-FA72-4B85-908A-20157EF2E374}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <r>
       <t>launch angle/</t>
@@ -227,6 +227,21 @@
   <si>
     <t>range/m(R)</t>
   </si>
+  <si>
+    <t>x apogee/m</t>
+  </si>
+  <si>
+    <t>t/s</t>
+  </si>
+  <si>
+    <t>x/m</t>
+  </si>
+  <si>
+    <t>y apogee/m</t>
+  </si>
+  <si>
+    <t>time of flight/s(T)</t>
+  </si>
 </sst>
 </file>
 
@@ -273,7 +288,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -301,6 +316,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -394,8 +415,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -14155,7 +14176,7 @@
   <dimension ref="B2:G79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14170,9 +14191,13 @@
       <c r="C2" s="1">
         <v>42</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
+      <c r="E2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
@@ -14182,9 +14207,14 @@
         <f>($C2*PI()/180)</f>
         <v>0.73303828583761843</v>
       </c>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="11">
+        <f>E3*$C$4*COS($C$3)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="12"/>
     </row>
     <row r="4" spans="2:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
@@ -14193,9 +14223,15 @@
       <c r="C4" s="1">
         <v>10</v>
       </c>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
+      <c r="E4" s="7">
+        <f>E3+$C$7</f>
+        <v>0.02</v>
+      </c>
+      <c r="F4" s="11">
+        <f t="shared" ref="F4:F67" si="0">E4*$C$4*COS($C$3)</f>
+        <v>0.14862896509547885</v>
+      </c>
+      <c r="G4" s="12"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
@@ -14204,9 +14240,15 @@
       <c r="C5" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
+      <c r="E5" s="7">
+        <f t="shared" ref="E5:E68" si="1">E4+$C$7</f>
+        <v>0.04</v>
+      </c>
+      <c r="F5" s="11">
+        <f t="shared" si="0"/>
+        <v>0.2972579301909577</v>
+      </c>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" spans="2:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
@@ -14215,9 +14257,15 @@
       <c r="C6" s="1">
         <v>9.81</v>
       </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
+      <c r="E6" s="7">
+        <f t="shared" si="1"/>
+        <v>0.06</v>
+      </c>
+      <c r="F6" s="11">
+        <f t="shared" si="0"/>
+        <v>0.44588689528643655</v>
+      </c>
+      <c r="G6" s="12"/>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
@@ -14226,14 +14274,26 @@
       <c r="C7" s="1">
         <v>0.02</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
+      <c r="E7" s="7">
+        <f t="shared" si="1"/>
+        <v>0.08</v>
+      </c>
+      <c r="F7" s="11">
+        <f t="shared" si="0"/>
+        <v>0.5945158603819154</v>
+      </c>
+      <c r="G7" s="12"/>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
+      <c r="E8" s="7">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="F8" s="11">
+        <f t="shared" si="0"/>
+        <v>0.74314482547739424</v>
+      </c>
+      <c r="G8" s="12"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
@@ -14243,365 +14303,404 @@
         <f>(($C$4*$C$4)/$C$6)*(SIN($C$3)*COS($C$3)+COS($C$3)*SQRT((SIN($C$3)*SIN($C$3)+((2*$C$6*$C$5)/($C$4*$C$4)))))</f>
         <v>11.147829102248627</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
+      <c r="E9" s="7">
+        <f t="shared" si="1"/>
+        <v>0.12000000000000001</v>
+      </c>
+      <c r="F9" s="11">
+        <f t="shared" si="0"/>
+        <v>0.8917737905728732</v>
+      </c>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3">
+        <f>(($C$4*$C$4)/($C$6))*SIN($C$3)*COS($C$3)</f>
+        <v>5.0689189366374778</v>
+      </c>
+      <c r="E10" s="7">
+        <f t="shared" si="1"/>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F10" s="11">
+        <f t="shared" si="0"/>
+        <v>1.0404027556683519</v>
+      </c>
+      <c r="G10" s="12"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="11"/>
-      <c r="C11" s="12"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="3">
+        <f>$C$5+(($C$4*$C$4)/(2*$C$6))*(SIN($C$3)*SIN($C$3))</f>
+        <v>3.282037555383146</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" si="1"/>
+        <v>0.16</v>
+      </c>
+      <c r="F11" s="11">
+        <f t="shared" si="0"/>
+        <v>1.1890317207638308</v>
+      </c>
+      <c r="G11" s="12"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
+      <c r="B12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="3">
+        <f>$C$9/($C$4*COS($C$3))</f>
+        <v>1.5000883704044219</v>
+      </c>
+      <c r="E12" s="7">
+        <f t="shared" si="1"/>
+        <v>0.18</v>
+      </c>
+      <c r="F12" s="11">
+        <f t="shared" si="0"/>
+        <v>1.3376606858593094</v>
+      </c>
+      <c r="G12" s="12"/>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
     </row>
     <row r="17" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
     </row>
     <row r="18" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
     </row>
     <row r="19" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
     </row>
     <row r="20" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
     </row>
     <row r="21" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
     </row>
     <row r="22" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
     </row>
     <row r="23" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
     </row>
     <row r="24" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
     </row>
     <row r="25" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
     </row>
     <row r="26" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
     </row>
     <row r="27" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
     </row>
     <row r="28" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
     </row>
     <row r="29" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
     </row>
     <row r="30" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
     </row>
     <row r="31" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="12"/>
+      <c r="G31" s="12"/>
     </row>
     <row r="32" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E32" s="11"/>
-      <c r="F32" s="11"/>
-      <c r="G32" s="11"/>
+      <c r="E32" s="12"/>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12"/>
     </row>
     <row r="33" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
     </row>
     <row r="34" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
     </row>
     <row r="35" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
     </row>
     <row r="36" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E36" s="11"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
     </row>
     <row r="37" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
     </row>
     <row r="38" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="12"/>
+      <c r="G38" s="12"/>
     </row>
     <row r="39" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E39" s="11"/>
-      <c r="F39" s="11"/>
-      <c r="G39" s="11"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12"/>
+      <c r="G39" s="12"/>
     </row>
     <row r="40" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E40" s="11"/>
-      <c r="F40" s="11"/>
-      <c r="G40" s="11"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="12"/>
+      <c r="G40" s="12"/>
     </row>
     <row r="41" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E41" s="11"/>
-      <c r="F41" s="11"/>
-      <c r="G41" s="11"/>
+      <c r="E41" s="12"/>
+      <c r="F41" s="12"/>
+      <c r="G41" s="12"/>
     </row>
     <row r="42" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E42" s="11"/>
-      <c r="F42" s="11"/>
-      <c r="G42" s="11"/>
+      <c r="E42" s="12"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
     </row>
     <row r="43" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E43" s="11"/>
-      <c r="F43" s="11"/>
-      <c r="G43" s="11"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
     </row>
     <row r="44" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E44" s="11"/>
-      <c r="F44" s="11"/>
-      <c r="G44" s="11"/>
+      <c r="E44" s="12"/>
+      <c r="F44" s="12"/>
+      <c r="G44" s="12"/>
     </row>
     <row r="45" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
     </row>
     <row r="46" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
     </row>
     <row r="47" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E47" s="11"/>
-      <c r="F47" s="11"/>
-      <c r="G47" s="11"/>
+      <c r="E47" s="12"/>
+      <c r="F47" s="12"/>
+      <c r="G47" s="12"/>
     </row>
     <row r="48" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E48" s="11"/>
-      <c r="F48" s="11"/>
-      <c r="G48" s="11"/>
+      <c r="E48" s="12"/>
+      <c r="F48" s="12"/>
+      <c r="G48" s="12"/>
     </row>
     <row r="49" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" s="11"/>
+      <c r="E49" s="12"/>
+      <c r="F49" s="12"/>
+      <c r="G49" s="12"/>
     </row>
     <row r="50" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E50" s="11"/>
-      <c r="F50" s="11"/>
-      <c r="G50" s="11"/>
+      <c r="E50" s="12"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12"/>
     </row>
     <row r="51" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E51" s="11"/>
-      <c r="F51" s="11"/>
-      <c r="G51" s="11"/>
+      <c r="E51" s="12"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="12"/>
     </row>
     <row r="52" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E52" s="11"/>
-      <c r="F52" s="11"/>
-      <c r="G52" s="11"/>
+      <c r="E52" s="12"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="12"/>
     </row>
     <row r="53" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E53" s="11"/>
-      <c r="F53" s="11"/>
-      <c r="G53" s="11"/>
+      <c r="E53" s="12"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="12"/>
     </row>
     <row r="54" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E54" s="11"/>
-      <c r="F54" s="11"/>
-      <c r="G54" s="11"/>
+      <c r="E54" s="12"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="12"/>
     </row>
     <row r="55" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
-      <c r="G55" s="11"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
     </row>
     <row r="56" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E56" s="11"/>
-      <c r="F56" s="11"/>
-      <c r="G56" s="11"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12"/>
     </row>
     <row r="57" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E57" s="11"/>
-      <c r="F57" s="11"/>
-      <c r="G57" s="11"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="12"/>
     </row>
     <row r="58" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E58" s="11"/>
-      <c r="F58" s="11"/>
-      <c r="G58" s="11"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
     </row>
     <row r="59" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E59" s="11"/>
-      <c r="F59" s="11"/>
-      <c r="G59" s="11"/>
+      <c r="E59" s="12"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="12"/>
     </row>
     <row r="60" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E60" s="11"/>
-      <c r="F60" s="11"/>
-      <c r="G60" s="11"/>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
     </row>
     <row r="61" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E61" s="11"/>
-      <c r="F61" s="11"/>
-      <c r="G61" s="11"/>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
     </row>
     <row r="62" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E62" s="11"/>
-      <c r="F62" s="11"/>
-      <c r="G62" s="11"/>
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
+      <c r="G62" s="12"/>
     </row>
     <row r="63" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E63" s="11"/>
-      <c r="F63" s="11"/>
-      <c r="G63" s="11"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="12"/>
     </row>
     <row r="64" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E64" s="11"/>
-      <c r="F64" s="11"/>
-      <c r="G64" s="11"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
     </row>
     <row r="65" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E65" s="11"/>
-      <c r="F65" s="11"/>
-      <c r="G65" s="11"/>
+      <c r="E65" s="12"/>
+      <c r="F65" s="12"/>
+      <c r="G65" s="12"/>
     </row>
     <row r="66" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E66" s="11"/>
-      <c r="F66" s="11"/>
-      <c r="G66" s="11"/>
+      <c r="E66" s="12"/>
+      <c r="F66" s="12"/>
+      <c r="G66" s="12"/>
     </row>
     <row r="67" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E67" s="11"/>
-      <c r="F67" s="11"/>
-      <c r="G67" s="11"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="12"/>
+      <c r="G67" s="12"/>
     </row>
     <row r="68" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E68" s="11"/>
-      <c r="F68" s="11"/>
-      <c r="G68" s="11"/>
+      <c r="E68" s="12"/>
+      <c r="F68" s="12"/>
+      <c r="G68" s="12"/>
     </row>
     <row r="69" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E69" s="11"/>
-      <c r="F69" s="11"/>
-      <c r="G69" s="11"/>
+      <c r="E69" s="12"/>
+      <c r="F69" s="12"/>
+      <c r="G69" s="12"/>
     </row>
     <row r="70" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E70" s="11"/>
-      <c r="F70" s="11"/>
-      <c r="G70" s="11"/>
+      <c r="E70" s="12"/>
+      <c r="F70" s="12"/>
+      <c r="G70" s="12"/>
     </row>
     <row r="71" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E71" s="11"/>
-      <c r="F71" s="11"/>
-      <c r="G71" s="11"/>
+      <c r="E71" s="12"/>
+      <c r="F71" s="12"/>
+      <c r="G71" s="12"/>
     </row>
     <row r="72" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E72" s="11"/>
-      <c r="F72" s="11"/>
-      <c r="G72" s="11"/>
+      <c r="E72" s="12"/>
+      <c r="F72" s="12"/>
+      <c r="G72" s="12"/>
     </row>
     <row r="73" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E73" s="11"/>
-      <c r="F73" s="11"/>
-      <c r="G73" s="11"/>
+      <c r="E73" s="12"/>
+      <c r="F73" s="12"/>
+      <c r="G73" s="12"/>
     </row>
     <row r="74" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E74" s="11"/>
-      <c r="F74" s="11"/>
-      <c r="G74" s="11"/>
+      <c r="E74" s="12"/>
+      <c r="F74" s="12"/>
+      <c r="G74" s="12"/>
     </row>
     <row r="75" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E75" s="11"/>
-      <c r="F75" s="11"/>
-      <c r="G75" s="11"/>
+      <c r="E75" s="12"/>
+      <c r="F75" s="12"/>
+      <c r="G75" s="12"/>
     </row>
     <row r="76" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E76" s="11"/>
-      <c r="F76" s="11"/>
-      <c r="G76" s="11"/>
+      <c r="E76" s="12"/>
+      <c r="F76" s="12"/>
+      <c r="G76" s="12"/>
     </row>
     <row r="77" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E77" s="11"/>
-      <c r="F77" s="11"/>
-      <c r="G77" s="11"/>
+      <c r="E77" s="12"/>
+      <c r="F77" s="12"/>
+      <c r="G77" s="12"/>
     </row>
     <row r="78" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E78" s="11"/>
-      <c r="F78" s="11"/>
-      <c r="G78" s="11"/>
+      <c r="E78" s="12"/>
+      <c r="F78" s="12"/>
+      <c r="G78" s="12"/>
     </row>
     <row r="79" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E79" s="11"/>
-      <c r="F79" s="11"/>
-      <c r="G79" s="11"/>
+      <c r="E79" s="12"/>
+      <c r="F79" s="12"/>
+      <c r="G79" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finished more accurate model of projectile
</commit_message>
<xml_diff>
--- a/models.xlsx
+++ b/models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssb\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D0495D-5562-4FE7-B438-C23A8FB14D08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A685E8-BEBD-4513-BBD0-5EE86063088F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{6422CA17-FA72-4B85-908A-20157EF2E374}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <r>
       <t>launch angle/</t>
@@ -242,6 +242,9 @@
   <si>
     <t>time of flight/s(T)</t>
   </si>
+  <si>
+    <t>y/m</t>
+  </si>
 </sst>
 </file>
 
@@ -403,7 +406,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -416,7 +419,6 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1783,13 +1785,1588 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Projectile Trajectory</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.12848381452318461"/>
+          <c:y val="0.2229445236668251"/>
+          <c:w val="0.82829396325459315"/>
+          <c:h val="0.65411887490441645"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>y vs x</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>[1]Sheet2!$F$3:$F$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="76"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.14862896509547885</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2972579301909577</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.44588689528643655</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.5945158603819154</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.74314482547739424</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8917737905728732</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0404027556683519</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1890317207638308</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.3376606858593094</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.4862896509547883</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.6349186160502671</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.7835475811457457</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.9321765462412248</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.0808055113367039</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.229434476432183</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.3780634415276616</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.5266924066231407</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.6753213717186197</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.8239503368140988</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.9725793019095774</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.1212082670050565</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.2698372321005356</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.4184661971960146</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.5670951622914937</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.7157241273869719</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.864353092482451</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>4.01298205757793</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.1616110226734087</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.3102399877688882</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.4588689528643668</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.6074979179598454</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.7561268830553249</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.9047558481508036</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>5.0533848132462831</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>5.2020137783417617</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.3506427434372403</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.4992717085327198</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>5.6479006736281985</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>5.796529638723678</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5.9451586038191566</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>6.0937875689146361</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>6.2424165340101148</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>6.3910454991055943</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>6.5396744642010729</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>6.6883034292965524</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>6.8369323943920302</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>6.9855613594875106</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>7.1341903245829883</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>7.2828192896784678</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>7.4314482547739447</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>7.5800772198694251</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>7.7287061849649046</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>7.8773351500603823</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>8.0259641151558618</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>8.1745930802513413</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>8.3232220453468209</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>8.4718510104422986</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>8.6204799755377763</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>8.7691089406332559</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>8.9177379057287354</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>9.0663668708242149</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>9.2149958359196926</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>9.3636248010151721</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>9.5122537661106517</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>9.6608827312061312</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>9.8095116963016089</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>9.9581406613970884</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>10.106769626492568</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>10.255398591588046</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>10.404027556683525</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>10.552656521779005</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>10.701285486874484</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>10.849914451969962</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>10.998543417065441</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>11.147172382160921</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>[1]Sheet2!$G$3:$G$78</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="76"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1318641212717717</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2598042425435432</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.383820363815315</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.5039124850870864</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6200806063588582</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7323247276306299</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.8406448489024014</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.9450409701741731</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.0455130914459443</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.1420612127177163</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.2346853339894879</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.3233854552612594</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.4081615765330313</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.4890136978048032</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.5659418190765746</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.6389459403483464</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.7080260616201182</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.7731821828918899</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.8344143041636611</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.8917224254354332</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.9451065467072048</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.9945666679789764</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.0401027892507479</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.0817149105225203</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.1194030317942918</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.1531671530660628</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.183007274337835</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.2089233956096059</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.2309155168813781</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>3.2489836381531494</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.2631277594249211</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.2733478806966927</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.2796440019684647</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3.2820161232402363</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3.2804642445120078</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3.2749883657837788</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3.2655884870555507</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.2522646083273221</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>3.2350167295990939</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.2138448508708652</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>3.1887489721426379</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.1597290934144091</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>3.1267852146861799</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.0899173359579519</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3.0491254572297226</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3.0044095785014946</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.9557696997732652</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.903205821045038</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.8467179423168094</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.7863060635885812</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.7219701848603526</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2.6537103061321234</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>2.5815264274038947</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2.5054185486756673</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.4253866699474367</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2.3414307912192092</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>2.2535509124909812</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>2.1617470337627536</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>2.0660191550345246</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.966367276306296</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.862791397578067</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.7552915188498384</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.6438676401216101</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.5285197613933796</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.4092478826651522</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.2860520039369234</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.1589321252086968</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.0278882464804671</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.89292036775223949</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.75402848902401054</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.611212610295782</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.46447273156755209</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.31380885283932436</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.15922097411109526</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>7.0909538286656471E-4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2D5C-4F08-BE76-B10ACE4AA5DB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>apogee</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="sq">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent3">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="star"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>[1]Sheet2!$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5.0689189366374778</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>[1]Sheet2!$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.0000</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3.282037555383146</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2D5C-4F08-BE76-B10ACE4AA5DB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="292843663"/>
+        <c:axId val="292845583"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="292843663"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>x/m</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:noFill/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="292845583"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="292845583"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>y/m</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="292843663"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="25">
   <a:schemeClr val="accent5"/>
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="11">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent5"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2370,6 +3947,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E44DD0EA-CD18-4744-9F7B-B9815C4ED0EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -14173,10 +15793,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CCE5E17-412F-4B65-BE92-5E427918CCA8}">
-  <dimension ref="B2:G79"/>
+  <dimension ref="B2:G78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14197,7 +15817,9 @@
       <c r="F2" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="12"/>
+      <c r="G2" s="11" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
@@ -14214,7 +15836,10 @@
         <f>E3*$C$4*COS($C$3)</f>
         <v>0</v>
       </c>
-      <c r="G3" s="12"/>
+      <c r="G3" s="11">
+        <f>$C$5+F3*TAN($C$3)-($C$6/(2*$C$4*$C$4))*(1+TAN($C$3)*TAN($C$3))*F3*F3</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="2:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
@@ -14231,7 +15856,10 @@
         <f t="shared" ref="F4:F67" si="0">E4*$C$4*COS($C$3)</f>
         <v>0.14862896509547885</v>
       </c>
-      <c r="G4" s="12"/>
+      <c r="G4" s="11">
+        <f t="shared" ref="G4:G67" si="1">$C$5+F4*TAN($C$3)-($C$6/(2*$C$4*$C$4))*(1+TAN($C$3)*TAN($C$3))*F4*F4</f>
+        <v>1.1318641212717717</v>
+      </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
@@ -14241,14 +15869,17 @@
         <v>1</v>
       </c>
       <c r="E5" s="7">
-        <f t="shared" ref="E5:E68" si="1">E4+$C$7</f>
+        <f t="shared" ref="E5:E68" si="2">E4+$C$7</f>
         <v>0.04</v>
       </c>
       <c r="F5" s="11">
         <f t="shared" si="0"/>
         <v>0.2972579301909577</v>
       </c>
-      <c r="G5" s="12"/>
+      <c r="G5" s="11">
+        <f t="shared" si="1"/>
+        <v>1.2598042425435432</v>
+      </c>
     </row>
     <row r="6" spans="2:7" ht="16.2" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
@@ -14258,14 +15889,17 @@
         <v>9.81</v>
       </c>
       <c r="E6" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.06</v>
       </c>
       <c r="F6" s="11">
         <f t="shared" si="0"/>
         <v>0.44588689528643655</v>
       </c>
-      <c r="G6" s="12"/>
+      <c r="G6" s="11">
+        <f t="shared" si="1"/>
+        <v>1.383820363815315</v>
+      </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
@@ -14275,25 +15909,31 @@
         <v>0.02</v>
       </c>
       <c r="E7" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.08</v>
       </c>
       <c r="F7" s="11">
         <f t="shared" si="0"/>
         <v>0.5945158603819154</v>
       </c>
-      <c r="G7" s="12"/>
+      <c r="G7" s="11">
+        <f t="shared" si="1"/>
+        <v>1.5039124850870864</v>
+      </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="E8" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.1</v>
       </c>
       <c r="F8" s="11">
         <f t="shared" si="0"/>
         <v>0.74314482547739424</v>
       </c>
-      <c r="G8" s="12"/>
+      <c r="G8" s="11">
+        <f t="shared" si="1"/>
+        <v>1.6200806063588582</v>
+      </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
@@ -14304,14 +15944,17 @@
         <v>11.147829102248627</v>
       </c>
       <c r="E9" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.12000000000000001</v>
       </c>
       <c r="F9" s="11">
         <f t="shared" si="0"/>
         <v>0.8917737905728732</v>
       </c>
-      <c r="G9" s="12"/>
+      <c r="G9" s="11">
+        <f t="shared" si="1"/>
+        <v>1.7323247276306299</v>
+      </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
@@ -14322,14 +15965,17 @@
         <v>5.0689189366374778</v>
       </c>
       <c r="E10" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.14000000000000001</v>
       </c>
       <c r="F10" s="11">
         <f t="shared" si="0"/>
         <v>1.0404027556683519</v>
       </c>
-      <c r="G10" s="12"/>
+      <c r="G10" s="11">
+        <f t="shared" si="1"/>
+        <v>1.8406448489024014</v>
+      </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
@@ -14340,14 +15986,17 @@
         <v>3.282037555383146</v>
       </c>
       <c r="E11" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.16</v>
       </c>
       <c r="F11" s="11">
         <f t="shared" si="0"/>
         <v>1.1890317207638308</v>
       </c>
-      <c r="G11" s="12"/>
+      <c r="G11" s="11">
+        <f t="shared" si="1"/>
+        <v>1.9450409701741731</v>
+      </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
@@ -14358,351 +16007,944 @@
         <v>1.5000883704044219</v>
       </c>
       <c r="E12" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.18</v>
       </c>
       <c r="F12" s="11">
         <f t="shared" si="0"/>
         <v>1.3376606858593094</v>
       </c>
-      <c r="G12" s="12"/>
+      <c r="G12" s="11">
+        <f t="shared" si="1"/>
+        <v>2.0455130914459443</v>
+      </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
+      <c r="E13" s="7">
+        <f t="shared" si="2"/>
+        <v>0.19999999999999998</v>
+      </c>
+      <c r="F13" s="11">
+        <f t="shared" si="0"/>
+        <v>1.4862896509547883</v>
+      </c>
+      <c r="G13" s="11">
+        <f t="shared" si="1"/>
+        <v>2.1420612127177163</v>
+      </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
+      <c r="E14" s="7">
+        <f t="shared" si="2"/>
+        <v>0.21999999999999997</v>
+      </c>
+      <c r="F14" s="11">
+        <f t="shared" si="0"/>
+        <v>1.6349186160502671</v>
+      </c>
+      <c r="G14" s="11">
+        <f t="shared" si="1"/>
+        <v>2.2346853339894879</v>
+      </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
+      <c r="E15" s="7">
+        <f t="shared" si="2"/>
+        <v>0.23999999999999996</v>
+      </c>
+      <c r="F15" s="11">
+        <f t="shared" si="0"/>
+        <v>1.7835475811457457</v>
+      </c>
+      <c r="G15" s="11">
+        <f t="shared" si="1"/>
+        <v>2.3233854552612594</v>
+      </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
+      <c r="E16" s="7">
+        <f t="shared" si="2"/>
+        <v>0.25999999999999995</v>
+      </c>
+      <c r="F16" s="11">
+        <f t="shared" si="0"/>
+        <v>1.9321765462412248</v>
+      </c>
+      <c r="G16" s="11">
+        <f t="shared" si="1"/>
+        <v>2.4081615765330313</v>
+      </c>
     </row>
     <row r="17" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
+      <c r="E17" s="7">
+        <f t="shared" si="2"/>
+        <v>0.27999999999999997</v>
+      </c>
+      <c r="F17" s="11">
+        <f t="shared" si="0"/>
+        <v>2.0808055113367039</v>
+      </c>
+      <c r="G17" s="11">
+        <f t="shared" si="1"/>
+        <v>2.4890136978048032</v>
+      </c>
     </row>
     <row r="18" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
+      <c r="E18" s="7">
+        <f t="shared" si="2"/>
+        <v>0.3</v>
+      </c>
+      <c r="F18" s="11">
+        <f t="shared" si="0"/>
+        <v>2.229434476432183</v>
+      </c>
+      <c r="G18" s="11">
+        <f t="shared" si="1"/>
+        <v>2.5659418190765746</v>
+      </c>
     </row>
     <row r="19" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
-      <c r="G19" s="12"/>
+      <c r="E19" s="7">
+        <f t="shared" si="2"/>
+        <v>0.32</v>
+      </c>
+      <c r="F19" s="11">
+        <f t="shared" si="0"/>
+        <v>2.3780634415276616</v>
+      </c>
+      <c r="G19" s="11">
+        <f t="shared" si="1"/>
+        <v>2.6389459403483464</v>
+      </c>
     </row>
     <row r="20" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
+      <c r="E20" s="7">
+        <f t="shared" si="2"/>
+        <v>0.34</v>
+      </c>
+      <c r="F20" s="11">
+        <f t="shared" si="0"/>
+        <v>2.5266924066231407</v>
+      </c>
+      <c r="G20" s="11">
+        <f t="shared" si="1"/>
+        <v>2.7080260616201182</v>
+      </c>
     </row>
     <row r="21" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E21" s="12"/>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12"/>
+      <c r="E21" s="7">
+        <f t="shared" si="2"/>
+        <v>0.36000000000000004</v>
+      </c>
+      <c r="F21" s="11">
+        <f t="shared" si="0"/>
+        <v>2.6753213717186197</v>
+      </c>
+      <c r="G21" s="11">
+        <f t="shared" si="1"/>
+        <v>2.7731821828918899</v>
+      </c>
     </row>
     <row r="22" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12"/>
+      <c r="E22" s="7">
+        <f t="shared" si="2"/>
+        <v>0.38000000000000006</v>
+      </c>
+      <c r="F22" s="11">
+        <f t="shared" si="0"/>
+        <v>2.8239503368140988</v>
+      </c>
+      <c r="G22" s="11">
+        <f t="shared" si="1"/>
+        <v>2.8344143041636611</v>
+      </c>
     </row>
     <row r="23" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
+      <c r="E23" s="7">
+        <f t="shared" si="2"/>
+        <v>0.40000000000000008</v>
+      </c>
+      <c r="F23" s="11">
+        <f t="shared" si="0"/>
+        <v>2.9725793019095774</v>
+      </c>
+      <c r="G23" s="11">
+        <f t="shared" si="1"/>
+        <v>2.8917224254354332</v>
+      </c>
     </row>
     <row r="24" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
+      <c r="E24" s="7">
+        <f t="shared" si="2"/>
+        <v>0.4200000000000001</v>
+      </c>
+      <c r="F24" s="11">
+        <f t="shared" si="0"/>
+        <v>3.1212082670050565</v>
+      </c>
+      <c r="G24" s="11">
+        <f t="shared" si="1"/>
+        <v>2.9451065467072048</v>
+      </c>
     </row>
     <row r="25" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
+      <c r="E25" s="7">
+        <f t="shared" si="2"/>
+        <v>0.44000000000000011</v>
+      </c>
+      <c r="F25" s="11">
+        <f t="shared" si="0"/>
+        <v>3.2698372321005356</v>
+      </c>
+      <c r="G25" s="11">
+        <f t="shared" si="1"/>
+        <v>2.9945666679789764</v>
+      </c>
     </row>
     <row r="26" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
+      <c r="E26" s="7">
+        <f t="shared" si="2"/>
+        <v>0.46000000000000013</v>
+      </c>
+      <c r="F26" s="11">
+        <f t="shared" si="0"/>
+        <v>3.4184661971960146</v>
+      </c>
+      <c r="G26" s="11">
+        <f t="shared" si="1"/>
+        <v>3.0401027892507479</v>
+      </c>
     </row>
     <row r="27" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
+      <c r="E27" s="7">
+        <f t="shared" si="2"/>
+        <v>0.48000000000000015</v>
+      </c>
+      <c r="F27" s="11">
+        <f t="shared" si="0"/>
+        <v>3.5670951622914937</v>
+      </c>
+      <c r="G27" s="11">
+        <f t="shared" si="1"/>
+        <v>3.0817149105225203</v>
+      </c>
     </row>
     <row r="28" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
+      <c r="E28" s="7">
+        <f t="shared" si="2"/>
+        <v>0.50000000000000011</v>
+      </c>
+      <c r="F28" s="11">
+        <f t="shared" si="0"/>
+        <v>3.7157241273869719</v>
+      </c>
+      <c r="G28" s="11">
+        <f t="shared" si="1"/>
+        <v>3.1194030317942918</v>
+      </c>
     </row>
     <row r="29" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
+      <c r="E29" s="7">
+        <f t="shared" si="2"/>
+        <v>0.52000000000000013</v>
+      </c>
+      <c r="F29" s="11">
+        <f t="shared" si="0"/>
+        <v>3.864353092482451</v>
+      </c>
+      <c r="G29" s="11">
+        <f t="shared" si="1"/>
+        <v>3.1531671530660628</v>
+      </c>
     </row>
     <row r="30" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E30" s="12"/>
-      <c r="F30" s="12"/>
-      <c r="G30" s="12"/>
+      <c r="E30" s="7">
+        <f t="shared" si="2"/>
+        <v>0.54000000000000015</v>
+      </c>
+      <c r="F30" s="11">
+        <f t="shared" si="0"/>
+        <v>4.01298205757793</v>
+      </c>
+      <c r="G30" s="11">
+        <f t="shared" si="1"/>
+        <v>3.183007274337835</v>
+      </c>
     </row>
     <row r="31" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
+      <c r="E31" s="7">
+        <f t="shared" si="2"/>
+        <v>0.56000000000000016</v>
+      </c>
+      <c r="F31" s="11">
+        <f t="shared" si="0"/>
+        <v>4.1616110226734087</v>
+      </c>
+      <c r="G31" s="11">
+        <f t="shared" si="1"/>
+        <v>3.2089233956096059</v>
+      </c>
     </row>
     <row r="32" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
+      <c r="E32" s="7">
+        <f t="shared" si="2"/>
+        <v>0.58000000000000018</v>
+      </c>
+      <c r="F32" s="11">
+        <f t="shared" si="0"/>
+        <v>4.3102399877688882</v>
+      </c>
+      <c r="G32" s="11">
+        <f t="shared" si="1"/>
+        <v>3.2309155168813781</v>
+      </c>
     </row>
     <row r="33" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
+      <c r="E33" s="7">
+        <f t="shared" si="2"/>
+        <v>0.6000000000000002</v>
+      </c>
+      <c r="F33" s="11">
+        <f t="shared" si="0"/>
+        <v>4.4588689528643668</v>
+      </c>
+      <c r="G33" s="11">
+        <f t="shared" si="1"/>
+        <v>3.2489836381531494</v>
+      </c>
     </row>
     <row r="34" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
+      <c r="E34" s="7">
+        <f t="shared" si="2"/>
+        <v>0.62000000000000022</v>
+      </c>
+      <c r="F34" s="11">
+        <f t="shared" si="0"/>
+        <v>4.6074979179598454</v>
+      </c>
+      <c r="G34" s="11">
+        <f t="shared" si="1"/>
+        <v>3.2631277594249211</v>
+      </c>
     </row>
     <row r="35" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
+      <c r="E35" s="7">
+        <f t="shared" si="2"/>
+        <v>0.64000000000000024</v>
+      </c>
+      <c r="F35" s="11">
+        <f t="shared" si="0"/>
+        <v>4.7561268830553249</v>
+      </c>
+      <c r="G35" s="11">
+        <f t="shared" si="1"/>
+        <v>3.2733478806966927</v>
+      </c>
     </row>
     <row r="36" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
+      <c r="E36" s="7">
+        <f t="shared" si="2"/>
+        <v>0.66000000000000025</v>
+      </c>
+      <c r="F36" s="11">
+        <f t="shared" si="0"/>
+        <v>4.9047558481508036</v>
+      </c>
+      <c r="G36" s="11">
+        <f t="shared" si="1"/>
+        <v>3.2796440019684647</v>
+      </c>
     </row>
     <row r="37" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
+      <c r="E37" s="7">
+        <f t="shared" si="2"/>
+        <v>0.68000000000000027</v>
+      </c>
+      <c r="F37" s="11">
+        <f t="shared" si="0"/>
+        <v>5.0533848132462831</v>
+      </c>
+      <c r="G37" s="11">
+        <f t="shared" si="1"/>
+        <v>3.2820161232402363</v>
+      </c>
     </row>
     <row r="38" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
+      <c r="E38" s="7">
+        <f t="shared" si="2"/>
+        <v>0.70000000000000029</v>
+      </c>
+      <c r="F38" s="11">
+        <f t="shared" si="0"/>
+        <v>5.2020137783417617</v>
+      </c>
+      <c r="G38" s="11">
+        <f t="shared" si="1"/>
+        <v>3.2804642445120078</v>
+      </c>
     </row>
     <row r="39" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
+      <c r="E39" s="7">
+        <f t="shared" si="2"/>
+        <v>0.72000000000000031</v>
+      </c>
+      <c r="F39" s="11">
+        <f t="shared" si="0"/>
+        <v>5.3506427434372403</v>
+      </c>
+      <c r="G39" s="11">
+        <f t="shared" si="1"/>
+        <v>3.2749883657837788</v>
+      </c>
     </row>
     <row r="40" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
+      <c r="E40" s="7">
+        <f t="shared" si="2"/>
+        <v>0.74000000000000032</v>
+      </c>
+      <c r="F40" s="11">
+        <f t="shared" si="0"/>
+        <v>5.4992717085327198</v>
+      </c>
+      <c r="G40" s="11">
+        <f t="shared" si="1"/>
+        <v>3.2655884870555507</v>
+      </c>
     </row>
     <row r="41" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
+      <c r="E41" s="7">
+        <f t="shared" si="2"/>
+        <v>0.76000000000000034</v>
+      </c>
+      <c r="F41" s="11">
+        <f t="shared" si="0"/>
+        <v>5.6479006736281985</v>
+      </c>
+      <c r="G41" s="11">
+        <f t="shared" si="1"/>
+        <v>3.2522646083273221</v>
+      </c>
     </row>
     <row r="42" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
+      <c r="E42" s="7">
+        <f t="shared" si="2"/>
+        <v>0.78000000000000036</v>
+      </c>
+      <c r="F42" s="11">
+        <f t="shared" si="0"/>
+        <v>5.796529638723678</v>
+      </c>
+      <c r="G42" s="11">
+        <f t="shared" si="1"/>
+        <v>3.2350167295990939</v>
+      </c>
     </row>
     <row r="43" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
+      <c r="E43" s="7">
+        <f t="shared" si="2"/>
+        <v>0.80000000000000038</v>
+      </c>
+      <c r="F43" s="11">
+        <f t="shared" si="0"/>
+        <v>5.9451586038191566</v>
+      </c>
+      <c r="G43" s="11">
+        <f t="shared" si="1"/>
+        <v>3.2138448508708652</v>
+      </c>
     </row>
     <row r="44" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
+      <c r="E44" s="7">
+        <f t="shared" si="2"/>
+        <v>0.8200000000000004</v>
+      </c>
+      <c r="F44" s="11">
+        <f t="shared" si="0"/>
+        <v>6.0937875689146361</v>
+      </c>
+      <c r="G44" s="11">
+        <f t="shared" si="1"/>
+        <v>3.1887489721426379</v>
+      </c>
     </row>
     <row r="45" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
+      <c r="E45" s="7">
+        <f t="shared" si="2"/>
+        <v>0.84000000000000041</v>
+      </c>
+      <c r="F45" s="11">
+        <f t="shared" si="0"/>
+        <v>6.2424165340101148</v>
+      </c>
+      <c r="G45" s="11">
+        <f t="shared" si="1"/>
+        <v>3.1597290934144091</v>
+      </c>
     </row>
     <row r="46" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
+      <c r="E46" s="7">
+        <f t="shared" si="2"/>
+        <v>0.86000000000000043</v>
+      </c>
+      <c r="F46" s="11">
+        <f t="shared" si="0"/>
+        <v>6.3910454991055943</v>
+      </c>
+      <c r="G46" s="11">
+        <f t="shared" si="1"/>
+        <v>3.1267852146861799</v>
+      </c>
     </row>
     <row r="47" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
+      <c r="E47" s="7">
+        <f t="shared" si="2"/>
+        <v>0.88000000000000045</v>
+      </c>
+      <c r="F47" s="11">
+        <f t="shared" si="0"/>
+        <v>6.5396744642010729</v>
+      </c>
+      <c r="G47" s="11">
+        <f t="shared" si="1"/>
+        <v>3.0899173359579519</v>
+      </c>
     </row>
     <row r="48" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E48" s="12"/>
-      <c r="F48" s="12"/>
-      <c r="G48" s="12"/>
+      <c r="E48" s="7">
+        <f t="shared" si="2"/>
+        <v>0.90000000000000047</v>
+      </c>
+      <c r="F48" s="11">
+        <f t="shared" si="0"/>
+        <v>6.6883034292965524</v>
+      </c>
+      <c r="G48" s="11">
+        <f t="shared" si="1"/>
+        <v>3.0491254572297226</v>
+      </c>
     </row>
     <row r="49" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E49" s="12"/>
-      <c r="F49" s="12"/>
-      <c r="G49" s="12"/>
+      <c r="E49" s="7">
+        <f t="shared" si="2"/>
+        <v>0.92000000000000048</v>
+      </c>
+      <c r="F49" s="11">
+        <f t="shared" si="0"/>
+        <v>6.8369323943920302</v>
+      </c>
+      <c r="G49" s="11">
+        <f t="shared" si="1"/>
+        <v>3.0044095785014946</v>
+      </c>
     </row>
     <row r="50" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E50" s="12"/>
-      <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
+      <c r="E50" s="7">
+        <f t="shared" si="2"/>
+        <v>0.9400000000000005</v>
+      </c>
+      <c r="F50" s="11">
+        <f t="shared" si="0"/>
+        <v>6.9855613594875106</v>
+      </c>
+      <c r="G50" s="11">
+        <f t="shared" si="1"/>
+        <v>2.9557696997732652</v>
+      </c>
     </row>
     <row r="51" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E51" s="12"/>
-      <c r="F51" s="12"/>
-      <c r="G51" s="12"/>
+      <c r="E51" s="7">
+        <f t="shared" si="2"/>
+        <v>0.96000000000000052</v>
+      </c>
+      <c r="F51" s="11">
+        <f t="shared" si="0"/>
+        <v>7.1341903245829883</v>
+      </c>
+      <c r="G51" s="11">
+        <f t="shared" si="1"/>
+        <v>2.903205821045038</v>
+      </c>
     </row>
     <row r="52" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E52" s="12"/>
-      <c r="F52" s="12"/>
-      <c r="G52" s="12"/>
+      <c r="E52" s="7">
+        <f t="shared" si="2"/>
+        <v>0.98000000000000054</v>
+      </c>
+      <c r="F52" s="11">
+        <f t="shared" si="0"/>
+        <v>7.2828192896784678</v>
+      </c>
+      <c r="G52" s="11">
+        <f t="shared" si="1"/>
+        <v>2.8467179423168094</v>
+      </c>
     </row>
     <row r="53" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E53" s="12"/>
-      <c r="F53" s="12"/>
-      <c r="G53" s="12"/>
+      <c r="E53" s="7">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000004</v>
+      </c>
+      <c r="F53" s="11">
+        <f t="shared" si="0"/>
+        <v>7.4314482547739447</v>
+      </c>
+      <c r="G53" s="11">
+        <f t="shared" si="1"/>
+        <v>2.7863060635885812</v>
+      </c>
     </row>
     <row r="54" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E54" s="12"/>
-      <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
+      <c r="E54" s="7">
+        <f t="shared" si="2"/>
+        <v>1.0200000000000005</v>
+      </c>
+      <c r="F54" s="11">
+        <f t="shared" si="0"/>
+        <v>7.5800772198694251</v>
+      </c>
+      <c r="G54" s="11">
+        <f t="shared" si="1"/>
+        <v>2.7219701848603526</v>
+      </c>
     </row>
     <row r="55" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E55" s="12"/>
-      <c r="F55" s="12"/>
-      <c r="G55" s="12"/>
+      <c r="E55" s="7">
+        <f t="shared" si="2"/>
+        <v>1.0400000000000005</v>
+      </c>
+      <c r="F55" s="11">
+        <f t="shared" si="0"/>
+        <v>7.7287061849649046</v>
+      </c>
+      <c r="G55" s="11">
+        <f t="shared" si="1"/>
+        <v>2.6537103061321234</v>
+      </c>
     </row>
     <row r="56" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E56" s="12"/>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12"/>
+      <c r="E56" s="7">
+        <f t="shared" si="2"/>
+        <v>1.0600000000000005</v>
+      </c>
+      <c r="F56" s="11">
+        <f t="shared" si="0"/>
+        <v>7.8773351500603823</v>
+      </c>
+      <c r="G56" s="11">
+        <f t="shared" si="1"/>
+        <v>2.5815264274038947</v>
+      </c>
     </row>
     <row r="57" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E57" s="12"/>
-      <c r="F57" s="12"/>
-      <c r="G57" s="12"/>
+      <c r="E57" s="7">
+        <f t="shared" si="2"/>
+        <v>1.0800000000000005</v>
+      </c>
+      <c r="F57" s="11">
+        <f t="shared" si="0"/>
+        <v>8.0259641151558618</v>
+      </c>
+      <c r="G57" s="11">
+        <f t="shared" si="1"/>
+        <v>2.5054185486756673</v>
+      </c>
     </row>
     <row r="58" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E58" s="12"/>
-      <c r="F58" s="12"/>
-      <c r="G58" s="12"/>
+      <c r="E58" s="7">
+        <f t="shared" si="2"/>
+        <v>1.1000000000000005</v>
+      </c>
+      <c r="F58" s="11">
+        <f t="shared" si="0"/>
+        <v>8.1745930802513413</v>
+      </c>
+      <c r="G58" s="11">
+        <f t="shared" si="1"/>
+        <v>2.4253866699474367</v>
+      </c>
     </row>
     <row r="59" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E59" s="12"/>
-      <c r="F59" s="12"/>
-      <c r="G59" s="12"/>
+      <c r="E59" s="7">
+        <f t="shared" si="2"/>
+        <v>1.1200000000000006</v>
+      </c>
+      <c r="F59" s="11">
+        <f t="shared" si="0"/>
+        <v>8.3232220453468209</v>
+      </c>
+      <c r="G59" s="11">
+        <f t="shared" si="1"/>
+        <v>2.3414307912192092</v>
+      </c>
     </row>
     <row r="60" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E60" s="12"/>
-      <c r="F60" s="12"/>
-      <c r="G60" s="12"/>
+      <c r="E60" s="7">
+        <f t="shared" si="2"/>
+        <v>1.1400000000000006</v>
+      </c>
+      <c r="F60" s="11">
+        <f t="shared" si="0"/>
+        <v>8.4718510104422986</v>
+      </c>
+      <c r="G60" s="11">
+        <f t="shared" si="1"/>
+        <v>2.2535509124909812</v>
+      </c>
     </row>
     <row r="61" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E61" s="12"/>
-      <c r="F61" s="12"/>
-      <c r="G61" s="12"/>
+      <c r="E61" s="7">
+        <f t="shared" si="2"/>
+        <v>1.1600000000000006</v>
+      </c>
+      <c r="F61" s="11">
+        <f t="shared" si="0"/>
+        <v>8.6204799755377763</v>
+      </c>
+      <c r="G61" s="11">
+        <f t="shared" si="1"/>
+        <v>2.1617470337627536</v>
+      </c>
     </row>
     <row r="62" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E62" s="12"/>
-      <c r="F62" s="12"/>
-      <c r="G62" s="12"/>
+      <c r="E62" s="7">
+        <f t="shared" si="2"/>
+        <v>1.1800000000000006</v>
+      </c>
+      <c r="F62" s="11">
+        <f t="shared" si="0"/>
+        <v>8.7691089406332559</v>
+      </c>
+      <c r="G62" s="11">
+        <f t="shared" si="1"/>
+        <v>2.0660191550345246</v>
+      </c>
     </row>
     <row r="63" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E63" s="12"/>
-      <c r="F63" s="12"/>
-      <c r="G63" s="12"/>
+      <c r="E63" s="7">
+        <f t="shared" si="2"/>
+        <v>1.2000000000000006</v>
+      </c>
+      <c r="F63" s="11">
+        <f t="shared" si="0"/>
+        <v>8.9177379057287354</v>
+      </c>
+      <c r="G63" s="11">
+        <f t="shared" si="1"/>
+        <v>1.966367276306296</v>
+      </c>
     </row>
     <row r="64" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E64" s="12"/>
-      <c r="F64" s="12"/>
-      <c r="G64" s="12"/>
+      <c r="E64" s="7">
+        <f t="shared" si="2"/>
+        <v>1.2200000000000006</v>
+      </c>
+      <c r="F64" s="11">
+        <f t="shared" si="0"/>
+        <v>9.0663668708242149</v>
+      </c>
+      <c r="G64" s="11">
+        <f t="shared" si="1"/>
+        <v>1.862791397578067</v>
+      </c>
     </row>
     <row r="65" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E65" s="12"/>
-      <c r="F65" s="12"/>
-      <c r="G65" s="12"/>
+      <c r="E65" s="7">
+        <f t="shared" si="2"/>
+        <v>1.2400000000000007</v>
+      </c>
+      <c r="F65" s="11">
+        <f t="shared" si="0"/>
+        <v>9.2149958359196926</v>
+      </c>
+      <c r="G65" s="11">
+        <f t="shared" si="1"/>
+        <v>1.7552915188498384</v>
+      </c>
     </row>
     <row r="66" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E66" s="12"/>
-      <c r="F66" s="12"/>
-      <c r="G66" s="12"/>
+      <c r="E66" s="7">
+        <f t="shared" si="2"/>
+        <v>1.2600000000000007</v>
+      </c>
+      <c r="F66" s="11">
+        <f t="shared" si="0"/>
+        <v>9.3636248010151721</v>
+      </c>
+      <c r="G66" s="11">
+        <f t="shared" si="1"/>
+        <v>1.6438676401216101</v>
+      </c>
     </row>
     <row r="67" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E67" s="12"/>
-      <c r="F67" s="12"/>
-      <c r="G67" s="12"/>
+      <c r="E67" s="7">
+        <f t="shared" si="2"/>
+        <v>1.2800000000000007</v>
+      </c>
+      <c r="F67" s="11">
+        <f t="shared" si="0"/>
+        <v>9.5122537661106517</v>
+      </c>
+      <c r="G67" s="11">
+        <f t="shared" si="1"/>
+        <v>1.5285197613933796</v>
+      </c>
     </row>
     <row r="68" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E68" s="12"/>
-      <c r="F68" s="12"/>
-      <c r="G68" s="12"/>
+      <c r="E68" s="7">
+        <f t="shared" si="2"/>
+        <v>1.3000000000000007</v>
+      </c>
+      <c r="F68" s="11">
+        <f t="shared" ref="F68:F78" si="3">E68*$C$4*COS($C$3)</f>
+        <v>9.6608827312061312</v>
+      </c>
+      <c r="G68" s="11">
+        <f t="shared" ref="G68:G78" si="4">$C$5+F68*TAN($C$3)-($C$6/(2*$C$4*$C$4))*(1+TAN($C$3)*TAN($C$3))*F68*F68</f>
+        <v>1.4092478826651522</v>
+      </c>
     </row>
     <row r="69" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E69" s="12"/>
-      <c r="F69" s="12"/>
-      <c r="G69" s="12"/>
+      <c r="E69" s="7">
+        <f t="shared" ref="E69:E78" si="5">E68+$C$7</f>
+        <v>1.3200000000000007</v>
+      </c>
+      <c r="F69" s="11">
+        <f t="shared" si="3"/>
+        <v>9.8095116963016089</v>
+      </c>
+      <c r="G69" s="11">
+        <f t="shared" si="4"/>
+        <v>1.2860520039369234</v>
+      </c>
     </row>
     <row r="70" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E70" s="12"/>
-      <c r="F70" s="12"/>
-      <c r="G70" s="12"/>
+      <c r="E70" s="7">
+        <f t="shared" si="5"/>
+        <v>1.3400000000000007</v>
+      </c>
+      <c r="F70" s="11">
+        <f t="shared" si="3"/>
+        <v>9.9581406613970884</v>
+      </c>
+      <c r="G70" s="11">
+        <f t="shared" si="4"/>
+        <v>1.1589321252086968</v>
+      </c>
     </row>
     <row r="71" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E71" s="12"/>
-      <c r="F71" s="12"/>
-      <c r="G71" s="12"/>
+      <c r="E71" s="7">
+        <f t="shared" si="5"/>
+        <v>1.3600000000000008</v>
+      </c>
+      <c r="F71" s="11">
+        <f t="shared" si="3"/>
+        <v>10.106769626492568</v>
+      </c>
+      <c r="G71" s="11">
+        <f t="shared" si="4"/>
+        <v>1.0278882464804671</v>
+      </c>
     </row>
     <row r="72" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E72" s="12"/>
-      <c r="F72" s="12"/>
-      <c r="G72" s="12"/>
+      <c r="E72" s="7">
+        <f t="shared" si="5"/>
+        <v>1.3800000000000008</v>
+      </c>
+      <c r="F72" s="11">
+        <f t="shared" si="3"/>
+        <v>10.255398591588046</v>
+      </c>
+      <c r="G72" s="11">
+        <f t="shared" si="4"/>
+        <v>0.89292036775223949</v>
+      </c>
     </row>
     <row r="73" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E73" s="12"/>
-      <c r="F73" s="12"/>
-      <c r="G73" s="12"/>
+      <c r="E73" s="7">
+        <f t="shared" si="5"/>
+        <v>1.4000000000000008</v>
+      </c>
+      <c r="F73" s="11">
+        <f t="shared" si="3"/>
+        <v>10.404027556683525</v>
+      </c>
+      <c r="G73" s="11">
+        <f t="shared" si="4"/>
+        <v>0.75402848902401054</v>
+      </c>
     </row>
     <row r="74" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E74" s="12"/>
-      <c r="F74" s="12"/>
-      <c r="G74" s="12"/>
+      <c r="E74" s="7">
+        <f t="shared" si="5"/>
+        <v>1.4200000000000008</v>
+      </c>
+      <c r="F74" s="11">
+        <f t="shared" si="3"/>
+        <v>10.552656521779005</v>
+      </c>
+      <c r="G74" s="11">
+        <f t="shared" si="4"/>
+        <v>0.611212610295782</v>
+      </c>
     </row>
     <row r="75" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E75" s="12"/>
-      <c r="F75" s="12"/>
-      <c r="G75" s="12"/>
+      <c r="E75" s="7">
+        <f t="shared" si="5"/>
+        <v>1.4400000000000008</v>
+      </c>
+      <c r="F75" s="11">
+        <f t="shared" si="3"/>
+        <v>10.701285486874484</v>
+      </c>
+      <c r="G75" s="11">
+        <f t="shared" si="4"/>
+        <v>0.46447273156755209</v>
+      </c>
     </row>
     <row r="76" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E76" s="12"/>
-      <c r="F76" s="12"/>
-      <c r="G76" s="12"/>
+      <c r="E76" s="7">
+        <f t="shared" si="5"/>
+        <v>1.4600000000000009</v>
+      </c>
+      <c r="F76" s="11">
+        <f t="shared" si="3"/>
+        <v>10.849914451969962</v>
+      </c>
+      <c r="G76" s="11">
+        <f t="shared" si="4"/>
+        <v>0.31380885283932436</v>
+      </c>
     </row>
     <row r="77" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E77" s="12"/>
-      <c r="F77" s="12"/>
-      <c r="G77" s="12"/>
+      <c r="E77" s="7">
+        <f t="shared" si="5"/>
+        <v>1.4800000000000009</v>
+      </c>
+      <c r="F77" s="11">
+        <f t="shared" si="3"/>
+        <v>10.998543417065441</v>
+      </c>
+      <c r="G77" s="11">
+        <f t="shared" si="4"/>
+        <v>0.15922097411109526</v>
+      </c>
     </row>
     <row r="78" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E78" s="12"/>
-      <c r="F78" s="12"/>
-      <c r="G78" s="12"/>
-    </row>
-    <row r="79" spans="5:7" x14ac:dyDescent="0.3">
-      <c r="E79" s="12"/>
-      <c r="F79" s="12"/>
-      <c r="G79" s="12"/>
+      <c r="E78" s="7">
+        <f t="shared" si="5"/>
+        <v>1.5000000000000009</v>
+      </c>
+      <c r="F78" s="11">
+        <f t="shared" si="3"/>
+        <v>11.147172382160921</v>
+      </c>
+      <c r="G78" s="11">
+        <f t="shared" si="4"/>
+        <v>7.0909538286656471E-4</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
initialized variables for a model to predict the time taken for a projectile to reach a certain point
</commit_message>
<xml_diff>
--- a/models.xlsx
+++ b/models.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssb\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1A685E8-BEBD-4513-BBD0-5EE86063088F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6511630F-927A-44E3-9625-272D73D29414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{6422CA17-FA72-4B85-908A-20157EF2E374}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{6422CA17-FA72-4B85-908A-20157EF2E374}"/>
   </bookViews>
   <sheets>
     <sheet name="model 1" sheetId="1" r:id="rId1"/>
     <sheet name="model 2" sheetId="2" r:id="rId2"/>
+    <sheet name="model 3" sheetId="3" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <r>
       <t>launch angle/</t>
@@ -245,6 +246,24 @@
   <si>
     <t>y/m</t>
   </si>
+  <si>
+    <t xml:space="preserve">Target X,Y in m </t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>g/ms⁻²</t>
+  </si>
+  <si>
+    <t>u/ms⁻¹</t>
+  </si>
+  <si>
+    <t>minimum launch speed/ ms⁻¹</t>
+  </si>
 </sst>
 </file>
 
@@ -291,7 +310,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -325,6 +344,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -406,7 +437,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -419,6 +450,12 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -15795,8 +15832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CCE5E17-412F-4B65-BE92-5E427918CCA8}">
   <dimension ref="B2:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:P80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16947,4 +16984,908 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEC10B89-8002-4438-80A5-6E69B9FCD18F}">
+  <dimension ref="B2:I115"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="24.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B2" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="12"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="12">
+        <v>1000</v>
+      </c>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="12">
+        <v>300</v>
+      </c>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="2">
+        <v>9.81</v>
+      </c>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="2">
+        <v>150</v>
+      </c>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="14">
+        <f>SQRT($C$5)*SQRT($C$4+SQRT(($C$3*$C$3)+($C$4*$C$4)))</f>
+        <v>114.82569697259082</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="16"/>
+      <c r="C8" s="17"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="17"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11" s="16"/>
+      <c r="C11" s="17"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="17"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="17"/>
+      <c r="I12" s="17"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="17"/>
+      <c r="H17" s="17"/>
+      <c r="I17" s="17"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E18" s="16"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="17"/>
+      <c r="I19" s="17"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="17"/>
+      <c r="H20" s="17"/>
+      <c r="I20" s="17"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="17"/>
+      <c r="H21" s="17"/>
+      <c r="I21" s="17"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="17"/>
+      <c r="I27" s="17"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="17"/>
+      <c r="I28" s="17"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="16"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="17"/>
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E41" s="16"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="17"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="17"/>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E42" s="16"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E43" s="16"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E44" s="16"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="17"/>
+      <c r="H45" s="17"/>
+      <c r="I45" s="17"/>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="17"/>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E48" s="16"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="17"/>
+      <c r="H48" s="17"/>
+      <c r="I48" s="17"/>
+    </row>
+    <row r="49" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E49" s="16"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
+      <c r="I49" s="17"/>
+    </row>
+    <row r="50" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E50" s="16"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
+    </row>
+    <row r="51" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E51" s="16"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="17"/>
+      <c r="H51" s="17"/>
+      <c r="I51" s="17"/>
+    </row>
+    <row r="52" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="17"/>
+      <c r="H52" s="17"/>
+      <c r="I52" s="17"/>
+    </row>
+    <row r="53" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E53" s="16"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="17"/>
+      <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
+    </row>
+    <row r="54" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E54" s="16"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="17"/>
+      <c r="H54" s="17"/>
+      <c r="I54" s="17"/>
+    </row>
+    <row r="55" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E55" s="16"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="17"/>
+      <c r="H55" s="17"/>
+      <c r="I55" s="17"/>
+    </row>
+    <row r="56" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="17"/>
+      <c r="H56" s="17"/>
+      <c r="I56" s="17"/>
+    </row>
+    <row r="57" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E57" s="16"/>
+      <c r="F57" s="16"/>
+      <c r="G57" s="17"/>
+      <c r="H57" s="17"/>
+      <c r="I57" s="17"/>
+    </row>
+    <row r="58" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E58" s="16"/>
+      <c r="F58" s="16"/>
+      <c r="G58" s="17"/>
+      <c r="H58" s="17"/>
+      <c r="I58" s="17"/>
+    </row>
+    <row r="59" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E59" s="16"/>
+      <c r="F59" s="16"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="17"/>
+      <c r="I59" s="17"/>
+    </row>
+    <row r="60" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E60" s="16"/>
+      <c r="F60" s="16"/>
+      <c r="G60" s="17"/>
+      <c r="H60" s="17"/>
+      <c r="I60" s="17"/>
+    </row>
+    <row r="61" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E61" s="16"/>
+      <c r="F61" s="16"/>
+      <c r="G61" s="17"/>
+      <c r="H61" s="17"/>
+      <c r="I61" s="17"/>
+    </row>
+    <row r="62" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E62" s="16"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="17"/>
+      <c r="H62" s="17"/>
+      <c r="I62" s="17"/>
+    </row>
+    <row r="63" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E63" s="16"/>
+      <c r="F63" s="16"/>
+      <c r="G63" s="17"/>
+      <c r="H63" s="17"/>
+      <c r="I63" s="17"/>
+    </row>
+    <row r="64" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="17"/>
+      <c r="H64" s="17"/>
+      <c r="I64" s="17"/>
+    </row>
+    <row r="65" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E65" s="16"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="17"/>
+      <c r="H65" s="17"/>
+      <c r="I65" s="17"/>
+    </row>
+    <row r="66" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E66" s="16"/>
+      <c r="F66" s="16"/>
+      <c r="G66" s="17"/>
+      <c r="H66" s="17"/>
+      <c r="I66" s="17"/>
+    </row>
+    <row r="67" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E67" s="16"/>
+      <c r="F67" s="16"/>
+      <c r="G67" s="17"/>
+      <c r="H67" s="17"/>
+      <c r="I67" s="17"/>
+    </row>
+    <row r="68" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E68" s="16"/>
+      <c r="F68" s="16"/>
+      <c r="G68" s="17"/>
+      <c r="H68" s="17"/>
+      <c r="I68" s="17"/>
+    </row>
+    <row r="69" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E69" s="16"/>
+      <c r="F69" s="16"/>
+      <c r="G69" s="17"/>
+      <c r="H69" s="17"/>
+      <c r="I69" s="17"/>
+    </row>
+    <row r="70" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E70" s="16"/>
+      <c r="F70" s="16"/>
+      <c r="G70" s="17"/>
+      <c r="H70" s="17"/>
+      <c r="I70" s="17"/>
+    </row>
+    <row r="71" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E71" s="16"/>
+      <c r="F71" s="16"/>
+      <c r="G71" s="17"/>
+      <c r="H71" s="17"/>
+      <c r="I71" s="17"/>
+    </row>
+    <row r="72" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E72" s="16"/>
+      <c r="F72" s="16"/>
+      <c r="G72" s="17"/>
+      <c r="H72" s="17"/>
+      <c r="I72" s="17"/>
+    </row>
+    <row r="73" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E73" s="16"/>
+      <c r="F73" s="16"/>
+      <c r="G73" s="17"/>
+      <c r="H73" s="17"/>
+      <c r="I73" s="17"/>
+    </row>
+    <row r="74" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E74" s="16"/>
+      <c r="F74" s="16"/>
+      <c r="G74" s="17"/>
+      <c r="H74" s="17"/>
+      <c r="I74" s="17"/>
+    </row>
+    <row r="75" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E75" s="16"/>
+      <c r="F75" s="16"/>
+      <c r="G75" s="17"/>
+      <c r="H75" s="17"/>
+      <c r="I75" s="17"/>
+    </row>
+    <row r="76" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E76" s="16"/>
+      <c r="F76" s="16"/>
+      <c r="G76" s="17"/>
+      <c r="H76" s="17"/>
+      <c r="I76" s="17"/>
+    </row>
+    <row r="77" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E77" s="16"/>
+      <c r="F77" s="16"/>
+      <c r="G77" s="17"/>
+      <c r="H77" s="17"/>
+      <c r="I77" s="17"/>
+    </row>
+    <row r="78" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E78" s="16"/>
+      <c r="F78" s="16"/>
+      <c r="G78" s="17"/>
+      <c r="H78" s="17"/>
+      <c r="I78" s="17"/>
+    </row>
+    <row r="79" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E79" s="16"/>
+      <c r="F79" s="16"/>
+      <c r="G79" s="17"/>
+      <c r="H79" s="17"/>
+      <c r="I79" s="17"/>
+    </row>
+    <row r="80" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E80" s="16"/>
+      <c r="F80" s="16"/>
+      <c r="G80" s="17"/>
+      <c r="H80" s="17"/>
+      <c r="I80" s="17"/>
+    </row>
+    <row r="81" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E81" s="16"/>
+      <c r="F81" s="16"/>
+      <c r="G81" s="17"/>
+      <c r="H81" s="17"/>
+      <c r="I81" s="17"/>
+    </row>
+    <row r="82" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E82" s="16"/>
+      <c r="F82" s="16"/>
+      <c r="G82" s="17"/>
+      <c r="H82" s="17"/>
+      <c r="I82" s="17"/>
+    </row>
+    <row r="83" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E83" s="16"/>
+      <c r="F83" s="16"/>
+      <c r="G83" s="17"/>
+      <c r="H83" s="17"/>
+      <c r="I83" s="17"/>
+    </row>
+    <row r="84" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E84" s="16"/>
+      <c r="F84" s="16"/>
+      <c r="G84" s="17"/>
+      <c r="H84" s="17"/>
+      <c r="I84" s="17"/>
+    </row>
+    <row r="85" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E85" s="16"/>
+      <c r="F85" s="16"/>
+      <c r="G85" s="17"/>
+      <c r="H85" s="17"/>
+      <c r="I85" s="17"/>
+    </row>
+    <row r="86" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E86" s="16"/>
+      <c r="F86" s="16"/>
+      <c r="G86" s="17"/>
+      <c r="H86" s="17"/>
+      <c r="I86" s="17"/>
+    </row>
+    <row r="87" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E87" s="16"/>
+      <c r="F87" s="16"/>
+      <c r="G87" s="17"/>
+      <c r="H87" s="17"/>
+      <c r="I87" s="17"/>
+    </row>
+    <row r="88" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E88" s="16"/>
+      <c r="F88" s="16"/>
+      <c r="G88" s="17"/>
+      <c r="H88" s="17"/>
+      <c r="I88" s="17"/>
+    </row>
+    <row r="89" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E89" s="16"/>
+      <c r="F89" s="16"/>
+      <c r="G89" s="17"/>
+      <c r="H89" s="17"/>
+      <c r="I89" s="17"/>
+    </row>
+    <row r="90" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E90" s="16"/>
+      <c r="F90" s="16"/>
+      <c r="G90" s="17"/>
+      <c r="H90" s="17"/>
+      <c r="I90" s="17"/>
+    </row>
+    <row r="91" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E91" s="16"/>
+      <c r="F91" s="16"/>
+      <c r="G91" s="17"/>
+      <c r="H91" s="17"/>
+      <c r="I91" s="17"/>
+    </row>
+    <row r="92" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E92" s="16"/>
+      <c r="F92" s="16"/>
+      <c r="G92" s="17"/>
+      <c r="H92" s="17"/>
+      <c r="I92" s="17"/>
+    </row>
+    <row r="93" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E93" s="16"/>
+      <c r="F93" s="16"/>
+      <c r="G93" s="17"/>
+      <c r="H93" s="17"/>
+      <c r="I93" s="17"/>
+    </row>
+    <row r="94" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E94" s="16"/>
+      <c r="F94" s="16"/>
+      <c r="G94" s="17"/>
+      <c r="H94" s="17"/>
+      <c r="I94" s="17"/>
+    </row>
+    <row r="95" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E95" s="16"/>
+      <c r="F95" s="16"/>
+      <c r="G95" s="17"/>
+      <c r="H95" s="17"/>
+      <c r="I95" s="17"/>
+    </row>
+    <row r="96" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E96" s="16"/>
+      <c r="F96" s="16"/>
+      <c r="G96" s="17"/>
+      <c r="H96" s="17"/>
+      <c r="I96" s="17"/>
+    </row>
+    <row r="97" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E97" s="16"/>
+      <c r="F97" s="16"/>
+      <c r="G97" s="17"/>
+      <c r="H97" s="17"/>
+      <c r="I97" s="17"/>
+    </row>
+    <row r="98" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E98" s="16"/>
+      <c r="F98" s="16"/>
+      <c r="G98" s="17"/>
+      <c r="H98" s="17"/>
+      <c r="I98" s="17"/>
+    </row>
+    <row r="99" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E99" s="16"/>
+      <c r="F99" s="16"/>
+      <c r="G99" s="17"/>
+      <c r="H99" s="17"/>
+      <c r="I99" s="17"/>
+    </row>
+    <row r="100" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E100" s="16"/>
+      <c r="F100" s="16"/>
+      <c r="G100" s="17"/>
+      <c r="H100" s="17"/>
+      <c r="I100" s="17"/>
+    </row>
+    <row r="101" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E101" s="16"/>
+      <c r="F101" s="16"/>
+      <c r="G101" s="17"/>
+      <c r="H101" s="17"/>
+      <c r="I101" s="17"/>
+    </row>
+    <row r="102" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E102" s="16"/>
+      <c r="F102" s="16"/>
+      <c r="G102" s="17"/>
+      <c r="H102" s="17"/>
+      <c r="I102" s="17"/>
+    </row>
+    <row r="103" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E103" s="16"/>
+      <c r="F103" s="16"/>
+      <c r="G103" s="17"/>
+      <c r="H103" s="17"/>
+      <c r="I103" s="17"/>
+    </row>
+    <row r="104" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E104" s="16"/>
+      <c r="F104" s="16"/>
+      <c r="G104" s="16"/>
+      <c r="H104" s="16"/>
+      <c r="I104" s="16"/>
+    </row>
+    <row r="105" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E105" s="16"/>
+      <c r="F105" s="16"/>
+      <c r="G105" s="16"/>
+      <c r="H105" s="16"/>
+      <c r="I105" s="16"/>
+    </row>
+    <row r="106" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E106" s="16"/>
+      <c r="F106" s="16"/>
+      <c r="G106" s="16"/>
+      <c r="H106" s="16"/>
+      <c r="I106" s="16"/>
+    </row>
+    <row r="107" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E107" s="16"/>
+      <c r="F107" s="16"/>
+      <c r="G107" s="16"/>
+      <c r="H107" s="16"/>
+      <c r="I107" s="16"/>
+    </row>
+    <row r="108" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E108" s="16"/>
+      <c r="F108" s="16"/>
+      <c r="G108" s="16"/>
+      <c r="H108" s="16"/>
+      <c r="I108" s="16"/>
+    </row>
+    <row r="109" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E109" s="16"/>
+      <c r="F109" s="16"/>
+      <c r="G109" s="16"/>
+      <c r="H109" s="16"/>
+      <c r="I109" s="16"/>
+    </row>
+    <row r="110" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E110" s="16"/>
+      <c r="F110" s="16"/>
+      <c r="G110" s="16"/>
+      <c r="H110" s="16"/>
+      <c r="I110" s="16"/>
+    </row>
+    <row r="111" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E111" s="16"/>
+      <c r="F111" s="16"/>
+      <c r="G111" s="16"/>
+      <c r="H111" s="16"/>
+      <c r="I111" s="16"/>
+    </row>
+    <row r="112" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E112" s="16"/>
+      <c r="F112" s="16"/>
+      <c r="G112" s="16"/>
+      <c r="H112" s="16"/>
+      <c r="I112" s="16"/>
+    </row>
+    <row r="113" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E113" s="16"/>
+      <c r="F113" s="16"/>
+      <c r="G113" s="16"/>
+      <c r="H113" s="16"/>
+      <c r="I113" s="16"/>
+    </row>
+    <row r="114" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E114" s="16"/>
+      <c r="F114" s="16"/>
+      <c r="G114" s="16"/>
+      <c r="H114" s="16"/>
+      <c r="I114" s="16"/>
+    </row>
+    <row r="115" spans="5:9" x14ac:dyDescent="0.3">
+      <c r="E115" s="16"/>
+      <c r="F115" s="16"/>
+      <c r="G115" s="16"/>
+      <c r="H115" s="16"/>
+      <c r="I115" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
calculated high ball and low ball equations for the projectile
</commit_message>
<xml_diff>
--- a/models.xlsx
+++ b/models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssb\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6511630F-927A-44E3-9625-272D73D29414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E469DFD4-47C0-47A0-97E7-3BD5811B30CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{6422CA17-FA72-4B85-908A-20157EF2E374}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <r>
       <t>launch angle/</t>
@@ -264,6 +264,21 @@
   <si>
     <t>minimum launch speed/ ms⁻¹</t>
   </si>
+  <si>
+    <t xml:space="preserve">High ball angle/ c </t>
+  </si>
+  <si>
+    <t>High ball angle/ °</t>
+  </si>
+  <si>
+    <t>Time of flight/ s</t>
+  </si>
+  <si>
+    <t>Low ball angle/ c</t>
+  </si>
+  <si>
+    <t>Low ball angle/ °</t>
+  </si>
 </sst>
 </file>
 
@@ -310,7 +325,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -359,8 +374,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -433,11 +454,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -453,7 +487,11 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -16991,7 +17029,7 @@
   <dimension ref="B2:I115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17004,11 +17042,11 @@
         <v>24</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="12" t="s">
@@ -17017,11 +17055,11 @@
       <c r="C3" s="12">
         <v>1000</v>
       </c>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -17030,11 +17068,11 @@
       <c r="C4" s="12">
         <v>300</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
@@ -17043,11 +17081,11 @@
       <c r="C5" s="2">
         <v>9.81</v>
       </c>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
@@ -17056,11 +17094,11 @@
       <c r="C6" s="2">
         <v>150</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="13" t="s">
@@ -17070,820 +17108,850 @@
         <f>SQRT($C$5)*SQRT($C$4+SQRT(($C$3*$C$3)+($C$4*$C$4)))</f>
         <v>114.82569697259082</v>
       </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="16"/>
-      <c r="C8" s="17"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
+      <c r="B8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="15">
+        <f>ATAN(($C$3+SQRT($C$3*$C$3-(4*(($C$5/(2*$C$6*$C$6))*$C$3*$C$3)*($C$4+(($C$5*$C$3*$C$3)/(2*$C$6*$C$6))))))/(2*(($C$5/(2*$C$6*$C$6))*$C$3*$C$3)))</f>
+        <v>1.3253412479491977</v>
+      </c>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
+      <c r="B9" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="15">
+        <f>$C$8*(180/PI())</f>
+        <v>75.936459922090606</v>
+      </c>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
+      <c r="B10" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="15">
+        <f>$C$3/($C$6*COS($C$8))</f>
+        <v>27.435091916779431</v>
+      </c>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="16"/>
-      <c r="C11" s="17"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
+      <c r="B11" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="17">
+        <f>ATAN(($C$3-SQRT($C$3*$C$3-(4*(($C$5/(2*$C$6*$C$6))*$C$3*$C$3)*($C$4+(($C$5*$C$3*$C$3)/(2*$C$6*$C$6))))))/(2*(($C$5/(2*$C$6*$C$6))*$C$3*$C$3)))</f>
+        <v>0.53691187332356594</v>
+      </c>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
+      <c r="B12" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="19">
+        <f>$C$11*(180/PI())</f>
+        <v>30.762784311903019</v>
+      </c>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="17"/>
-      <c r="I13" s="17"/>
+      <c r="B13" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="17">
+        <f>$C$3/($C$6*COS($C$11))</f>
+        <v>7.7583223067140521</v>
+      </c>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
-      <c r="I14" s="17"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="17"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E18" s="16"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="17"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E20" s="16"/>
-      <c r="F20" s="16"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="17"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
+      <c r="G20" s="21"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="17"/>
+      <c r="C21" s="18"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="16"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
+      <c r="C22" s="18"/>
+      <c r="D22" s="18"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="16"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="17"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="17"/>
-      <c r="I24" s="17"/>
+      <c r="C24" s="18"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="16"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17"/>
+      <c r="C25" s="18"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="16"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="17"/>
+      <c r="C26" s="18"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="16"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="17"/>
+      <c r="C27" s="18"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="17"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="17"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="16"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="17"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="18"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="16"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="17"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="17"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="16"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="G37" s="17"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="17"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="17"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E39" s="16"/>
-      <c r="F39" s="16"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="17"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E40" s="16"/>
-      <c r="F40" s="16"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="17"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E41" s="16"/>
-      <c r="F41" s="16"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
-      <c r="I41" s="17"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E42" s="16"/>
-      <c r="F42" s="16"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17"/>
-      <c r="I42" s="17"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="21"/>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E43" s="16"/>
-      <c r="F43" s="16"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17"/>
-      <c r="I43" s="17"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="21"/>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E44" s="16"/>
-      <c r="F44" s="16"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="17"/>
-      <c r="I44" s="17"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="21"/>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E45" s="16"/>
-      <c r="F45" s="16"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17"/>
-      <c r="I45" s="17"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E46" s="16"/>
-      <c r="F46" s="16"/>
-      <c r="G46" s="17"/>
-      <c r="H46" s="17"/>
-      <c r="I46" s="17"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="G47" s="17"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="17"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="21"/>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E48" s="16"/>
-      <c r="F48" s="16"/>
-      <c r="G48" s="17"/>
-      <c r="H48" s="17"/>
-      <c r="I48" s="17"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="21"/>
     </row>
     <row r="49" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E49" s="16"/>
-      <c r="F49" s="16"/>
-      <c r="G49" s="17"/>
-      <c r="H49" s="17"/>
-      <c r="I49" s="17"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="21"/>
     </row>
     <row r="50" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E50" s="16"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="17"/>
-      <c r="H50" s="17"/>
-      <c r="I50" s="17"/>
+      <c r="E50" s="20"/>
+      <c r="F50" s="20"/>
+      <c r="G50" s="21"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="21"/>
     </row>
     <row r="51" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E51" s="16"/>
-      <c r="F51" s="16"/>
-      <c r="G51" s="17"/>
-      <c r="H51" s="17"/>
-      <c r="I51" s="17"/>
+      <c r="E51" s="20"/>
+      <c r="F51" s="20"/>
+      <c r="G51" s="21"/>
+      <c r="H51" s="21"/>
+      <c r="I51" s="21"/>
     </row>
     <row r="52" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E52" s="16"/>
-      <c r="F52" s="16"/>
-      <c r="G52" s="17"/>
-      <c r="H52" s="17"/>
-      <c r="I52" s="17"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+      <c r="G52" s="21"/>
+      <c r="H52" s="21"/>
+      <c r="I52" s="21"/>
     </row>
     <row r="53" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E53" s="16"/>
-      <c r="F53" s="16"/>
-      <c r="G53" s="17"/>
-      <c r="H53" s="17"/>
-      <c r="I53" s="17"/>
+      <c r="E53" s="20"/>
+      <c r="F53" s="20"/>
+      <c r="G53" s="21"/>
+      <c r="H53" s="21"/>
+      <c r="I53" s="21"/>
     </row>
     <row r="54" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E54" s="16"/>
-      <c r="F54" s="16"/>
-      <c r="G54" s="17"/>
-      <c r="H54" s="17"/>
-      <c r="I54" s="17"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="21"/>
+      <c r="H54" s="21"/>
+      <c r="I54" s="21"/>
     </row>
     <row r="55" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E55" s="16"/>
-      <c r="F55" s="16"/>
-      <c r="G55" s="17"/>
-      <c r="H55" s="17"/>
-      <c r="I55" s="17"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="21"/>
+      <c r="H55" s="21"/>
+      <c r="I55" s="21"/>
     </row>
     <row r="56" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E56" s="16"/>
-      <c r="F56" s="16"/>
-      <c r="G56" s="17"/>
-      <c r="H56" s="17"/>
-      <c r="I56" s="17"/>
+      <c r="E56" s="20"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="21"/>
+      <c r="H56" s="21"/>
+      <c r="I56" s="21"/>
     </row>
     <row r="57" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E57" s="16"/>
-      <c r="F57" s="16"/>
-      <c r="G57" s="17"/>
-      <c r="H57" s="17"/>
-      <c r="I57" s="17"/>
+      <c r="E57" s="20"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="21"/>
+      <c r="H57" s="21"/>
+      <c r="I57" s="21"/>
     </row>
     <row r="58" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E58" s="16"/>
-      <c r="F58" s="16"/>
-      <c r="G58" s="17"/>
-      <c r="H58" s="17"/>
-      <c r="I58" s="17"/>
+      <c r="E58" s="20"/>
+      <c r="F58" s="20"/>
+      <c r="G58" s="21"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="21"/>
     </row>
     <row r="59" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E59" s="16"/>
-      <c r="F59" s="16"/>
-      <c r="G59" s="17"/>
-      <c r="H59" s="17"/>
-      <c r="I59" s="17"/>
+      <c r="E59" s="20"/>
+      <c r="F59" s="20"/>
+      <c r="G59" s="21"/>
+      <c r="H59" s="21"/>
+      <c r="I59" s="21"/>
     </row>
     <row r="60" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E60" s="16"/>
-      <c r="F60" s="16"/>
-      <c r="G60" s="17"/>
-      <c r="H60" s="17"/>
-      <c r="I60" s="17"/>
+      <c r="E60" s="20"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="21"/>
+      <c r="H60" s="21"/>
+      <c r="I60" s="21"/>
     </row>
     <row r="61" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E61" s="16"/>
-      <c r="F61" s="16"/>
-      <c r="G61" s="17"/>
-      <c r="H61" s="17"/>
-      <c r="I61" s="17"/>
+      <c r="E61" s="20"/>
+      <c r="F61" s="20"/>
+      <c r="G61" s="21"/>
+      <c r="H61" s="21"/>
+      <c r="I61" s="21"/>
     </row>
     <row r="62" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E62" s="16"/>
-      <c r="F62" s="16"/>
-      <c r="G62" s="17"/>
-      <c r="H62" s="17"/>
-      <c r="I62" s="17"/>
+      <c r="E62" s="20"/>
+      <c r="F62" s="20"/>
+      <c r="G62" s="21"/>
+      <c r="H62" s="21"/>
+      <c r="I62" s="21"/>
     </row>
     <row r="63" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E63" s="16"/>
-      <c r="F63" s="16"/>
-      <c r="G63" s="17"/>
-      <c r="H63" s="17"/>
-      <c r="I63" s="17"/>
+      <c r="E63" s="20"/>
+      <c r="F63" s="20"/>
+      <c r="G63" s="21"/>
+      <c r="H63" s="21"/>
+      <c r="I63" s="21"/>
     </row>
     <row r="64" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E64" s="16"/>
-      <c r="F64" s="16"/>
-      <c r="G64" s="17"/>
-      <c r="H64" s="17"/>
-      <c r="I64" s="17"/>
+      <c r="E64" s="20"/>
+      <c r="F64" s="20"/>
+      <c r="G64" s="21"/>
+      <c r="H64" s="21"/>
+      <c r="I64" s="21"/>
     </row>
     <row r="65" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E65" s="16"/>
-      <c r="F65" s="16"/>
-      <c r="G65" s="17"/>
-      <c r="H65" s="17"/>
-      <c r="I65" s="17"/>
+      <c r="E65" s="20"/>
+      <c r="F65" s="20"/>
+      <c r="G65" s="21"/>
+      <c r="H65" s="21"/>
+      <c r="I65" s="21"/>
     </row>
     <row r="66" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E66" s="16"/>
-      <c r="F66" s="16"/>
-      <c r="G66" s="17"/>
-      <c r="H66" s="17"/>
-      <c r="I66" s="17"/>
+      <c r="E66" s="20"/>
+      <c r="F66" s="20"/>
+      <c r="G66" s="21"/>
+      <c r="H66" s="21"/>
+      <c r="I66" s="21"/>
     </row>
     <row r="67" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E67" s="16"/>
-      <c r="F67" s="16"/>
-      <c r="G67" s="17"/>
-      <c r="H67" s="17"/>
-      <c r="I67" s="17"/>
+      <c r="E67" s="20"/>
+      <c r="F67" s="20"/>
+      <c r="G67" s="21"/>
+      <c r="H67" s="21"/>
+      <c r="I67" s="21"/>
     </row>
     <row r="68" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E68" s="16"/>
-      <c r="F68" s="16"/>
-      <c r="G68" s="17"/>
-      <c r="H68" s="17"/>
-      <c r="I68" s="17"/>
+      <c r="E68" s="20"/>
+      <c r="F68" s="20"/>
+      <c r="G68" s="21"/>
+      <c r="H68" s="21"/>
+      <c r="I68" s="21"/>
     </row>
     <row r="69" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E69" s="16"/>
-      <c r="F69" s="16"/>
-      <c r="G69" s="17"/>
-      <c r="H69" s="17"/>
-      <c r="I69" s="17"/>
+      <c r="E69" s="20"/>
+      <c r="F69" s="20"/>
+      <c r="G69" s="21"/>
+      <c r="H69" s="21"/>
+      <c r="I69" s="21"/>
     </row>
     <row r="70" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E70" s="16"/>
-      <c r="F70" s="16"/>
-      <c r="G70" s="17"/>
-      <c r="H70" s="17"/>
-      <c r="I70" s="17"/>
+      <c r="E70" s="20"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="21"/>
+      <c r="H70" s="21"/>
+      <c r="I70" s="21"/>
     </row>
     <row r="71" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E71" s="16"/>
-      <c r="F71" s="16"/>
-      <c r="G71" s="17"/>
-      <c r="H71" s="17"/>
-      <c r="I71" s="17"/>
+      <c r="E71" s="20"/>
+      <c r="F71" s="20"/>
+      <c r="G71" s="21"/>
+      <c r="H71" s="21"/>
+      <c r="I71" s="21"/>
     </row>
     <row r="72" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E72" s="16"/>
-      <c r="F72" s="16"/>
-      <c r="G72" s="17"/>
-      <c r="H72" s="17"/>
-      <c r="I72" s="17"/>
+      <c r="E72" s="20"/>
+      <c r="F72" s="20"/>
+      <c r="G72" s="21"/>
+      <c r="H72" s="21"/>
+      <c r="I72" s="21"/>
     </row>
     <row r="73" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E73" s="16"/>
-      <c r="F73" s="16"/>
-      <c r="G73" s="17"/>
-      <c r="H73" s="17"/>
-      <c r="I73" s="17"/>
+      <c r="E73" s="20"/>
+      <c r="F73" s="20"/>
+      <c r="G73" s="21"/>
+      <c r="H73" s="21"/>
+      <c r="I73" s="21"/>
     </row>
     <row r="74" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E74" s="16"/>
-      <c r="F74" s="16"/>
-      <c r="G74" s="17"/>
-      <c r="H74" s="17"/>
-      <c r="I74" s="17"/>
+      <c r="E74" s="20"/>
+      <c r="F74" s="20"/>
+      <c r="G74" s="21"/>
+      <c r="H74" s="21"/>
+      <c r="I74" s="21"/>
     </row>
     <row r="75" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E75" s="16"/>
-      <c r="F75" s="16"/>
-      <c r="G75" s="17"/>
-      <c r="H75" s="17"/>
-      <c r="I75" s="17"/>
+      <c r="E75" s="20"/>
+      <c r="F75" s="20"/>
+      <c r="G75" s="21"/>
+      <c r="H75" s="21"/>
+      <c r="I75" s="21"/>
     </row>
     <row r="76" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E76" s="16"/>
-      <c r="F76" s="16"/>
-      <c r="G76" s="17"/>
-      <c r="H76" s="17"/>
-      <c r="I76" s="17"/>
+      <c r="E76" s="20"/>
+      <c r="F76" s="20"/>
+      <c r="G76" s="21"/>
+      <c r="H76" s="21"/>
+      <c r="I76" s="21"/>
     </row>
     <row r="77" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E77" s="16"/>
-      <c r="F77" s="16"/>
-      <c r="G77" s="17"/>
-      <c r="H77" s="17"/>
-      <c r="I77" s="17"/>
+      <c r="E77" s="20"/>
+      <c r="F77" s="20"/>
+      <c r="G77" s="21"/>
+      <c r="H77" s="21"/>
+      <c r="I77" s="21"/>
     </row>
     <row r="78" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E78" s="16"/>
-      <c r="F78" s="16"/>
-      <c r="G78" s="17"/>
-      <c r="H78" s="17"/>
-      <c r="I78" s="17"/>
+      <c r="E78" s="20"/>
+      <c r="F78" s="20"/>
+      <c r="G78" s="21"/>
+      <c r="H78" s="21"/>
+      <c r="I78" s="21"/>
     </row>
     <row r="79" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E79" s="16"/>
-      <c r="F79" s="16"/>
-      <c r="G79" s="17"/>
-      <c r="H79" s="17"/>
-      <c r="I79" s="17"/>
+      <c r="E79" s="20"/>
+      <c r="F79" s="20"/>
+      <c r="G79" s="21"/>
+      <c r="H79" s="21"/>
+      <c r="I79" s="21"/>
     </row>
     <row r="80" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E80" s="16"/>
-      <c r="F80" s="16"/>
-      <c r="G80" s="17"/>
-      <c r="H80" s="17"/>
-      <c r="I80" s="17"/>
+      <c r="E80" s="20"/>
+      <c r="F80" s="20"/>
+      <c r="G80" s="21"/>
+      <c r="H80" s="21"/>
+      <c r="I80" s="21"/>
     </row>
     <row r="81" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E81" s="16"/>
-      <c r="F81" s="16"/>
-      <c r="G81" s="17"/>
-      <c r="H81" s="17"/>
-      <c r="I81" s="17"/>
+      <c r="E81" s="20"/>
+      <c r="F81" s="20"/>
+      <c r="G81" s="21"/>
+      <c r="H81" s="21"/>
+      <c r="I81" s="21"/>
     </row>
     <row r="82" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E82" s="16"/>
-      <c r="F82" s="16"/>
-      <c r="G82" s="17"/>
-      <c r="H82" s="17"/>
-      <c r="I82" s="17"/>
+      <c r="E82" s="20"/>
+      <c r="F82" s="20"/>
+      <c r="G82" s="21"/>
+      <c r="H82" s="21"/>
+      <c r="I82" s="21"/>
     </row>
     <row r="83" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E83" s="16"/>
-      <c r="F83" s="16"/>
-      <c r="G83" s="17"/>
-      <c r="H83" s="17"/>
-      <c r="I83" s="17"/>
+      <c r="E83" s="20"/>
+      <c r="F83" s="20"/>
+      <c r="G83" s="21"/>
+      <c r="H83" s="21"/>
+      <c r="I83" s="21"/>
     </row>
     <row r="84" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E84" s="16"/>
-      <c r="F84" s="16"/>
-      <c r="G84" s="17"/>
-      <c r="H84" s="17"/>
-      <c r="I84" s="17"/>
+      <c r="E84" s="20"/>
+      <c r="F84" s="20"/>
+      <c r="G84" s="21"/>
+      <c r="H84" s="21"/>
+      <c r="I84" s="21"/>
     </row>
     <row r="85" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E85" s="16"/>
-      <c r="F85" s="16"/>
-      <c r="G85" s="17"/>
-      <c r="H85" s="17"/>
-      <c r="I85" s="17"/>
+      <c r="E85" s="20"/>
+      <c r="F85" s="20"/>
+      <c r="G85" s="21"/>
+      <c r="H85" s="21"/>
+      <c r="I85" s="21"/>
     </row>
     <row r="86" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E86" s="16"/>
-      <c r="F86" s="16"/>
-      <c r="G86" s="17"/>
-      <c r="H86" s="17"/>
-      <c r="I86" s="17"/>
+      <c r="E86" s="20"/>
+      <c r="F86" s="20"/>
+      <c r="G86" s="21"/>
+      <c r="H86" s="21"/>
+      <c r="I86" s="21"/>
     </row>
     <row r="87" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E87" s="16"/>
-      <c r="F87" s="16"/>
-      <c r="G87" s="17"/>
-      <c r="H87" s="17"/>
-      <c r="I87" s="17"/>
+      <c r="E87" s="20"/>
+      <c r="F87" s="20"/>
+      <c r="G87" s="21"/>
+      <c r="H87" s="21"/>
+      <c r="I87" s="21"/>
     </row>
     <row r="88" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E88" s="16"/>
-      <c r="F88" s="16"/>
-      <c r="G88" s="17"/>
-      <c r="H88" s="17"/>
-      <c r="I88" s="17"/>
+      <c r="E88" s="20"/>
+      <c r="F88" s="20"/>
+      <c r="G88" s="21"/>
+      <c r="H88" s="21"/>
+      <c r="I88" s="21"/>
     </row>
     <row r="89" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E89" s="16"/>
-      <c r="F89" s="16"/>
-      <c r="G89" s="17"/>
-      <c r="H89" s="17"/>
-      <c r="I89" s="17"/>
+      <c r="E89" s="20"/>
+      <c r="F89" s="20"/>
+      <c r="G89" s="21"/>
+      <c r="H89" s="21"/>
+      <c r="I89" s="21"/>
     </row>
     <row r="90" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E90" s="16"/>
-      <c r="F90" s="16"/>
-      <c r="G90" s="17"/>
-      <c r="H90" s="17"/>
-      <c r="I90" s="17"/>
+      <c r="E90" s="20"/>
+      <c r="F90" s="20"/>
+      <c r="G90" s="21"/>
+      <c r="H90" s="21"/>
+      <c r="I90" s="21"/>
     </row>
     <row r="91" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E91" s="16"/>
-      <c r="F91" s="16"/>
-      <c r="G91" s="17"/>
-      <c r="H91" s="17"/>
-      <c r="I91" s="17"/>
+      <c r="E91" s="20"/>
+      <c r="F91" s="20"/>
+      <c r="G91" s="21"/>
+      <c r="H91" s="21"/>
+      <c r="I91" s="21"/>
     </row>
     <row r="92" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E92" s="16"/>
-      <c r="F92" s="16"/>
-      <c r="G92" s="17"/>
-      <c r="H92" s="17"/>
-      <c r="I92" s="17"/>
+      <c r="E92" s="20"/>
+      <c r="F92" s="20"/>
+      <c r="G92" s="21"/>
+      <c r="H92" s="21"/>
+      <c r="I92" s="21"/>
     </row>
     <row r="93" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E93" s="16"/>
-      <c r="F93" s="16"/>
-      <c r="G93" s="17"/>
-      <c r="H93" s="17"/>
-      <c r="I93" s="17"/>
+      <c r="E93" s="20"/>
+      <c r="F93" s="20"/>
+      <c r="G93" s="21"/>
+      <c r="H93" s="21"/>
+      <c r="I93" s="21"/>
     </row>
     <row r="94" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E94" s="16"/>
-      <c r="F94" s="16"/>
-      <c r="G94" s="17"/>
-      <c r="H94" s="17"/>
-      <c r="I94" s="17"/>
+      <c r="E94" s="20"/>
+      <c r="F94" s="20"/>
+      <c r="G94" s="21"/>
+      <c r="H94" s="21"/>
+      <c r="I94" s="21"/>
     </row>
     <row r="95" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E95" s="16"/>
-      <c r="F95" s="16"/>
-      <c r="G95" s="17"/>
-      <c r="H95" s="17"/>
-      <c r="I95" s="17"/>
+      <c r="E95" s="20"/>
+      <c r="F95" s="20"/>
+      <c r="G95" s="21"/>
+      <c r="H95" s="21"/>
+      <c r="I95" s="21"/>
     </row>
     <row r="96" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E96" s="16"/>
-      <c r="F96" s="16"/>
-      <c r="G96" s="17"/>
-      <c r="H96" s="17"/>
-      <c r="I96" s="17"/>
+      <c r="E96" s="20"/>
+      <c r="F96" s="20"/>
+      <c r="G96" s="21"/>
+      <c r="H96" s="21"/>
+      <c r="I96" s="21"/>
     </row>
     <row r="97" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E97" s="16"/>
-      <c r="F97" s="16"/>
-      <c r="G97" s="17"/>
-      <c r="H97" s="17"/>
-      <c r="I97" s="17"/>
+      <c r="E97" s="20"/>
+      <c r="F97" s="20"/>
+      <c r="G97" s="21"/>
+      <c r="H97" s="21"/>
+      <c r="I97" s="21"/>
     </row>
     <row r="98" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E98" s="16"/>
-      <c r="F98" s="16"/>
-      <c r="G98" s="17"/>
-      <c r="H98" s="17"/>
-      <c r="I98" s="17"/>
+      <c r="E98" s="20"/>
+      <c r="F98" s="20"/>
+      <c r="G98" s="21"/>
+      <c r="H98" s="21"/>
+      <c r="I98" s="21"/>
     </row>
     <row r="99" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E99" s="16"/>
-      <c r="F99" s="16"/>
-      <c r="G99" s="17"/>
-      <c r="H99" s="17"/>
-      <c r="I99" s="17"/>
+      <c r="E99" s="20"/>
+      <c r="F99" s="20"/>
+      <c r="G99" s="21"/>
+      <c r="H99" s="21"/>
+      <c r="I99" s="21"/>
     </row>
     <row r="100" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E100" s="16"/>
-      <c r="F100" s="16"/>
-      <c r="G100" s="17"/>
-      <c r="H100" s="17"/>
-      <c r="I100" s="17"/>
+      <c r="E100" s="20"/>
+      <c r="F100" s="20"/>
+      <c r="G100" s="21"/>
+      <c r="H100" s="21"/>
+      <c r="I100" s="21"/>
     </row>
     <row r="101" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E101" s="16"/>
-      <c r="F101" s="16"/>
-      <c r="G101" s="17"/>
-      <c r="H101" s="17"/>
-      <c r="I101" s="17"/>
+      <c r="E101" s="20"/>
+      <c r="F101" s="20"/>
+      <c r="G101" s="21"/>
+      <c r="H101" s="21"/>
+      <c r="I101" s="21"/>
     </row>
     <row r="102" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E102" s="16"/>
-      <c r="F102" s="16"/>
-      <c r="G102" s="17"/>
-      <c r="H102" s="17"/>
-      <c r="I102" s="17"/>
+      <c r="E102" s="20"/>
+      <c r="F102" s="20"/>
+      <c r="G102" s="21"/>
+      <c r="H102" s="21"/>
+      <c r="I102" s="21"/>
     </row>
     <row r="103" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E103" s="16"/>
-      <c r="F103" s="16"/>
-      <c r="G103" s="17"/>
-      <c r="H103" s="17"/>
-      <c r="I103" s="17"/>
+      <c r="E103" s="20"/>
+      <c r="F103" s="20"/>
+      <c r="G103" s="21"/>
+      <c r="H103" s="21"/>
+      <c r="I103" s="21"/>
     </row>
     <row r="104" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E104" s="16"/>
-      <c r="F104" s="16"/>
-      <c r="G104" s="16"/>
-      <c r="H104" s="16"/>
-      <c r="I104" s="16"/>
+      <c r="E104" s="20"/>
+      <c r="F104" s="20"/>
+      <c r="G104" s="20"/>
+      <c r="H104" s="20"/>
+      <c r="I104" s="20"/>
     </row>
     <row r="105" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E105" s="16"/>
-      <c r="F105" s="16"/>
-      <c r="G105" s="16"/>
-      <c r="H105" s="16"/>
-      <c r="I105" s="16"/>
+      <c r="E105" s="20"/>
+      <c r="F105" s="20"/>
+      <c r="G105" s="20"/>
+      <c r="H105" s="20"/>
+      <c r="I105" s="20"/>
     </row>
     <row r="106" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E106" s="16"/>
-      <c r="F106" s="16"/>
-      <c r="G106" s="16"/>
-      <c r="H106" s="16"/>
-      <c r="I106" s="16"/>
+      <c r="E106" s="20"/>
+      <c r="F106" s="20"/>
+      <c r="G106" s="20"/>
+      <c r="H106" s="20"/>
+      <c r="I106" s="20"/>
     </row>
     <row r="107" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E107" s="16"/>
-      <c r="F107" s="16"/>
-      <c r="G107" s="16"/>
-      <c r="H107" s="16"/>
-      <c r="I107" s="16"/>
+      <c r="E107" s="20"/>
+      <c r="F107" s="20"/>
+      <c r="G107" s="20"/>
+      <c r="H107" s="20"/>
+      <c r="I107" s="20"/>
     </row>
     <row r="108" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E108" s="16"/>
-      <c r="F108" s="16"/>
-      <c r="G108" s="16"/>
-      <c r="H108" s="16"/>
-      <c r="I108" s="16"/>
+      <c r="E108" s="20"/>
+      <c r="F108" s="20"/>
+      <c r="G108" s="20"/>
+      <c r="H108" s="20"/>
+      <c r="I108" s="20"/>
     </row>
     <row r="109" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E109" s="16"/>
-      <c r="F109" s="16"/>
-      <c r="G109" s="16"/>
-      <c r="H109" s="16"/>
-      <c r="I109" s="16"/>
+      <c r="E109" s="20"/>
+      <c r="F109" s="20"/>
+      <c r="G109" s="20"/>
+      <c r="H109" s="20"/>
+      <c r="I109" s="20"/>
     </row>
     <row r="110" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E110" s="16"/>
-      <c r="F110" s="16"/>
-      <c r="G110" s="16"/>
-      <c r="H110" s="16"/>
-      <c r="I110" s="16"/>
+      <c r="E110" s="20"/>
+      <c r="F110" s="20"/>
+      <c r="G110" s="20"/>
+      <c r="H110" s="20"/>
+      <c r="I110" s="20"/>
     </row>
     <row r="111" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E111" s="16"/>
-      <c r="F111" s="16"/>
-      <c r="G111" s="16"/>
-      <c r="H111" s="16"/>
-      <c r="I111" s="16"/>
+      <c r="E111" s="20"/>
+      <c r="F111" s="20"/>
+      <c r="G111" s="20"/>
+      <c r="H111" s="20"/>
+      <c r="I111" s="20"/>
     </row>
     <row r="112" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E112" s="16"/>
-      <c r="F112" s="16"/>
-      <c r="G112" s="16"/>
-      <c r="H112" s="16"/>
-      <c r="I112" s="16"/>
+      <c r="E112" s="20"/>
+      <c r="F112" s="20"/>
+      <c r="G112" s="20"/>
+      <c r="H112" s="20"/>
+      <c r="I112" s="20"/>
     </row>
     <row r="113" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E113" s="16"/>
-      <c r="F113" s="16"/>
-      <c r="G113" s="16"/>
-      <c r="H113" s="16"/>
-      <c r="I113" s="16"/>
+      <c r="E113" s="20"/>
+      <c r="F113" s="20"/>
+      <c r="G113" s="20"/>
+      <c r="H113" s="20"/>
+      <c r="I113" s="20"/>
     </row>
     <row r="114" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E114" s="16"/>
-      <c r="F114" s="16"/>
-      <c r="G114" s="16"/>
-      <c r="H114" s="16"/>
-      <c r="I114" s="16"/>
+      <c r="E114" s="20"/>
+      <c r="F114" s="20"/>
+      <c r="G114" s="20"/>
+      <c r="H114" s="20"/>
+      <c r="I114" s="20"/>
     </row>
     <row r="115" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E115" s="16"/>
-      <c r="F115" s="16"/>
-      <c r="G115" s="16"/>
-      <c r="H115" s="16"/>
-      <c r="I115" s="16"/>
+      <c r="E115" s="20"/>
+      <c r="F115" s="20"/>
+      <c r="G115" s="20"/>
+      <c r="H115" s="20"/>
+      <c r="I115" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
calculated minimum values, initialised x and y values
</commit_message>
<xml_diff>
--- a/models.xlsx
+++ b/models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssb\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E469DFD4-47C0-47A0-97E7-3BD5811B30CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF512D7-D07A-4D50-8390-A16B5F2B6ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{6422CA17-FA72-4B85-908A-20157EF2E374}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <r>
       <t>launch angle/</t>
@@ -279,6 +279,21 @@
   <si>
     <t>Low ball angle/ °</t>
   </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>y low ball</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum speed angle/ c </t>
+  </si>
+  <si>
+    <t>Minimum speed angle/ °</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time of flight/s </t>
+  </si>
 </sst>
 </file>
 
@@ -325,7 +340,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -380,8 +395,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -454,24 +475,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -490,10 +498,11 @@
     <xf numFmtId="2" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -17029,7 +17038,7 @@
   <dimension ref="B2:I115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17042,9 +17051,15 @@
         <v>24</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
+      <c r="E2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>36</v>
+      </c>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
     </row>
@@ -17055,9 +17070,16 @@
       <c r="C3" s="12">
         <v>1000</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="21"/>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="22">
+        <v>0</v>
+      </c>
+      <c r="G3" s="17">
+        <f t="shared" ref="G3:G16" si="0">F3*TAN($C$11)-($C$5/(2*$C$6*$C$6))*(1+(TAN($C$11)*TAN($C$11)))*F3*F3</f>
+        <v>0</v>
+      </c>
       <c r="H3" s="21"/>
       <c r="I3" s="21"/>
     </row>
@@ -17068,9 +17090,18 @@
       <c r="C4" s="12">
         <v>300</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="21"/>
+      <c r="E4" s="7">
+        <f>E3+0.01</f>
+        <v>0.01</v>
+      </c>
+      <c r="F4" s="22">
+        <f>F3+10</f>
+        <v>10</v>
+      </c>
+      <c r="G4" s="17">
+        <f t="shared" si="0"/>
+        <v>5.9228723013389413</v>
+      </c>
       <c r="H4" s="21"/>
       <c r="I4" s="21"/>
     </row>
@@ -17081,9 +17112,18 @@
       <c r="C5" s="2">
         <v>9.81</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="21"/>
+      <c r="E5" s="7">
+        <f t="shared" ref="E5:E68" si="1">E4+0.01</f>
+        <v>0.02</v>
+      </c>
+      <c r="F5" s="22">
+        <f t="shared" ref="F5:F68" si="2">F4+10</f>
+        <v>20</v>
+      </c>
+      <c r="G5" s="17">
+        <f t="shared" si="0"/>
+        <v>11.786696677398309</v>
+      </c>
       <c r="H5" s="21"/>
       <c r="I5" s="21"/>
     </row>
@@ -17094,9 +17134,18 @@
       <c r="C6" s="2">
         <v>150</v>
       </c>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="21"/>
+      <c r="E6" s="7">
+        <f t="shared" si="1"/>
+        <v>0.03</v>
+      </c>
+      <c r="F6" s="22">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="G6" s="17">
+        <f t="shared" si="0"/>
+        <v>17.591473128178098</v>
+      </c>
       <c r="H6" s="21"/>
       <c r="I6" s="21"/>
     </row>
@@ -17108,9 +17157,18 @@
         <f>SQRT($C$5)*SQRT($C$4+SQRT(($C$3*$C$3)+($C$4*$C$4)))</f>
         <v>114.82569697259082</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
-      <c r="G7" s="21"/>
+      <c r="E7" s="7">
+        <f t="shared" si="1"/>
+        <v>0.04</v>
+      </c>
+      <c r="F7" s="22">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="G7" s="17">
+        <f t="shared" si="0"/>
+        <v>23.337201653678321</v>
+      </c>
       <c r="H7" s="21"/>
       <c r="I7" s="21"/>
     </row>
@@ -17122,9 +17180,18 @@
         <f>ATAN(($C$3+SQRT($C$3*$C$3-(4*(($C$5/(2*$C$6*$C$6))*$C$3*$C$3)*($C$4+(($C$5*$C$3*$C$3)/(2*$C$6*$C$6))))))/(2*(($C$5/(2*$C$6*$C$6))*$C$3*$C$3)))</f>
         <v>1.3253412479491977</v>
       </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
-      <c r="G8" s="21"/>
+      <c r="E8" s="7">
+        <f t="shared" si="1"/>
+        <v>0.05</v>
+      </c>
+      <c r="F8" s="22">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="G8" s="17">
+        <f t="shared" si="0"/>
+        <v>29.023882253898961</v>
+      </c>
       <c r="H8" s="21"/>
       <c r="I8" s="21"/>
     </row>
@@ -17136,9 +17203,18 @@
         <f>$C$8*(180/PI())</f>
         <v>75.936459922090606</v>
       </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
-      <c r="G9" s="21"/>
+      <c r="E9" s="7">
+        <f t="shared" si="1"/>
+        <v>6.0000000000000005E-2</v>
+      </c>
+      <c r="F9" s="22">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="G9" s="17">
+        <f t="shared" si="0"/>
+        <v>34.651514928840029</v>
+      </c>
       <c r="H9" s="21"/>
       <c r="I9" s="21"/>
     </row>
@@ -17150,9 +17226,18 @@
         <f>$C$3/($C$6*COS($C$8))</f>
         <v>27.435091916779431</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="21"/>
+      <c r="E10" s="7">
+        <f t="shared" si="1"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F10" s="22">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="G10" s="17">
+        <f t="shared" si="0"/>
+        <v>40.220099678501526</v>
+      </c>
       <c r="H10" s="21"/>
       <c r="I10" s="21"/>
     </row>
@@ -17164,23 +17249,41 @@
         <f>ATAN(($C$3-SQRT($C$3*$C$3-(4*(($C$5/(2*$C$6*$C$6))*$C$3*$C$3)*($C$4+(($C$5*$C$3*$C$3)/(2*$C$6*$C$6))))))/(2*(($C$5/(2*$C$6*$C$6))*$C$3*$C$3)))</f>
         <v>0.53691187332356594</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="21"/>
+      <c r="E11" s="7">
+        <f t="shared" si="1"/>
+        <v>0.08</v>
+      </c>
+      <c r="F11" s="22">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="G11" s="17">
+        <f t="shared" si="0"/>
+        <v>45.729636502883444</v>
+      </c>
       <c r="H11" s="21"/>
       <c r="I11" s="21"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="17">
         <f>$C$11*(180/PI())</f>
         <v>30.762784311903019</v>
       </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="21"/>
+      <c r="E12" s="7">
+        <f t="shared" si="1"/>
+        <v>0.09</v>
+      </c>
+      <c r="F12" s="22">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="G12" s="17">
+        <f t="shared" si="0"/>
+        <v>51.180125401985791</v>
+      </c>
       <c r="H12" s="21"/>
       <c r="I12" s="21"/>
     </row>
@@ -17192,36 +17295,87 @@
         <f>$C$3/($C$6*COS($C$11))</f>
         <v>7.7583223067140521</v>
       </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
-      <c r="G13" s="21"/>
+      <c r="E13" s="7">
+        <f t="shared" si="1"/>
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="F13" s="22">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="G13" s="17">
+        <f t="shared" si="0"/>
+        <v>56.571566375808558</v>
+      </c>
       <c r="H13" s="21"/>
       <c r="I13" s="21"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
-      <c r="G14" s="21"/>
+      <c r="B14" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="18">
+        <f>ATAN(($C$4+SQRT(($C$3*$C$3)+($C$4*$C$4)))/$C$3)</f>
+        <v>0.93112656063638188</v>
+      </c>
+      <c r="E14" s="7">
+        <f t="shared" si="1"/>
+        <v>0.10999999999999999</v>
+      </c>
+      <c r="F14" s="22">
+        <f t="shared" si="2"/>
+        <v>110</v>
+      </c>
+      <c r="G14" s="17">
+        <f t="shared" si="0"/>
+        <v>61.903959424351754</v>
+      </c>
       <c r="H14" s="21"/>
       <c r="I14" s="21"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="21"/>
+      <c r="B15" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="18">
+        <f>$C$14*(180/PI())</f>
+        <v>53.349622116996812</v>
+      </c>
+      <c r="E15" s="7">
+        <f t="shared" si="1"/>
+        <v>0.11999999999999998</v>
+      </c>
+      <c r="F15" s="22">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="G15" s="17">
+        <f t="shared" si="0"/>
+        <v>67.177304547615364</v>
+      </c>
       <c r="H15" s="21"/>
       <c r="I15" s="21"/>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
-      <c r="G16" s="21"/>
+      <c r="B16" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" s="18">
+        <f>$C$3/($C$6*COS($C$14))</f>
+        <v>11.168245441696904</v>
+      </c>
+      <c r="E16" s="7">
+        <f t="shared" si="1"/>
+        <v>0.12999999999999998</v>
+      </c>
+      <c r="F16" s="22">
+        <f t="shared" si="2"/>
+        <v>130</v>
+      </c>
+      <c r="G16" s="17">
+        <f t="shared" si="0"/>
+        <v>72.391601745599417</v>
+      </c>
       <c r="H16" s="21"/>
       <c r="I16" s="21"/>
     </row>
@@ -17254,8 +17408,8 @@
       <c r="I20" s="21"/>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C21" s="18"/>
-      <c r="D21" s="18"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
       <c r="E21" s="20"/>
       <c r="F21" s="20"/>
       <c r="G21" s="21"/>
@@ -17263,8 +17417,8 @@
       <c r="I21" s="21"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
       <c r="E22" s="20"/>
       <c r="F22" s="20"/>
       <c r="G22" s="21"/>
@@ -17272,8 +17426,8 @@
       <c r="I22" s="21"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
       <c r="E23" s="20"/>
       <c r="F23" s="20"/>
       <c r="G23" s="21"/>
@@ -17281,8 +17435,8 @@
       <c r="I23" s="21"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
       <c r="E24" s="20"/>
       <c r="F24" s="20"/>
       <c r="G24" s="21"/>
@@ -17290,8 +17444,8 @@
       <c r="I24" s="21"/>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
       <c r="E25" s="20"/>
       <c r="F25" s="20"/>
       <c r="G25" s="21"/>
@@ -17299,8 +17453,8 @@
       <c r="I25" s="21"/>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
       <c r="E26" s="20"/>
       <c r="F26" s="20"/>
       <c r="G26" s="21"/>
@@ -17308,8 +17462,8 @@
       <c r="I26" s="21"/>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C27" s="18"/>
-      <c r="D27" s="18"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
       <c r="E27" s="20"/>
       <c r="F27" s="20"/>
       <c r="G27" s="21"/>
@@ -17317,9 +17471,9 @@
       <c r="I27" s="21"/>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
       <c r="E28" s="20"/>
       <c r="F28" s="20"/>
       <c r="G28" s="21"/>
@@ -17327,8 +17481,8 @@
       <c r="I28" s="21"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
       <c r="E29" s="20"/>
       <c r="F29" s="20"/>
       <c r="G29" s="21"/>
@@ -17336,8 +17490,8 @@
       <c r="I29" s="21"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
       <c r="E30" s="20"/>
       <c r="F30" s="20"/>
       <c r="G30" s="21"/>
@@ -17345,9 +17499,9 @@
       <c r="I30" s="21"/>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B31" s="18"/>
-      <c r="C31" s="18"/>
-      <c r="D31" s="18"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
       <c r="E31" s="20"/>
       <c r="F31" s="20"/>
       <c r="G31" s="21"/>
@@ -17355,8 +17509,8 @@
       <c r="I31" s="21"/>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C32" s="18"/>
-      <c r="D32" s="18"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
       <c r="E32" s="20"/>
       <c r="F32" s="20"/>
       <c r="G32" s="21"/>
@@ -17364,8 +17518,8 @@
       <c r="I32" s="21"/>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C33" s="18"/>
-      <c r="D33" s="18"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
       <c r="E33" s="20"/>
       <c r="F33" s="20"/>
       <c r="G33" s="21"/>
@@ -17373,9 +17527,9 @@
       <c r="I33" s="21"/>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B34" s="18"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
       <c r="E34" s="20"/>
       <c r="F34" s="20"/>
       <c r="G34" s="21"/>
@@ -17383,8 +17537,8 @@
       <c r="I34" s="21"/>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
       <c r="E35" s="20"/>
       <c r="F35" s="20"/>
       <c r="G35" s="21"/>
@@ -17392,8 +17546,8 @@
       <c r="I35" s="21"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C36" s="18"/>
-      <c r="D36" s="18"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
       <c r="E36" s="20"/>
       <c r="F36" s="20"/>
       <c r="G36" s="21"/>

</xml_diff>

<commit_message>
finished setting up columns for model
</commit_message>
<xml_diff>
--- a/models.xlsx
+++ b/models.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssb\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF512D7-D07A-4D50-8390-A16B5F2B6ED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A96BB06-EEF3-42F6-BB9B-D6620C6153A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{6422CA17-FA72-4B85-908A-20157EF2E374}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <r>
       <t>launch angle/</t>
@@ -294,6 +294,12 @@
   <si>
     <t xml:space="preserve">Time of flight/s </t>
   </si>
+  <si>
+    <t xml:space="preserve">y high ball </t>
+  </si>
+  <si>
+    <t xml:space="preserve">y min u </t>
+  </si>
 </sst>
 </file>
 
@@ -479,7 +485,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -499,10 +505,8 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -17035,10 +17039,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEC10B89-8002-4438-80A5-6E69B9FCD18F}">
-  <dimension ref="B2:I115"/>
+  <dimension ref="B2:I103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17054,14 +17058,18 @@
       <c r="E2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="7" t="s">
         <v>12</v>
       </c>
       <c r="G2" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
+      <c r="H2" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B3" s="12" t="s">
@@ -17073,15 +17081,21 @@
       <c r="E3" s="7">
         <v>0</v>
       </c>
-      <c r="F3" s="22">
+      <c r="F3" s="7">
         <v>0</v>
       </c>
       <c r="G3" s="17">
-        <f t="shared" ref="G3:G16" si="0">F3*TAN($C$11)-($C$5/(2*$C$6*$C$6))*(1+(TAN($C$11)*TAN($C$11)))*F3*F3</f>
+        <f t="shared" ref="G3:G66" si="0">F3*TAN($C$11)-($C$5/(2*$C$6*$C$6))*(1+(TAN($C$11)*TAN($C$11)))*F3*F3</f>
         <v>0</v>
       </c>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
+      <c r="H3" s="15">
+        <f t="shared" ref="H3:H66" si="1">F3*TAN($C$8)-($C$5/(2*$C$6*$C$6))*(1+(TAN($C$8)*TAN($C$8)))*F3*F3</f>
+        <v>0</v>
+      </c>
+      <c r="I3" s="18">
+        <f t="shared" ref="I3:I66" si="2">F3*(($C$4+SQRT(($C$3*$C$3)+($C$4*$C$4)))/$C$3)-(SQRT(($C$3*$C$3)+($C$4*$C$4))/($C$3*$C$3))*(F3*F3)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="12" t="s">
@@ -17094,7 +17108,7 @@
         <f>E3+0.01</f>
         <v>0.01</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="7">
         <f>F3+10</f>
         <v>10</v>
       </c>
@@ -17102,8 +17116,14 @@
         <f t="shared" si="0"/>
         <v>5.9228723013389413</v>
       </c>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
+      <c r="H4" s="15">
+        <f t="shared" si="1"/>
+        <v>39.549971735358291</v>
+      </c>
+      <c r="I4" s="18">
+        <f t="shared" si="2"/>
+        <v>13.335903443821445</v>
+      </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
@@ -17113,19 +17133,25 @@
         <v>9.81</v>
       </c>
       <c r="E5" s="7">
-        <f t="shared" ref="E5:E68" si="1">E4+0.01</f>
+        <f t="shared" ref="E5:E68" si="3">E4+0.01</f>
         <v>0.02</v>
       </c>
-      <c r="F5" s="22">
-        <f t="shared" ref="F5:F68" si="2">F4+10</f>
+      <c r="F5" s="7">
+        <f t="shared" ref="F5:F68" si="4">F4+10</f>
         <v>20</v>
       </c>
       <c r="G5" s="17">
         <f t="shared" si="0"/>
         <v>11.786696677398309</v>
       </c>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
+      <c r="H5" s="15">
+        <f t="shared" si="1"/>
+        <v>78.361560203335614</v>
+      </c>
+      <c r="I5" s="18">
+        <f t="shared" si="2"/>
+        <v>26.46300075746468</v>
+      </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
@@ -17135,19 +17161,25 @@
         <v>150</v>
       </c>
       <c r="E6" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.03</v>
       </c>
-      <c r="F6" s="22">
-        <f t="shared" si="2"/>
+      <c r="F6" s="7">
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="G6" s="17">
         <f t="shared" si="0"/>
         <v>17.591473128178098</v>
       </c>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
+      <c r="H6" s="15">
+        <f t="shared" si="1"/>
+        <v>116.43476540393195</v>
+      </c>
+      <c r="I6" s="18">
+        <f t="shared" si="2"/>
+        <v>39.3812919409297</v>
+      </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="13" t="s">
@@ -17158,19 +17190,25 @@
         <v>114.82569697259082</v>
       </c>
       <c r="E7" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.04</v>
       </c>
-      <c r="F7" s="22">
-        <f t="shared" si="2"/>
+      <c r="F7" s="7">
+        <f t="shared" si="4"/>
         <v>40</v>
       </c>
       <c r="G7" s="17">
         <f t="shared" si="0"/>
         <v>23.337201653678321</v>
       </c>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
+      <c r="H7" s="15">
+        <f t="shared" si="1"/>
+        <v>153.76958733714733</v>
+      </c>
+      <c r="I7" s="18">
+        <f t="shared" si="2"/>
+        <v>52.090776994216512</v>
+      </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
@@ -17181,19 +17219,25 @@
         <v>1.3253412479491977</v>
       </c>
       <c r="E8" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.05</v>
       </c>
-      <c r="F8" s="22">
-        <f t="shared" si="2"/>
+      <c r="F8" s="7">
+        <f t="shared" si="4"/>
         <v>50</v>
       </c>
       <c r="G8" s="17">
         <f t="shared" si="0"/>
         <v>29.023882253898961</v>
       </c>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
+      <c r="H8" s="15">
+        <f t="shared" si="1"/>
+        <v>190.3660260029817</v>
+      </c>
+      <c r="I8" s="18">
+        <f t="shared" si="2"/>
+        <v>64.591455917325121</v>
+      </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="15" t="s">
@@ -17204,19 +17248,25 @@
         <v>75.936459922090606</v>
       </c>
       <c r="E9" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>6.0000000000000005E-2</v>
       </c>
-      <c r="F9" s="22">
-        <f t="shared" si="2"/>
+      <c r="F9" s="7">
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="G9" s="17">
         <f t="shared" si="0"/>
         <v>34.651514928840029</v>
       </c>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
+      <c r="H9" s="15">
+        <f t="shared" si="1"/>
+        <v>226.22408140143511</v>
+      </c>
+      <c r="I9" s="18">
+        <f t="shared" si="2"/>
+        <v>76.883328710255498</v>
+      </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B10" s="15" t="s">
@@ -17227,19 +17277,25 @@
         <v>27.435091916779431</v>
       </c>
       <c r="E10" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F10" s="22">
-        <f t="shared" si="2"/>
+      <c r="F10" s="7">
+        <f t="shared" si="4"/>
         <v>70</v>
       </c>
       <c r="G10" s="17">
         <f t="shared" si="0"/>
         <v>40.220099678501526</v>
       </c>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
+      <c r="H10" s="15">
+        <f t="shared" si="1"/>
+        <v>261.34375353250755</v>
+      </c>
+      <c r="I10" s="18">
+        <f t="shared" si="2"/>
+        <v>88.966395373007686</v>
+      </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="16" t="s">
@@ -17250,19 +17306,25 @@
         <v>0.53691187332356594</v>
       </c>
       <c r="E11" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.08</v>
       </c>
-      <c r="F11" s="22">
-        <f t="shared" si="2"/>
+      <c r="F11" s="7">
+        <f t="shared" si="4"/>
         <v>80</v>
       </c>
       <c r="G11" s="17">
         <f t="shared" si="0"/>
         <v>45.729636502883444</v>
       </c>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
+      <c r="H11" s="15">
+        <f t="shared" si="1"/>
+        <v>295.72504239619906</v>
+      </c>
+      <c r="I11" s="18">
+        <f t="shared" si="2"/>
+        <v>100.84065590558166</v>
+      </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" s="17" t="s">
@@ -17273,19 +17335,25 @@
         <v>30.762784311903019</v>
       </c>
       <c r="E12" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.09</v>
       </c>
-      <c r="F12" s="22">
-        <f t="shared" si="2"/>
+      <c r="F12" s="7">
+        <f t="shared" si="4"/>
         <v>90</v>
       </c>
       <c r="G12" s="17">
         <f t="shared" si="0"/>
         <v>51.180125401985791</v>
       </c>
-      <c r="H12" s="21"/>
-      <c r="I12" s="21"/>
+      <c r="H12" s="15">
+        <f t="shared" si="1"/>
+        <v>329.36794799250953</v>
+      </c>
+      <c r="I12" s="18">
+        <f t="shared" si="2"/>
+        <v>112.50611030797741</v>
+      </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="17" t="s">
@@ -17296,19 +17364,25 @@
         <v>7.7583223067140521</v>
       </c>
       <c r="E13" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>9.9999999999999992E-2</v>
       </c>
-      <c r="F13" s="22">
-        <f t="shared" si="2"/>
+      <c r="F13" s="7">
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
       <c r="G13" s="17">
         <f t="shared" si="0"/>
         <v>56.571566375808558</v>
       </c>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
+      <c r="H13" s="15">
+        <f t="shared" si="1"/>
+        <v>362.27247032143902</v>
+      </c>
+      <c r="I13" s="18">
+        <f t="shared" si="2"/>
+        <v>123.96275858019497</v>
+      </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" s="18" t="s">
@@ -17319,19 +17393,25 @@
         <v>0.93112656063638188</v>
       </c>
       <c r="E14" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.10999999999999999</v>
       </c>
-      <c r="F14" s="22">
-        <f t="shared" si="2"/>
+      <c r="F14" s="7">
+        <f t="shared" si="4"/>
         <v>110</v>
       </c>
       <c r="G14" s="17">
         <f t="shared" si="0"/>
         <v>61.903959424351754</v>
       </c>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
+      <c r="H14" s="15">
+        <f t="shared" si="1"/>
+        <v>394.43860938298758</v>
+      </c>
+      <c r="I14" s="18">
+        <f t="shared" si="2"/>
+        <v>135.21060072223429</v>
+      </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" s="18" t="s">
@@ -17342,19 +17422,25 @@
         <v>53.349622116996812</v>
       </c>
       <c r="E15" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.11999999999999998</v>
       </c>
-      <c r="F15" s="22">
-        <f t="shared" si="2"/>
+      <c r="F15" s="7">
+        <f t="shared" si="4"/>
         <v>120</v>
       </c>
       <c r="G15" s="17">
         <f t="shared" si="0"/>
         <v>67.177304547615364</v>
       </c>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
+      <c r="H15" s="15">
+        <f t="shared" si="1"/>
+        <v>425.8663651771551</v>
+      </c>
+      <c r="I15" s="18">
+        <f t="shared" si="2"/>
+        <v>146.24963673409542</v>
+      </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="18" t="s">
@@ -17365,747 +17451,1974 @@
         <v>11.168245441696904</v>
       </c>
       <c r="E16" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0.12999999999999998</v>
       </c>
-      <c r="F16" s="22">
-        <f t="shared" si="2"/>
+      <c r="F16" s="7">
+        <f t="shared" si="4"/>
         <v>130</v>
       </c>
       <c r="G16" s="17">
         <f t="shared" si="0"/>
         <v>72.391601745599417</v>
       </c>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
+      <c r="H16" s="15">
+        <f t="shared" si="1"/>
+        <v>456.5557377039417</v>
+      </c>
+      <c r="I16" s="18">
+        <f t="shared" si="2"/>
+        <v>157.07986661577834</v>
+      </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
+      <c r="E17" s="7">
+        <f t="shared" si="3"/>
+        <v>0.13999999999999999</v>
+      </c>
+      <c r="F17" s="7">
+        <f t="shared" si="4"/>
+        <v>140</v>
+      </c>
+      <c r="G17" s="17">
+        <f>F17*TAN($C$11)-($C$5/(2*$C$6*$C$6))*(1+(TAN($C$11)*TAN($C$11)))*F17*F17</f>
+        <v>77.546851018303897</v>
+      </c>
+      <c r="H17" s="15">
+        <f t="shared" si="1"/>
+        <v>486.50672696334726</v>
+      </c>
+      <c r="I17" s="18">
+        <f t="shared" si="2"/>
+        <v>167.70129036728304</v>
+      </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
+      <c r="E18" s="7">
+        <f t="shared" si="3"/>
+        <v>0.15</v>
+      </c>
+      <c r="F18" s="7">
+        <f t="shared" si="4"/>
+        <v>150</v>
+      </c>
+      <c r="G18" s="17">
+        <f t="shared" si="0"/>
+        <v>82.643052365728792</v>
+      </c>
+      <c r="H18" s="15">
+        <f t="shared" si="1"/>
+        <v>515.71933295537201</v>
+      </c>
+      <c r="I18" s="18">
+        <f t="shared" si="2"/>
+        <v>178.11390798860953</v>
+      </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
+      <c r="E19" s="7">
+        <f t="shared" si="3"/>
+        <v>0.16</v>
+      </c>
+      <c r="F19" s="7">
+        <f t="shared" si="4"/>
+        <v>160</v>
+      </c>
+      <c r="G19" s="17">
+        <f t="shared" si="0"/>
+        <v>87.680205787874115</v>
+      </c>
+      <c r="H19" s="15">
+        <f t="shared" si="1"/>
+        <v>544.19355568001561</v>
+      </c>
+      <c r="I19" s="18">
+        <f t="shared" si="2"/>
+        <v>188.31771947975781</v>
+      </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
+      <c r="E20" s="7">
+        <f t="shared" si="3"/>
+        <v>0.17</v>
+      </c>
+      <c r="F20" s="7">
+        <f t="shared" si="4"/>
+        <v>170</v>
+      </c>
+      <c r="G20" s="17">
+        <f t="shared" si="0"/>
+        <v>92.658311284739867</v>
+      </c>
+      <c r="H20" s="15">
+        <f t="shared" si="1"/>
+        <v>571.92939513727833</v>
+      </c>
+      <c r="I20" s="18">
+        <f t="shared" si="2"/>
+        <v>198.3127248407279</v>
+      </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="7">
+        <f t="shared" si="3"/>
+        <v>0.18000000000000002</v>
+      </c>
+      <c r="F21" s="7">
+        <f t="shared" si="4"/>
+        <v>180</v>
+      </c>
+      <c r="G21" s="17">
+        <f t="shared" si="0"/>
+        <v>97.577368856326032</v>
+      </c>
+      <c r="H21" s="15">
+        <f t="shared" si="1"/>
+        <v>598.92685132715997</v>
+      </c>
+      <c r="I21" s="18">
+        <f t="shared" si="2"/>
+        <v>208.09892407151972</v>
+      </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C22" s="19"/>
-      <c r="D22" s="19"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
-      <c r="I22" s="21"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="7">
+        <f t="shared" si="3"/>
+        <v>0.19000000000000003</v>
+      </c>
+      <c r="F22" s="7">
+        <f t="shared" si="4"/>
+        <v>190</v>
+      </c>
+      <c r="G22" s="17">
+        <f t="shared" si="0"/>
+        <v>102.43737850263264</v>
+      </c>
+      <c r="H22" s="15">
+        <f t="shared" si="1"/>
+        <v>625.18592424966073</v>
+      </c>
+      <c r="I22" s="18">
+        <f t="shared" si="2"/>
+        <v>217.67631717213339</v>
+      </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C23" s="19"/>
-      <c r="D23" s="19"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="21"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="7">
+        <f t="shared" si="3"/>
+        <v>0.20000000000000004</v>
+      </c>
+      <c r="F23" s="7">
+        <f t="shared" si="4"/>
+        <v>200</v>
+      </c>
+      <c r="G23" s="17">
+        <f t="shared" si="0"/>
+        <v>107.23834022365966</v>
+      </c>
+      <c r="H23" s="15">
+        <f t="shared" si="1"/>
+        <v>650.7066139047804</v>
+      </c>
+      <c r="I23" s="18">
+        <f t="shared" si="2"/>
+        <v>227.04490414256884</v>
+      </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="21"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="7">
+        <f t="shared" si="3"/>
+        <v>0.21000000000000005</v>
+      </c>
+      <c r="F24" s="7">
+        <f t="shared" si="4"/>
+        <v>210</v>
+      </c>
+      <c r="G24" s="17">
+        <f t="shared" si="0"/>
+        <v>111.9802540194071</v>
+      </c>
+      <c r="H24" s="15">
+        <f t="shared" si="1"/>
+        <v>675.48892029251931</v>
+      </c>
+      <c r="I24" s="18">
+        <f t="shared" si="2"/>
+        <v>236.20468498282602</v>
+      </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="7">
+        <f t="shared" si="3"/>
+        <v>0.22000000000000006</v>
+      </c>
+      <c r="F25" s="7">
+        <f t="shared" si="4"/>
+        <v>220</v>
+      </c>
+      <c r="G25" s="17">
+        <f t="shared" si="0"/>
+        <v>116.66311988987498</v>
+      </c>
+      <c r="H25" s="15">
+        <f t="shared" si="1"/>
+        <v>699.53284341287713</v>
+      </c>
+      <c r="I25" s="18">
+        <f t="shared" si="2"/>
+        <v>245.15565969290506</v>
+      </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="21"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="7">
+        <f>E25+0.01</f>
+        <v>0.23000000000000007</v>
+      </c>
+      <c r="F26" s="7">
+        <f t="shared" si="4"/>
+        <v>230</v>
+      </c>
+      <c r="G26" s="17">
+        <f t="shared" si="0"/>
+        <v>121.28693783506327</v>
+      </c>
+      <c r="H26" s="15">
+        <f t="shared" si="1"/>
+        <v>722.83838326585396</v>
+      </c>
+      <c r="I26" s="18">
+        <f t="shared" si="2"/>
+        <v>253.8978282728059</v>
+      </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="21"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="7">
+        <f t="shared" si="3"/>
+        <v>0.24000000000000007</v>
+      </c>
+      <c r="F27" s="7">
+        <f t="shared" si="4"/>
+        <v>240</v>
+      </c>
+      <c r="G27" s="17">
+        <f t="shared" si="0"/>
+        <v>125.85170785497201</v>
+      </c>
+      <c r="H27" s="15">
+        <f t="shared" si="1"/>
+        <v>745.4055398514497</v>
+      </c>
+      <c r="I27" s="18">
+        <f t="shared" si="2"/>
+        <v>262.43119072252841</v>
+      </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="21"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="7">
+        <f t="shared" si="3"/>
+        <v>0.25000000000000006</v>
+      </c>
+      <c r="F28" s="7">
+        <f t="shared" si="4"/>
+        <v>250</v>
+      </c>
+      <c r="G28" s="17">
+        <f t="shared" si="0"/>
+        <v>130.35742994960114</v>
+      </c>
+      <c r="H28" s="15">
+        <f t="shared" si="1"/>
+        <v>767.23431316966457</v>
+      </c>
+      <c r="I28" s="18">
+        <f t="shared" si="2"/>
+        <v>270.75574704207281</v>
+      </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="21"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="7">
+        <f t="shared" si="3"/>
+        <v>0.26000000000000006</v>
+      </c>
+      <c r="F29" s="7">
+        <f t="shared" si="4"/>
+        <v>260</v>
+      </c>
+      <c r="G29" s="17">
+        <f t="shared" si="0"/>
+        <v>134.80410411895073</v>
+      </c>
+      <c r="H29" s="15">
+        <f t="shared" si="1"/>
+        <v>788.32470322049846</v>
+      </c>
+      <c r="I29" s="18">
+        <f t="shared" si="2"/>
+        <v>278.87149723143898</v>
+      </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="21"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="7">
+        <f t="shared" si="3"/>
+        <v>0.27000000000000007</v>
+      </c>
+      <c r="F30" s="7">
+        <f t="shared" si="4"/>
+        <v>270</v>
+      </c>
+      <c r="G30" s="17">
+        <f t="shared" si="0"/>
+        <v>139.19173036302072</v>
+      </c>
+      <c r="H30" s="15">
+        <f t="shared" si="1"/>
+        <v>808.67671000395148</v>
+      </c>
+      <c r="I30" s="18">
+        <f t="shared" si="2"/>
+        <v>286.77844129062697</v>
+      </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B31" s="19"/>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
-      <c r="G31" s="21"/>
-      <c r="H31" s="21"/>
-      <c r="I31" s="21"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="7">
+        <f t="shared" si="3"/>
+        <v>0.28000000000000008</v>
+      </c>
+      <c r="F31" s="7">
+        <f t="shared" si="4"/>
+        <v>280</v>
+      </c>
+      <c r="G31" s="17">
+        <f t="shared" si="0"/>
+        <v>143.52030868181117</v>
+      </c>
+      <c r="H31" s="15">
+        <f t="shared" si="1"/>
+        <v>828.2903335200233</v>
+      </c>
+      <c r="I31" s="18">
+        <f t="shared" si="2"/>
+        <v>294.47657921963668</v>
+      </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
-      <c r="G32" s="21"/>
-      <c r="H32" s="21"/>
-      <c r="I32" s="21"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="7">
+        <f t="shared" si="3"/>
+        <v>0.29000000000000009</v>
+      </c>
+      <c r="F32" s="7">
+        <f t="shared" si="4"/>
+        <v>290</v>
+      </c>
+      <c r="G32" s="17">
+        <f t="shared" si="0"/>
+        <v>147.78983907532202</v>
+      </c>
+      <c r="H32" s="15">
+        <f t="shared" si="1"/>
+        <v>847.16557376871447</v>
+      </c>
+      <c r="I32" s="18">
+        <f t="shared" si="2"/>
+        <v>301.96591101846826</v>
+      </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
-      <c r="G33" s="21"/>
-      <c r="H33" s="21"/>
-      <c r="I33" s="21"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="7">
+        <f t="shared" si="3"/>
+        <v>0.3000000000000001</v>
+      </c>
+      <c r="F33" s="7">
+        <f t="shared" si="4"/>
+        <v>300</v>
+      </c>
+      <c r="G33" s="17">
+        <f t="shared" si="0"/>
+        <v>152.0003215435533</v>
+      </c>
+      <c r="H33" s="15">
+        <f t="shared" si="1"/>
+        <v>865.30243075002454</v>
+      </c>
+      <c r="I33" s="18">
+        <f t="shared" si="2"/>
+        <v>309.24643668712156</v>
+      </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B34" s="19"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="21"/>
-      <c r="H34" s="21"/>
-      <c r="I34" s="21"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="7">
+        <f t="shared" si="3"/>
+        <v>0.31000000000000011</v>
+      </c>
+      <c r="F34" s="7">
+        <f t="shared" si="4"/>
+        <v>310</v>
+      </c>
+      <c r="G34" s="17">
+        <f t="shared" si="0"/>
+        <v>156.151756086505</v>
+      </c>
+      <c r="H34" s="15">
+        <f t="shared" si="1"/>
+        <v>882.70090446395329</v>
+      </c>
+      <c r="I34" s="18">
+        <f t="shared" si="2"/>
+        <v>316.31815622559674</v>
+      </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="7">
+        <f>E34+0.01</f>
+        <v>0.32000000000000012</v>
+      </c>
+      <c r="F35" s="7">
+        <f t="shared" si="4"/>
+        <v>320</v>
+      </c>
+      <c r="G35" s="17">
+        <f t="shared" si="0"/>
+        <v>160.24414270417714</v>
+      </c>
+      <c r="H35" s="15">
+        <f t="shared" si="1"/>
+        <v>899.36099491050163</v>
+      </c>
+      <c r="I35" s="18">
+        <f t="shared" si="2"/>
+        <v>323.18106963389357</v>
+      </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="21"/>
-      <c r="H36" s="21"/>
-      <c r="I36" s="21"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="7">
+        <f t="shared" si="3"/>
+        <v>0.33000000000000013</v>
+      </c>
+      <c r="F36" s="7">
+        <f t="shared" si="4"/>
+        <v>330</v>
+      </c>
+      <c r="G36" s="17">
+        <f t="shared" si="0"/>
+        <v>164.2774813965697</v>
+      </c>
+      <c r="H36" s="15">
+        <f t="shared" si="1"/>
+        <v>915.28270208966842</v>
+      </c>
+      <c r="I36" s="18">
+        <f t="shared" si="2"/>
+        <v>329.83517691201229</v>
+      </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="21"/>
-      <c r="H37" s="21"/>
-      <c r="I37" s="21"/>
+      <c r="E37" s="7">
+        <f t="shared" si="3"/>
+        <v>0.34000000000000014</v>
+      </c>
+      <c r="F37" s="7">
+        <f t="shared" si="4"/>
+        <v>340</v>
+      </c>
+      <c r="G37" s="17">
+        <f t="shared" si="0"/>
+        <v>168.25177216368269</v>
+      </c>
+      <c r="H37" s="15">
+        <f t="shared" si="1"/>
+        <v>930.46602600145468</v>
+      </c>
+      <c r="I37" s="18">
+        <f t="shared" si="2"/>
+        <v>336.28047805995277</v>
+      </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
-      <c r="G38" s="21"/>
-      <c r="H38" s="21"/>
-      <c r="I38" s="21"/>
+      <c r="E38" s="7">
+        <f t="shared" si="3"/>
+        <v>0.35000000000000014</v>
+      </c>
+      <c r="F38" s="7">
+        <f t="shared" si="4"/>
+        <v>350</v>
+      </c>
+      <c r="G38" s="17">
+        <f t="shared" si="0"/>
+        <v>172.16701500551608</v>
+      </c>
+      <c r="H38" s="15">
+        <f t="shared" si="1"/>
+        <v>944.91096664585984</v>
+      </c>
+      <c r="I38" s="18">
+        <f t="shared" si="2"/>
+        <v>342.51697307771502</v>
+      </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="21"/>
-      <c r="H39" s="21"/>
-      <c r="I39" s="21"/>
+      <c r="E39" s="7">
+        <f t="shared" si="3"/>
+        <v>0.36000000000000015</v>
+      </c>
+      <c r="F39" s="7">
+        <f t="shared" si="4"/>
+        <v>360</v>
+      </c>
+      <c r="G39" s="17">
+        <f t="shared" si="0"/>
+        <v>176.0232099220699</v>
+      </c>
+      <c r="H39" s="15">
+        <f t="shared" si="1"/>
+        <v>958.61752402288403</v>
+      </c>
+      <c r="I39" s="18">
+        <f t="shared" si="2"/>
+        <v>348.5446619652991</v>
+      </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="21"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="21"/>
+      <c r="E40" s="7">
+        <f t="shared" si="3"/>
+        <v>0.37000000000000016</v>
+      </c>
+      <c r="F40" s="7">
+        <f t="shared" si="4"/>
+        <v>370</v>
+      </c>
+      <c r="G40" s="17">
+        <f t="shared" si="0"/>
+        <v>179.82035691334414</v>
+      </c>
+      <c r="H40" s="15">
+        <f t="shared" si="1"/>
+        <v>971.58569813252711</v>
+      </c>
+      <c r="I40" s="18">
+        <f t="shared" si="2"/>
+        <v>354.363544722705</v>
+      </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="21"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="21"/>
+      <c r="E41" s="7">
+        <f t="shared" si="3"/>
+        <v>0.38000000000000017</v>
+      </c>
+      <c r="F41" s="7">
+        <f t="shared" si="4"/>
+        <v>380</v>
+      </c>
+      <c r="G41" s="17">
+        <f t="shared" si="0"/>
+        <v>183.55845597933885</v>
+      </c>
+      <c r="H41" s="15">
+        <f t="shared" si="1"/>
+        <v>983.81548897478933</v>
+      </c>
+      <c r="I41" s="18">
+        <f t="shared" si="2"/>
+        <v>359.97362134993261</v>
+      </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="21"/>
-      <c r="H42" s="21"/>
-      <c r="I42" s="21"/>
+      <c r="E42" s="7">
+        <f t="shared" si="3"/>
+        <v>0.39000000000000018</v>
+      </c>
+      <c r="F42" s="7">
+        <f t="shared" si="4"/>
+        <v>390</v>
+      </c>
+      <c r="G42" s="17">
+        <f t="shared" si="0"/>
+        <v>187.23750712005395</v>
+      </c>
+      <c r="H42" s="15">
+        <f t="shared" si="1"/>
+        <v>995.30689654967057</v>
+      </c>
+      <c r="I42" s="18">
+        <f t="shared" si="2"/>
+        <v>365.37489184698205</v>
+      </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="21"/>
-      <c r="H43" s="21"/>
-      <c r="I43" s="21"/>
+      <c r="E43" s="7">
+        <f t="shared" si="3"/>
+        <v>0.40000000000000019</v>
+      </c>
+      <c r="F43" s="7">
+        <f t="shared" si="4"/>
+        <v>400</v>
+      </c>
+      <c r="G43" s="17">
+        <f t="shared" si="0"/>
+        <v>190.85751033548948</v>
+      </c>
+      <c r="H43" s="15">
+        <f t="shared" si="1"/>
+        <v>1006.0599208571707</v>
+      </c>
+      <c r="I43" s="18">
+        <f t="shared" si="2"/>
+        <v>370.56735621385326</v>
+      </c>
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="21"/>
-      <c r="H44" s="21"/>
-      <c r="I44" s="21"/>
+      <c r="E44" s="7">
+        <f t="shared" si="3"/>
+        <v>0.4100000000000002</v>
+      </c>
+      <c r="F44" s="7">
+        <f t="shared" si="4"/>
+        <v>410</v>
+      </c>
+      <c r="G44" s="17">
+        <f t="shared" si="0"/>
+        <v>194.41846562564544</v>
+      </c>
+      <c r="H44" s="15">
+        <f t="shared" si="1"/>
+        <v>1016.0745618972901</v>
+      </c>
+      <c r="I44" s="18">
+        <f t="shared" si="2"/>
+        <v>375.55101445054618</v>
+      </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="21"/>
-      <c r="H45" s="21"/>
-      <c r="I45" s="21"/>
+      <c r="E45" s="7">
+        <f t="shared" si="3"/>
+        <v>0.42000000000000021</v>
+      </c>
+      <c r="F45" s="7">
+        <f t="shared" si="4"/>
+        <v>420</v>
+      </c>
+      <c r="G45" s="17">
+        <f t="shared" si="0"/>
+        <v>197.9203729905218</v>
+      </c>
+      <c r="H45" s="15">
+        <f t="shared" si="1"/>
+        <v>1025.3508196700286</v>
+      </c>
+      <c r="I45" s="18">
+        <f t="shared" si="2"/>
+        <v>380.32586655706098</v>
+      </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="21"/>
-      <c r="H46" s="21"/>
-      <c r="I46" s="21"/>
+      <c r="E46" s="7">
+        <f t="shared" si="3"/>
+        <v>0.43000000000000022</v>
+      </c>
+      <c r="F46" s="7">
+        <f t="shared" si="4"/>
+        <v>430</v>
+      </c>
+      <c r="G46" s="17">
+        <f t="shared" si="0"/>
+        <v>201.36323243011861</v>
+      </c>
+      <c r="H46" s="15">
+        <f t="shared" si="1"/>
+        <v>1033.8886941753856</v>
+      </c>
+      <c r="I46" s="18">
+        <f t="shared" si="2"/>
+        <v>384.8919125333976</v>
+      </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="21"/>
+      <c r="E47" s="7">
+        <f t="shared" si="3"/>
+        <v>0.44000000000000022</v>
+      </c>
+      <c r="F47" s="7">
+        <f t="shared" si="4"/>
+        <v>440</v>
+      </c>
+      <c r="G47" s="17">
+        <f t="shared" si="0"/>
+        <v>204.74704394443586</v>
+      </c>
+      <c r="H47" s="15">
+        <f t="shared" si="1"/>
+        <v>1041.6881854133621</v>
+      </c>
+      <c r="I47" s="18">
+        <f t="shared" si="2"/>
+        <v>389.24915237955599</v>
+      </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E48" s="20"/>
-      <c r="F48" s="20"/>
-      <c r="G48" s="21"/>
-      <c r="H48" s="21"/>
-      <c r="I48" s="21"/>
+      <c r="E48" s="7">
+        <f t="shared" si="3"/>
+        <v>0.45000000000000023</v>
+      </c>
+      <c r="F48" s="7">
+        <f t="shared" si="4"/>
+        <v>450</v>
+      </c>
+      <c r="G48" s="17">
+        <f t="shared" si="0"/>
+        <v>208.07180753347353</v>
+      </c>
+      <c r="H48" s="15">
+        <f t="shared" si="1"/>
+        <v>1048.7492933839574</v>
+      </c>
+      <c r="I48" s="18">
+        <f t="shared" si="2"/>
+        <v>393.39758609553616</v>
+      </c>
     </row>
     <row r="49" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="21"/>
-      <c r="I49" s="21"/>
+      <c r="E49" s="7">
+        <f t="shared" si="3"/>
+        <v>0.46000000000000024</v>
+      </c>
+      <c r="F49" s="7">
+        <f t="shared" si="4"/>
+        <v>460</v>
+      </c>
+      <c r="G49" s="17">
+        <f t="shared" si="0"/>
+        <v>211.3375231972316</v>
+      </c>
+      <c r="H49" s="15">
+        <f t="shared" si="1"/>
+        <v>1055.0720180871717</v>
+      </c>
+      <c r="I49" s="18">
+        <f t="shared" si="2"/>
+        <v>397.33721368133814</v>
+      </c>
     </row>
     <row r="50" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="21"/>
-      <c r="H50" s="21"/>
-      <c r="I50" s="21"/>
+      <c r="E50" s="7">
+        <f t="shared" si="3"/>
+        <v>0.47000000000000025</v>
+      </c>
+      <c r="F50" s="7">
+        <f t="shared" si="4"/>
+        <v>470</v>
+      </c>
+      <c r="G50" s="17">
+        <f t="shared" si="0"/>
+        <v>214.54419093571013</v>
+      </c>
+      <c r="H50" s="15">
+        <f t="shared" si="1"/>
+        <v>1060.6563595230054</v>
+      </c>
+      <c r="I50" s="18">
+        <f t="shared" si="2"/>
+        <v>401.0680351369619</v>
+      </c>
     </row>
     <row r="51" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="21"/>
-      <c r="H51" s="21"/>
-      <c r="I51" s="21"/>
+      <c r="E51" s="7">
+        <f t="shared" si="3"/>
+        <v>0.48000000000000026</v>
+      </c>
+      <c r="F51" s="7">
+        <f t="shared" si="4"/>
+        <v>480</v>
+      </c>
+      <c r="G51" s="17">
+        <f t="shared" si="0"/>
+        <v>217.69181074890906</v>
+      </c>
+      <c r="H51" s="15">
+        <f t="shared" si="1"/>
+        <v>1065.5023176914576</v>
+      </c>
+      <c r="I51" s="18">
+        <f t="shared" si="2"/>
+        <v>404.59005046240731</v>
+      </c>
     </row>
     <row r="52" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
-      <c r="G52" s="21"/>
-      <c r="H52" s="21"/>
-      <c r="I52" s="21"/>
+      <c r="E52" s="7">
+        <f t="shared" si="3"/>
+        <v>0.49000000000000027</v>
+      </c>
+      <c r="F52" s="7">
+        <f t="shared" si="4"/>
+        <v>490</v>
+      </c>
+      <c r="G52" s="17">
+        <f t="shared" si="0"/>
+        <v>220.78038263682845</v>
+      </c>
+      <c r="H52" s="15">
+        <f t="shared" si="1"/>
+        <v>1069.6098925925291</v>
+      </c>
+      <c r="I52" s="18">
+        <f t="shared" si="2"/>
+        <v>407.90325965767465</v>
+      </c>
     </row>
     <row r="53" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
-      <c r="G53" s="21"/>
-      <c r="H53" s="21"/>
-      <c r="I53" s="21"/>
+      <c r="E53" s="7">
+        <f t="shared" si="3"/>
+        <v>0.50000000000000022</v>
+      </c>
+      <c r="F53" s="7">
+        <f t="shared" si="4"/>
+        <v>500</v>
+      </c>
+      <c r="G53" s="17">
+        <f t="shared" si="0"/>
+        <v>223.80990659946821</v>
+      </c>
+      <c r="H53" s="15">
+        <f t="shared" si="1"/>
+        <v>1072.9790842262196</v>
+      </c>
+      <c r="I53" s="18">
+        <f t="shared" si="2"/>
+        <v>411.00766272276377</v>
+      </c>
     </row>
     <row r="54" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E54" s="20"/>
-      <c r="F54" s="20"/>
-      <c r="G54" s="21"/>
-      <c r="H54" s="21"/>
-      <c r="I54" s="21"/>
+      <c r="E54" s="7">
+        <f t="shared" si="3"/>
+        <v>0.51000000000000023</v>
+      </c>
+      <c r="F54" s="7">
+        <f t="shared" si="4"/>
+        <v>510</v>
+      </c>
+      <c r="G54" s="17">
+        <f t="shared" si="0"/>
+        <v>226.78038263682842</v>
+      </c>
+      <c r="H54" s="15">
+        <f t="shared" si="1"/>
+        <v>1075.6098925925291</v>
+      </c>
+      <c r="I54" s="18">
+        <f t="shared" si="2"/>
+        <v>413.90325965767465</v>
+      </c>
     </row>
     <row r="55" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E55" s="20"/>
-      <c r="F55" s="20"/>
-      <c r="G55" s="21"/>
-      <c r="H55" s="21"/>
-      <c r="I55" s="21"/>
+      <c r="E55" s="7">
+        <f t="shared" si="3"/>
+        <v>0.52000000000000024</v>
+      </c>
+      <c r="F55" s="7">
+        <f t="shared" si="4"/>
+        <v>520</v>
+      </c>
+      <c r="G55" s="17">
+        <f t="shared" si="0"/>
+        <v>229.69181074890903</v>
+      </c>
+      <c r="H55" s="15">
+        <f t="shared" si="1"/>
+        <v>1077.5023176914574</v>
+      </c>
+      <c r="I55" s="18">
+        <f t="shared" si="2"/>
+        <v>416.59005046240736</v>
+      </c>
     </row>
     <row r="56" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E56" s="20"/>
-      <c r="F56" s="20"/>
-      <c r="G56" s="21"/>
-      <c r="H56" s="21"/>
-      <c r="I56" s="21"/>
+      <c r="E56" s="7">
+        <f t="shared" si="3"/>
+        <v>0.53000000000000025</v>
+      </c>
+      <c r="F56" s="7">
+        <f t="shared" si="4"/>
+        <v>530</v>
+      </c>
+      <c r="G56" s="17">
+        <f t="shared" si="0"/>
+        <v>232.54419093571011</v>
+      </c>
+      <c r="H56" s="15">
+        <f t="shared" si="1"/>
+        <v>1078.6563595230052</v>
+      </c>
+      <c r="I56" s="18">
+        <f t="shared" si="2"/>
+        <v>419.06803513696184</v>
+      </c>
     </row>
     <row r="57" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E57" s="20"/>
-      <c r="F57" s="20"/>
-      <c r="G57" s="21"/>
-      <c r="H57" s="21"/>
-      <c r="I57" s="21"/>
+      <c r="E57" s="7">
+        <f t="shared" si="3"/>
+        <v>0.54000000000000026</v>
+      </c>
+      <c r="F57" s="7">
+        <f t="shared" si="4"/>
+        <v>540</v>
+      </c>
+      <c r="G57" s="17">
+        <f t="shared" si="0"/>
+        <v>235.33752319723158</v>
+      </c>
+      <c r="H57" s="15">
+        <f t="shared" si="1"/>
+        <v>1079.072018087172</v>
+      </c>
+      <c r="I57" s="18">
+        <f t="shared" si="2"/>
+        <v>421.33721368133814</v>
+      </c>
     </row>
     <row r="58" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E58" s="20"/>
-      <c r="F58" s="20"/>
-      <c r="G58" s="21"/>
-      <c r="H58" s="21"/>
-      <c r="I58" s="21"/>
+      <c r="E58" s="7">
+        <f t="shared" si="3"/>
+        <v>0.55000000000000027</v>
+      </c>
+      <c r="F58" s="7">
+        <f t="shared" si="4"/>
+        <v>550</v>
+      </c>
+      <c r="G58" s="17">
+        <f t="shared" si="0"/>
+        <v>238.07180753347353</v>
+      </c>
+      <c r="H58" s="15">
+        <f t="shared" si="1"/>
+        <v>1078.7492933839576</v>
+      </c>
+      <c r="I58" s="18">
+        <f t="shared" si="2"/>
+        <v>423.3975860955361</v>
+      </c>
     </row>
     <row r="59" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E59" s="20"/>
-      <c r="F59" s="20"/>
-      <c r="G59" s="21"/>
-      <c r="H59" s="21"/>
-      <c r="I59" s="21"/>
+      <c r="E59" s="7">
+        <f t="shared" si="3"/>
+        <v>0.56000000000000028</v>
+      </c>
+      <c r="F59" s="7">
+        <f t="shared" si="4"/>
+        <v>560</v>
+      </c>
+      <c r="G59" s="17">
+        <f t="shared" si="0"/>
+        <v>240.74704394443592</v>
+      </c>
+      <c r="H59" s="15">
+        <f t="shared" si="1"/>
+        <v>1077.6881854133619</v>
+      </c>
+      <c r="I59" s="18">
+        <f t="shared" si="2"/>
+        <v>425.24915237955594</v>
+      </c>
     </row>
     <row r="60" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E60" s="20"/>
-      <c r="F60" s="20"/>
-      <c r="G60" s="21"/>
-      <c r="H60" s="21"/>
-      <c r="I60" s="21"/>
+      <c r="E60" s="7">
+        <f t="shared" si="3"/>
+        <v>0.57000000000000028</v>
+      </c>
+      <c r="F60" s="7">
+        <f t="shared" si="4"/>
+        <v>570</v>
+      </c>
+      <c r="G60" s="17">
+        <f t="shared" si="0"/>
+        <v>243.36323243011861</v>
+      </c>
+      <c r="H60" s="15">
+        <f t="shared" si="1"/>
+        <v>1075.8886941753858</v>
+      </c>
+      <c r="I60" s="18">
+        <f t="shared" si="2"/>
+        <v>426.8919125333976</v>
+      </c>
     </row>
     <row r="61" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E61" s="20"/>
-      <c r="F61" s="20"/>
-      <c r="G61" s="21"/>
-      <c r="H61" s="21"/>
-      <c r="I61" s="21"/>
+      <c r="E61" s="7">
+        <f t="shared" si="3"/>
+        <v>0.58000000000000029</v>
+      </c>
+      <c r="F61" s="7">
+        <f t="shared" si="4"/>
+        <v>580</v>
+      </c>
+      <c r="G61" s="17">
+        <f t="shared" si="0"/>
+        <v>245.92037299052186</v>
+      </c>
+      <c r="H61" s="15">
+        <f t="shared" si="1"/>
+        <v>1073.3508196700284</v>
+      </c>
+      <c r="I61" s="18">
+        <f t="shared" si="2"/>
+        <v>428.32586655706103</v>
+      </c>
     </row>
     <row r="62" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E62" s="20"/>
-      <c r="F62" s="20"/>
-      <c r="G62" s="21"/>
-      <c r="H62" s="21"/>
-      <c r="I62" s="21"/>
+      <c r="E62" s="7">
+        <f t="shared" si="3"/>
+        <v>0.5900000000000003</v>
+      </c>
+      <c r="F62" s="7">
+        <f t="shared" si="4"/>
+        <v>590</v>
+      </c>
+      <c r="G62" s="17">
+        <f t="shared" si="0"/>
+        <v>248.41846562564541</v>
+      </c>
+      <c r="H62" s="15">
+        <f t="shared" si="1"/>
+        <v>1070.0745618972901</v>
+      </c>
+      <c r="I62" s="18">
+        <f t="shared" si="2"/>
+        <v>429.55101445054623</v>
+      </c>
     </row>
     <row r="63" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E63" s="20"/>
-      <c r="F63" s="20"/>
-      <c r="G63" s="21"/>
-      <c r="H63" s="21"/>
-      <c r="I63" s="21"/>
+      <c r="E63" s="7">
+        <f t="shared" si="3"/>
+        <v>0.60000000000000031</v>
+      </c>
+      <c r="F63" s="7">
+        <f t="shared" si="4"/>
+        <v>600</v>
+      </c>
+      <c r="G63" s="17">
+        <f t="shared" si="0"/>
+        <v>250.85751033548951</v>
+      </c>
+      <c r="H63" s="15">
+        <f t="shared" si="1"/>
+        <v>1066.0599208571712</v>
+      </c>
+      <c r="I63" s="18">
+        <f t="shared" si="2"/>
+        <v>430.56735621385326</v>
+      </c>
     </row>
     <row r="64" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E64" s="20"/>
-      <c r="F64" s="20"/>
-      <c r="G64" s="21"/>
-      <c r="H64" s="21"/>
-      <c r="I64" s="21"/>
+      <c r="E64" s="7">
+        <f t="shared" si="3"/>
+        <v>0.61000000000000032</v>
+      </c>
+      <c r="F64" s="7">
+        <f t="shared" si="4"/>
+        <v>610</v>
+      </c>
+      <c r="G64" s="17">
+        <f t="shared" si="0"/>
+        <v>253.23750712005395</v>
+      </c>
+      <c r="H64" s="15">
+        <f t="shared" si="1"/>
+        <v>1061.3068965496705</v>
+      </c>
+      <c r="I64" s="18">
+        <f t="shared" si="2"/>
+        <v>431.37489184698205</v>
+      </c>
     </row>
     <row r="65" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E65" s="20"/>
-      <c r="F65" s="20"/>
-      <c r="G65" s="21"/>
-      <c r="H65" s="21"/>
-      <c r="I65" s="21"/>
+      <c r="E65" s="7">
+        <f t="shared" si="3"/>
+        <v>0.62000000000000033</v>
+      </c>
+      <c r="F65" s="7">
+        <f t="shared" si="4"/>
+        <v>620</v>
+      </c>
+      <c r="G65" s="17">
+        <f t="shared" si="0"/>
+        <v>255.55845597933885</v>
+      </c>
+      <c r="H65" s="15">
+        <f t="shared" si="1"/>
+        <v>1055.8154889747891</v>
+      </c>
+      <c r="I65" s="18">
+        <f t="shared" si="2"/>
+        <v>431.97362134993267</v>
+      </c>
     </row>
     <row r="66" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E66" s="20"/>
-      <c r="F66" s="20"/>
-      <c r="G66" s="21"/>
-      <c r="H66" s="21"/>
-      <c r="I66" s="21"/>
+      <c r="E66" s="7">
+        <f t="shared" si="3"/>
+        <v>0.63000000000000034</v>
+      </c>
+      <c r="F66" s="7">
+        <f t="shared" si="4"/>
+        <v>630</v>
+      </c>
+      <c r="G66" s="17">
+        <f t="shared" si="0"/>
+        <v>257.82035691334414</v>
+      </c>
+      <c r="H66" s="15">
+        <f t="shared" si="1"/>
+        <v>1049.5856981325271</v>
+      </c>
+      <c r="I66" s="18">
+        <f t="shared" si="2"/>
+        <v>432.36354472270494</v>
+      </c>
     </row>
     <row r="67" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E67" s="20"/>
-      <c r="F67" s="20"/>
-      <c r="G67" s="21"/>
-      <c r="H67" s="21"/>
-      <c r="I67" s="21"/>
+      <c r="E67" s="7">
+        <f t="shared" si="3"/>
+        <v>0.64000000000000035</v>
+      </c>
+      <c r="F67" s="7">
+        <f t="shared" si="4"/>
+        <v>640</v>
+      </c>
+      <c r="G67" s="17">
+        <f t="shared" ref="G67:G103" si="5">F67*TAN($C$11)-($C$5/(2*$C$6*$C$6))*(1+(TAN($C$11)*TAN($C$11)))*F67*F67</f>
+        <v>260.0232099220699</v>
+      </c>
+      <c r="H67" s="15">
+        <f t="shared" ref="H67:H103" si="6">F67*TAN($C$8)-($C$5/(2*$C$6*$C$6))*(1+(TAN($C$8)*TAN($C$8)))*F67*F67</f>
+        <v>1042.6175240228843</v>
+      </c>
+      <c r="I67" s="18">
+        <f t="shared" ref="I67:I103" si="7">F67*(($C$4+SQRT(($C$3*$C$3)+($C$4*$C$4)))/$C$3)-(SQRT(($C$3*$C$3)+($C$4*$C$4))/($C$3*$C$3))*(F67*F67)</f>
+        <v>432.5446619652991</v>
+      </c>
     </row>
     <row r="68" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E68" s="20"/>
-      <c r="F68" s="20"/>
-      <c r="G68" s="21"/>
-      <c r="H68" s="21"/>
-      <c r="I68" s="21"/>
+      <c r="E68" s="7">
+        <f t="shared" si="3"/>
+        <v>0.65000000000000036</v>
+      </c>
+      <c r="F68" s="7">
+        <f t="shared" si="4"/>
+        <v>650</v>
+      </c>
+      <c r="G68" s="17">
+        <f t="shared" si="5"/>
+        <v>262.16701500551608</v>
+      </c>
+      <c r="H68" s="15">
+        <f t="shared" si="6"/>
+        <v>1034.9109666458603</v>
+      </c>
+      <c r="I68" s="18">
+        <f t="shared" si="7"/>
+        <v>432.51697307771502</v>
+      </c>
     </row>
     <row r="69" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E69" s="20"/>
-      <c r="F69" s="20"/>
-      <c r="G69" s="21"/>
-      <c r="H69" s="21"/>
-      <c r="I69" s="21"/>
+      <c r="E69" s="7">
+        <f t="shared" ref="E69:E103" si="8">E68+0.01</f>
+        <v>0.66000000000000036</v>
+      </c>
+      <c r="F69" s="7">
+        <f t="shared" ref="F69:F103" si="9">F68+10</f>
+        <v>660</v>
+      </c>
+      <c r="G69" s="17">
+        <f t="shared" si="5"/>
+        <v>264.25177216368269</v>
+      </c>
+      <c r="H69" s="15">
+        <f t="shared" si="6"/>
+        <v>1026.4660260014546</v>
+      </c>
+      <c r="I69" s="18">
+        <f t="shared" si="7"/>
+        <v>432.28047805995277</v>
+      </c>
     </row>
     <row r="70" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E70" s="20"/>
-      <c r="F70" s="20"/>
-      <c r="G70" s="21"/>
-      <c r="H70" s="21"/>
-      <c r="I70" s="21"/>
+      <c r="E70" s="7">
+        <f t="shared" si="8"/>
+        <v>0.67000000000000037</v>
+      </c>
+      <c r="F70" s="7">
+        <f t="shared" si="9"/>
+        <v>670</v>
+      </c>
+      <c r="G70" s="17">
+        <f t="shared" si="5"/>
+        <v>266.27748139656967</v>
+      </c>
+      <c r="H70" s="15">
+        <f t="shared" si="6"/>
+        <v>1017.2827020896686</v>
+      </c>
+      <c r="I70" s="18">
+        <f t="shared" si="7"/>
+        <v>431.83517691201234</v>
+      </c>
     </row>
     <row r="71" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E71" s="20"/>
-      <c r="F71" s="20"/>
-      <c r="G71" s="21"/>
-      <c r="H71" s="21"/>
-      <c r="I71" s="21"/>
+      <c r="E71" s="7">
+        <f t="shared" si="8"/>
+        <v>0.68000000000000038</v>
+      </c>
+      <c r="F71" s="7">
+        <f t="shared" si="9"/>
+        <v>680</v>
+      </c>
+      <c r="G71" s="17">
+        <f t="shared" si="5"/>
+        <v>268.24414270417714</v>
+      </c>
+      <c r="H71" s="15">
+        <f t="shared" si="6"/>
+        <v>1007.3609949105016</v>
+      </c>
+      <c r="I71" s="18">
+        <f t="shared" si="7"/>
+        <v>431.18106963389363</v>
+      </c>
     </row>
     <row r="72" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E72" s="20"/>
-      <c r="F72" s="20"/>
-      <c r="G72" s="21"/>
-      <c r="H72" s="21"/>
-      <c r="I72" s="21"/>
+      <c r="E72" s="7">
+        <f t="shared" si="8"/>
+        <v>0.69000000000000039</v>
+      </c>
+      <c r="F72" s="7">
+        <f t="shared" si="9"/>
+        <v>690</v>
+      </c>
+      <c r="G72" s="17">
+        <f t="shared" si="5"/>
+        <v>270.15175608650497</v>
+      </c>
+      <c r="H72" s="15">
+        <f t="shared" si="6"/>
+        <v>996.70090446395375</v>
+      </c>
+      <c r="I72" s="18">
+        <f t="shared" si="7"/>
+        <v>430.31815622559674</v>
+      </c>
     </row>
     <row r="73" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E73" s="20"/>
-      <c r="F73" s="20"/>
-      <c r="G73" s="21"/>
-      <c r="H73" s="21"/>
-      <c r="I73" s="21"/>
+      <c r="E73" s="7">
+        <f t="shared" si="8"/>
+        <v>0.7000000000000004</v>
+      </c>
+      <c r="F73" s="7">
+        <f t="shared" si="9"/>
+        <v>700</v>
+      </c>
+      <c r="G73" s="17">
+        <f t="shared" si="5"/>
+        <v>272.0003215435533</v>
+      </c>
+      <c r="H73" s="15">
+        <f t="shared" si="6"/>
+        <v>985.30243075002477</v>
+      </c>
+      <c r="I73" s="18">
+        <f t="shared" si="7"/>
+        <v>429.24643668712156</v>
+      </c>
     </row>
     <row r="74" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E74" s="20"/>
-      <c r="F74" s="20"/>
-      <c r="G74" s="21"/>
-      <c r="H74" s="21"/>
-      <c r="I74" s="21"/>
+      <c r="E74" s="7">
+        <f t="shared" si="8"/>
+        <v>0.71000000000000041</v>
+      </c>
+      <c r="F74" s="7">
+        <f t="shared" si="9"/>
+        <v>710</v>
+      </c>
+      <c r="G74" s="17">
+        <f t="shared" si="5"/>
+        <v>273.78983907532199</v>
+      </c>
+      <c r="H74" s="15">
+        <f t="shared" si="6"/>
+        <v>973.16557376871447</v>
+      </c>
+      <c r="I74" s="18">
+        <f t="shared" si="7"/>
+        <v>427.9659110184682</v>
+      </c>
     </row>
     <row r="75" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E75" s="20"/>
-      <c r="F75" s="20"/>
-      <c r="G75" s="21"/>
-      <c r="H75" s="21"/>
-      <c r="I75" s="21"/>
+      <c r="E75" s="7">
+        <f t="shared" si="8"/>
+        <v>0.72000000000000042</v>
+      </c>
+      <c r="F75" s="7">
+        <f t="shared" si="9"/>
+        <v>720</v>
+      </c>
+      <c r="G75" s="17">
+        <f t="shared" si="5"/>
+        <v>275.52030868181112</v>
+      </c>
+      <c r="H75" s="15">
+        <f t="shared" si="6"/>
+        <v>960.29033352002375</v>
+      </c>
+      <c r="I75" s="18">
+        <f t="shared" si="7"/>
+        <v>426.47657921963673</v>
+      </c>
     </row>
     <row r="76" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E76" s="20"/>
-      <c r="F76" s="20"/>
-      <c r="G76" s="21"/>
-      <c r="H76" s="21"/>
-      <c r="I76" s="21"/>
+      <c r="E76" s="7">
+        <f t="shared" si="8"/>
+        <v>0.73000000000000043</v>
+      </c>
+      <c r="F76" s="7">
+        <f t="shared" si="9"/>
+        <v>730</v>
+      </c>
+      <c r="G76" s="17">
+        <f t="shared" si="5"/>
+        <v>277.19173036302072</v>
+      </c>
+      <c r="H76" s="15">
+        <f t="shared" si="6"/>
+        <v>946.67671000395148</v>
+      </c>
+      <c r="I76" s="18">
+        <f t="shared" si="7"/>
+        <v>424.77844129062703</v>
+      </c>
     </row>
     <row r="77" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E77" s="20"/>
-      <c r="F77" s="20"/>
-      <c r="G77" s="21"/>
-      <c r="H77" s="21"/>
-      <c r="I77" s="21"/>
+      <c r="E77" s="7">
+        <f t="shared" si="8"/>
+        <v>0.74000000000000044</v>
+      </c>
+      <c r="F77" s="7">
+        <f t="shared" si="9"/>
+        <v>740</v>
+      </c>
+      <c r="G77" s="17">
+        <f t="shared" si="5"/>
+        <v>278.8041041189507</v>
+      </c>
+      <c r="H77" s="15">
+        <f t="shared" si="6"/>
+        <v>932.3247032204988</v>
+      </c>
+      <c r="I77" s="18">
+        <f t="shared" si="7"/>
+        <v>422.87149723143909</v>
+      </c>
     </row>
     <row r="78" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E78" s="20"/>
-      <c r="F78" s="20"/>
-      <c r="G78" s="21"/>
-      <c r="H78" s="21"/>
-      <c r="I78" s="21"/>
+      <c r="E78" s="7">
+        <f t="shared" si="8"/>
+        <v>0.75000000000000044</v>
+      </c>
+      <c r="F78" s="7">
+        <f t="shared" si="9"/>
+        <v>750</v>
+      </c>
+      <c r="G78" s="17">
+        <f t="shared" si="5"/>
+        <v>280.35742994960117</v>
+      </c>
+      <c r="H78" s="15">
+        <f t="shared" si="6"/>
+        <v>917.2343131696648</v>
+      </c>
+      <c r="I78" s="18">
+        <f t="shared" si="7"/>
+        <v>420.75574704207293</v>
+      </c>
     </row>
     <row r="79" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E79" s="20"/>
-      <c r="F79" s="20"/>
-      <c r="G79" s="21"/>
-      <c r="H79" s="21"/>
-      <c r="I79" s="21"/>
+      <c r="E79" s="7">
+        <f t="shared" si="8"/>
+        <v>0.76000000000000045</v>
+      </c>
+      <c r="F79" s="7">
+        <f t="shared" si="9"/>
+        <v>760</v>
+      </c>
+      <c r="G79" s="17">
+        <f t="shared" si="5"/>
+        <v>281.85170785497201</v>
+      </c>
+      <c r="H79" s="15">
+        <f t="shared" si="6"/>
+        <v>901.40553985145016</v>
+      </c>
+      <c r="I79" s="18">
+        <f t="shared" si="7"/>
+        <v>418.43119072252853</v>
+      </c>
     </row>
     <row r="80" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E80" s="20"/>
-      <c r="F80" s="20"/>
-      <c r="G80" s="21"/>
-      <c r="H80" s="21"/>
-      <c r="I80" s="21"/>
+      <c r="E80" s="7">
+        <f t="shared" si="8"/>
+        <v>0.77000000000000046</v>
+      </c>
+      <c r="F80" s="7">
+        <f t="shared" si="9"/>
+        <v>770</v>
+      </c>
+      <c r="G80" s="17">
+        <f t="shared" si="5"/>
+        <v>283.28693783506333</v>
+      </c>
+      <c r="H80" s="15">
+        <f t="shared" si="6"/>
+        <v>884.83838326585374</v>
+      </c>
+      <c r="I80" s="18">
+        <f t="shared" si="7"/>
+        <v>415.89782827280578</v>
+      </c>
     </row>
     <row r="81" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E81" s="20"/>
-      <c r="F81" s="20"/>
-      <c r="G81" s="21"/>
-      <c r="H81" s="21"/>
-      <c r="I81" s="21"/>
+      <c r="E81" s="7">
+        <f t="shared" si="8"/>
+        <v>0.78000000000000047</v>
+      </c>
+      <c r="F81" s="7">
+        <f t="shared" si="9"/>
+        <v>780</v>
+      </c>
+      <c r="G81" s="17">
+        <f t="shared" si="5"/>
+        <v>284.66311988987496</v>
+      </c>
+      <c r="H81" s="15">
+        <f t="shared" si="6"/>
+        <v>867.53284341287736</v>
+      </c>
+      <c r="I81" s="18">
+        <f t="shared" si="7"/>
+        <v>413.15565969290515</v>
+      </c>
     </row>
     <row r="82" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E82" s="20"/>
-      <c r="F82" s="20"/>
-      <c r="G82" s="21"/>
-      <c r="H82" s="21"/>
-      <c r="I82" s="21"/>
+      <c r="E82" s="7">
+        <f t="shared" si="8"/>
+        <v>0.79000000000000048</v>
+      </c>
+      <c r="F82" s="7">
+        <f t="shared" si="9"/>
+        <v>790</v>
+      </c>
+      <c r="G82" s="17">
+        <f t="shared" si="5"/>
+        <v>285.98025401940708</v>
+      </c>
+      <c r="H82" s="15">
+        <f t="shared" si="6"/>
+        <v>849.48892029251965</v>
+      </c>
+      <c r="I82" s="18">
+        <f t="shared" si="7"/>
+        <v>410.20468498282605</v>
+      </c>
     </row>
     <row r="83" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E83" s="20"/>
-      <c r="F83" s="20"/>
-      <c r="G83" s="21"/>
-      <c r="H83" s="21"/>
-      <c r="I83" s="21"/>
+      <c r="E83" s="7">
+        <f t="shared" si="8"/>
+        <v>0.80000000000000049</v>
+      </c>
+      <c r="F83" s="7">
+        <f t="shared" si="9"/>
+        <v>800</v>
+      </c>
+      <c r="G83" s="17">
+        <f t="shared" si="5"/>
+        <v>287.23834022365963</v>
+      </c>
+      <c r="H83" s="15">
+        <f t="shared" si="6"/>
+        <v>830.70661390478062</v>
+      </c>
+      <c r="I83" s="18">
+        <f t="shared" si="7"/>
+        <v>407.04490414256895</v>
+      </c>
     </row>
     <row r="84" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E84" s="20"/>
-      <c r="F84" s="20"/>
-      <c r="G84" s="21"/>
-      <c r="H84" s="21"/>
-      <c r="I84" s="21"/>
+      <c r="E84" s="7">
+        <f t="shared" si="8"/>
+        <v>0.8100000000000005</v>
+      </c>
+      <c r="F84" s="7">
+        <f t="shared" si="9"/>
+        <v>810</v>
+      </c>
+      <c r="G84" s="17">
+        <f t="shared" si="5"/>
+        <v>288.43737850263267</v>
+      </c>
+      <c r="H84" s="15">
+        <f t="shared" si="6"/>
+        <v>811.18592424966073</v>
+      </c>
+      <c r="I84" s="18">
+        <f t="shared" si="7"/>
+        <v>403.67631717213339</v>
+      </c>
     </row>
     <row r="85" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E85" s="20"/>
-      <c r="F85" s="20"/>
-      <c r="G85" s="21"/>
-      <c r="H85" s="21"/>
-      <c r="I85" s="21"/>
+      <c r="E85" s="7">
+        <f t="shared" si="8"/>
+        <v>0.82000000000000051</v>
+      </c>
+      <c r="F85" s="7">
+        <f t="shared" si="9"/>
+        <v>820</v>
+      </c>
+      <c r="G85" s="17">
+        <f t="shared" si="5"/>
+        <v>289.57736885632602</v>
+      </c>
+      <c r="H85" s="15">
+        <f t="shared" si="6"/>
+        <v>790.92685132716042</v>
+      </c>
+      <c r="I85" s="18">
+        <f t="shared" si="7"/>
+        <v>400.09892407151972</v>
+      </c>
     </row>
     <row r="86" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E86" s="20"/>
-      <c r="F86" s="20"/>
-      <c r="G86" s="21"/>
-      <c r="H86" s="21"/>
-      <c r="I86" s="21"/>
+      <c r="E86" s="7">
+        <f t="shared" si="8"/>
+        <v>0.83000000000000052</v>
+      </c>
+      <c r="F86" s="7">
+        <f t="shared" si="9"/>
+        <v>830</v>
+      </c>
+      <c r="G86" s="17">
+        <f t="shared" si="5"/>
+        <v>290.65831128473985</v>
+      </c>
+      <c r="H86" s="15">
+        <f t="shared" si="6"/>
+        <v>769.92939513727879</v>
+      </c>
+      <c r="I86" s="18">
+        <f t="shared" si="7"/>
+        <v>396.31272484072792</v>
+      </c>
     </row>
     <row r="87" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E87" s="20"/>
-      <c r="F87" s="20"/>
-      <c r="G87" s="21"/>
-      <c r="H87" s="21"/>
-      <c r="I87" s="21"/>
+      <c r="E87" s="7">
+        <f t="shared" si="8"/>
+        <v>0.84000000000000052</v>
+      </c>
+      <c r="F87" s="7">
+        <f t="shared" si="9"/>
+        <v>840</v>
+      </c>
+      <c r="G87" s="17">
+        <f t="shared" si="5"/>
+        <v>291.68020578787406</v>
+      </c>
+      <c r="H87" s="15">
+        <f t="shared" si="6"/>
+        <v>748.19355568001629</v>
+      </c>
+      <c r="I87" s="18">
+        <f t="shared" si="7"/>
+        <v>392.31771947975778</v>
+      </c>
     </row>
     <row r="88" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E88" s="20"/>
-      <c r="F88" s="20"/>
-      <c r="G88" s="21"/>
-      <c r="H88" s="21"/>
-      <c r="I88" s="21"/>
+      <c r="E88" s="7">
+        <f t="shared" si="8"/>
+        <v>0.85000000000000053</v>
+      </c>
+      <c r="F88" s="7">
+        <f t="shared" si="9"/>
+        <v>850</v>
+      </c>
+      <c r="G88" s="17">
+        <f t="shared" si="5"/>
+        <v>292.64305236572881</v>
+      </c>
+      <c r="H88" s="15">
+        <f t="shared" si="6"/>
+        <v>725.71933295537201</v>
+      </c>
+      <c r="I88" s="18">
+        <f t="shared" si="7"/>
+        <v>388.11390798860964</v>
+      </c>
     </row>
     <row r="89" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E89" s="20"/>
-      <c r="F89" s="20"/>
-      <c r="G89" s="21"/>
-      <c r="H89" s="21"/>
-      <c r="I89" s="21"/>
+      <c r="E89" s="7">
+        <f t="shared" si="8"/>
+        <v>0.86000000000000054</v>
+      </c>
+      <c r="F89" s="7">
+        <f t="shared" si="9"/>
+        <v>860</v>
+      </c>
+      <c r="G89" s="17">
+        <f t="shared" si="5"/>
+        <v>293.54685101830387</v>
+      </c>
+      <c r="H89" s="15">
+        <f t="shared" si="6"/>
+        <v>702.50672696334732</v>
+      </c>
+      <c r="I89" s="18">
+        <f t="shared" si="7"/>
+        <v>383.70129036728304</v>
+      </c>
     </row>
     <row r="90" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E90" s="20"/>
-      <c r="F90" s="20"/>
-      <c r="G90" s="21"/>
-      <c r="H90" s="21"/>
-      <c r="I90" s="21"/>
+      <c r="E90" s="7">
+        <f t="shared" si="8"/>
+        <v>0.87000000000000055</v>
+      </c>
+      <c r="F90" s="7">
+        <f t="shared" si="9"/>
+        <v>870</v>
+      </c>
+      <c r="G90" s="17">
+        <f t="shared" si="5"/>
+        <v>294.39160174559936</v>
+      </c>
+      <c r="H90" s="15">
+        <f t="shared" si="6"/>
+        <v>678.55573770394221</v>
+      </c>
+      <c r="I90" s="18">
+        <f t="shared" si="7"/>
+        <v>379.07986661577843</v>
+      </c>
     </row>
     <row r="91" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E91" s="20"/>
-      <c r="F91" s="20"/>
-      <c r="G91" s="21"/>
-      <c r="H91" s="21"/>
-      <c r="I91" s="21"/>
+      <c r="E91" s="7">
+        <f t="shared" si="8"/>
+        <v>0.88000000000000056</v>
+      </c>
+      <c r="F91" s="7">
+        <f t="shared" si="9"/>
+        <v>880</v>
+      </c>
+      <c r="G91" s="17">
+        <f t="shared" si="5"/>
+        <v>295.17730454761534</v>
+      </c>
+      <c r="H91" s="15">
+        <f t="shared" si="6"/>
+        <v>653.86636517715533</v>
+      </c>
+      <c r="I91" s="18">
+        <f t="shared" si="7"/>
+        <v>374.24963673409547</v>
+      </c>
     </row>
     <row r="92" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E92" s="20"/>
-      <c r="F92" s="20"/>
-      <c r="G92" s="21"/>
-      <c r="H92" s="21"/>
-      <c r="I92" s="21"/>
+      <c r="E92" s="7">
+        <f t="shared" si="8"/>
+        <v>0.89000000000000057</v>
+      </c>
+      <c r="F92" s="7">
+        <f t="shared" si="9"/>
+        <v>890</v>
+      </c>
+      <c r="G92" s="17">
+        <f t="shared" si="5"/>
+        <v>295.90395942435168</v>
+      </c>
+      <c r="H92" s="15">
+        <f t="shared" si="6"/>
+        <v>628.43860938298803</v>
+      </c>
+      <c r="I92" s="18">
+        <f t="shared" si="7"/>
+        <v>369.21060072223418</v>
+      </c>
     </row>
     <row r="93" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E93" s="20"/>
-      <c r="F93" s="20"/>
-      <c r="G93" s="21"/>
-      <c r="H93" s="21"/>
-      <c r="I93" s="21"/>
+      <c r="E93" s="7">
+        <f t="shared" si="8"/>
+        <v>0.90000000000000058</v>
+      </c>
+      <c r="F93" s="7">
+        <f t="shared" si="9"/>
+        <v>900</v>
+      </c>
+      <c r="G93" s="17">
+        <f t="shared" si="5"/>
+        <v>296.57156637580857</v>
+      </c>
+      <c r="H93" s="15">
+        <f t="shared" si="6"/>
+        <v>602.27247032143941</v>
+      </c>
+      <c r="I93" s="18">
+        <f t="shared" si="7"/>
+        <v>363.96275858019499</v>
+      </c>
     </row>
     <row r="94" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E94" s="20"/>
-      <c r="F94" s="20"/>
-      <c r="G94" s="21"/>
-      <c r="H94" s="21"/>
-      <c r="I94" s="21"/>
+      <c r="E94" s="7">
+        <f t="shared" si="8"/>
+        <v>0.91000000000000059</v>
+      </c>
+      <c r="F94" s="7">
+        <f t="shared" si="9"/>
+        <v>910</v>
+      </c>
+      <c r="G94" s="17">
+        <f t="shared" si="5"/>
+        <v>297.18012540198578</v>
+      </c>
+      <c r="H94" s="15">
+        <f t="shared" si="6"/>
+        <v>575.36794799250993</v>
+      </c>
+      <c r="I94" s="18">
+        <f t="shared" si="7"/>
+        <v>358.50611030797734</v>
+      </c>
     </row>
     <row r="95" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E95" s="20"/>
-      <c r="F95" s="20"/>
-      <c r="G95" s="21"/>
-      <c r="H95" s="21"/>
-      <c r="I95" s="21"/>
+      <c r="E95" s="7">
+        <f t="shared" si="8"/>
+        <v>0.9200000000000006</v>
+      </c>
+      <c r="F95" s="7">
+        <f t="shared" si="9"/>
+        <v>920</v>
+      </c>
+      <c r="G95" s="17">
+        <f t="shared" si="5"/>
+        <v>297.72963650288341</v>
+      </c>
+      <c r="H95" s="15">
+        <f t="shared" si="6"/>
+        <v>547.72504239619911</v>
+      </c>
+      <c r="I95" s="18">
+        <f t="shared" si="7"/>
+        <v>352.8406559055818</v>
+      </c>
     </row>
     <row r="96" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E96" s="20"/>
-      <c r="F96" s="20"/>
-      <c r="G96" s="21"/>
-      <c r="H96" s="21"/>
-      <c r="I96" s="21"/>
+      <c r="E96" s="7">
+        <f t="shared" si="8"/>
+        <v>0.9300000000000006</v>
+      </c>
+      <c r="F96" s="7">
+        <f t="shared" si="9"/>
+        <v>930</v>
+      </c>
+      <c r="G96" s="17">
+        <f t="shared" si="5"/>
+        <v>298.22009967850158</v>
+      </c>
+      <c r="H96" s="15">
+        <f t="shared" si="6"/>
+        <v>519.34375353250789</v>
+      </c>
+      <c r="I96" s="18">
+        <f t="shared" si="7"/>
+        <v>346.96639537300769</v>
+      </c>
     </row>
     <row r="97" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E97" s="20"/>
-      <c r="F97" s="20"/>
-      <c r="G97" s="21"/>
-      <c r="H97" s="21"/>
-      <c r="I97" s="21"/>
+      <c r="E97" s="7">
+        <f t="shared" si="8"/>
+        <v>0.94000000000000061</v>
+      </c>
+      <c r="F97" s="7">
+        <f t="shared" si="9"/>
+        <v>940</v>
+      </c>
+      <c r="G97" s="17">
+        <f t="shared" si="5"/>
+        <v>298.65151492884002</v>
+      </c>
+      <c r="H97" s="15">
+        <f t="shared" si="6"/>
+        <v>490.2240814014358</v>
+      </c>
+      <c r="I97" s="18">
+        <f t="shared" si="7"/>
+        <v>340.88332871025568</v>
+      </c>
     </row>
     <row r="98" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E98" s="20"/>
-      <c r="F98" s="20"/>
-      <c r="G98" s="21"/>
-      <c r="H98" s="21"/>
-      <c r="I98" s="21"/>
+      <c r="E98" s="7">
+        <f t="shared" si="8"/>
+        <v>0.95000000000000062</v>
+      </c>
+      <c r="F98" s="7">
+        <f t="shared" si="9"/>
+        <v>950</v>
+      </c>
+      <c r="G98" s="17">
+        <f t="shared" si="5"/>
+        <v>299.02388225389893</v>
+      </c>
+      <c r="H98" s="15">
+        <f t="shared" si="6"/>
+        <v>460.36602600298193</v>
+      </c>
+      <c r="I98" s="18">
+        <f t="shared" si="7"/>
+        <v>334.59145591732511</v>
+      </c>
     </row>
     <row r="99" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E99" s="20"/>
-      <c r="F99" s="20"/>
-      <c r="G99" s="21"/>
-      <c r="H99" s="21"/>
-      <c r="I99" s="21"/>
+      <c r="E99" s="7">
+        <f t="shared" si="8"/>
+        <v>0.96000000000000063</v>
+      </c>
+      <c r="F99" s="7">
+        <f t="shared" si="9"/>
+        <v>960</v>
+      </c>
+      <c r="G99" s="17">
+        <f t="shared" si="5"/>
+        <v>299.33720165367828</v>
+      </c>
+      <c r="H99" s="15">
+        <f t="shared" si="6"/>
+        <v>429.76958733714764</v>
+      </c>
+      <c r="I99" s="18">
+        <f t="shared" si="7"/>
+        <v>328.09077699421641</v>
+      </c>
     </row>
     <row r="100" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E100" s="20"/>
-      <c r="F100" s="20"/>
-      <c r="G100" s="21"/>
-      <c r="H100" s="21"/>
-      <c r="I100" s="21"/>
+      <c r="E100" s="7">
+        <f t="shared" si="8"/>
+        <v>0.97000000000000064</v>
+      </c>
+      <c r="F100" s="7">
+        <f t="shared" si="9"/>
+        <v>970</v>
+      </c>
+      <c r="G100" s="17">
+        <f t="shared" si="5"/>
+        <v>299.59147312817811</v>
+      </c>
+      <c r="H100" s="15">
+        <f t="shared" si="6"/>
+        <v>398.43476540393249</v>
+      </c>
+      <c r="I100" s="18">
+        <f t="shared" si="7"/>
+        <v>321.38129194092971</v>
+      </c>
     </row>
     <row r="101" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E101" s="20"/>
-      <c r="F101" s="20"/>
-      <c r="G101" s="21"/>
-      <c r="H101" s="21"/>
-      <c r="I101" s="21"/>
+      <c r="E101" s="7">
+        <f t="shared" si="8"/>
+        <v>0.98000000000000065</v>
+      </c>
+      <c r="F101" s="7">
+        <f t="shared" si="9"/>
+        <v>980</v>
+      </c>
+      <c r="G101" s="17">
+        <f t="shared" si="5"/>
+        <v>299.78669667739831</v>
+      </c>
+      <c r="H101" s="15">
+        <f t="shared" si="6"/>
+        <v>366.36156020333601</v>
+      </c>
+      <c r="I101" s="18">
+        <f t="shared" si="7"/>
+        <v>314.46300075746467</v>
+      </c>
     </row>
     <row r="102" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E102" s="20"/>
-      <c r="F102" s="20"/>
-      <c r="G102" s="21"/>
-      <c r="H102" s="21"/>
-      <c r="I102" s="21"/>
+      <c r="E102" s="7">
+        <f t="shared" si="8"/>
+        <v>0.99000000000000066</v>
+      </c>
+      <c r="F102" s="7">
+        <f t="shared" si="9"/>
+        <v>990</v>
+      </c>
+      <c r="G102" s="17">
+        <f t="shared" si="5"/>
+        <v>299.92287230133888</v>
+      </c>
+      <c r="H102" s="15">
+        <f t="shared" si="6"/>
+        <v>333.54997173535912</v>
+      </c>
+      <c r="I102" s="18">
+        <f t="shared" si="7"/>
+        <v>307.33590344382151</v>
+      </c>
     </row>
     <row r="103" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E103" s="20"/>
-      <c r="F103" s="20"/>
-      <c r="G103" s="21"/>
-      <c r="H103" s="21"/>
-      <c r="I103" s="21"/>
-    </row>
-    <row r="104" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E104" s="20"/>
-      <c r="F104" s="20"/>
-      <c r="G104" s="20"/>
-      <c r="H104" s="20"/>
-      <c r="I104" s="20"/>
-    </row>
-    <row r="105" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E105" s="20"/>
-      <c r="F105" s="20"/>
-      <c r="G105" s="20"/>
-      <c r="H105" s="20"/>
-      <c r="I105" s="20"/>
-    </row>
-    <row r="106" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E106" s="20"/>
-      <c r="F106" s="20"/>
-      <c r="G106" s="20"/>
-      <c r="H106" s="20"/>
-      <c r="I106" s="20"/>
-    </row>
-    <row r="107" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E107" s="20"/>
-      <c r="F107" s="20"/>
-      <c r="G107" s="20"/>
-      <c r="H107" s="20"/>
-      <c r="I107" s="20"/>
-    </row>
-    <row r="108" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E108" s="20"/>
-      <c r="F108" s="20"/>
-      <c r="G108" s="20"/>
-      <c r="H108" s="20"/>
-      <c r="I108" s="20"/>
-    </row>
-    <row r="109" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E109" s="20"/>
-      <c r="F109" s="20"/>
-      <c r="G109" s="20"/>
-      <c r="H109" s="20"/>
-      <c r="I109" s="20"/>
-    </row>
-    <row r="110" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E110" s="20"/>
-      <c r="F110" s="20"/>
-      <c r="G110" s="20"/>
-      <c r="H110" s="20"/>
-      <c r="I110" s="20"/>
-    </row>
-    <row r="111" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E111" s="20"/>
-      <c r="F111" s="20"/>
-      <c r="G111" s="20"/>
-      <c r="H111" s="20"/>
-      <c r="I111" s="20"/>
-    </row>
-    <row r="112" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E112" s="20"/>
-      <c r="F112" s="20"/>
-      <c r="G112" s="20"/>
-      <c r="H112" s="20"/>
-      <c r="I112" s="20"/>
-    </row>
-    <row r="113" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E113" s="20"/>
-      <c r="F113" s="20"/>
-      <c r="G113" s="20"/>
-      <c r="H113" s="20"/>
-      <c r="I113" s="20"/>
-    </row>
-    <row r="114" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E114" s="20"/>
-      <c r="F114" s="20"/>
-      <c r="G114" s="20"/>
-      <c r="H114" s="20"/>
-      <c r="I114" s="20"/>
-    </row>
-    <row r="115" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E115" s="20"/>
-      <c r="F115" s="20"/>
-      <c r="G115" s="20"/>
-      <c r="H115" s="20"/>
-      <c r="I115" s="20"/>
+      <c r="E103" s="7">
+        <f t="shared" si="8"/>
+        <v>1.0000000000000007</v>
+      </c>
+      <c r="F103" s="7">
+        <f t="shared" si="9"/>
+        <v>1000</v>
+      </c>
+      <c r="G103" s="17">
+        <f t="shared" si="5"/>
+        <v>299.99999999999994</v>
+      </c>
+      <c r="H103" s="15">
+        <f t="shared" si="6"/>
+        <v>300</v>
+      </c>
+      <c r="I103" s="18">
+        <f t="shared" si="7"/>
+        <v>300</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added graph + formatted all columns to look nicer
</commit_message>
<xml_diff>
--- a/models.xlsx
+++ b/models.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ssb\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A96BB06-EEF3-42F6-BB9B-D6620C6153A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DEACD7E-78E4-4324-8882-D60E5B31F1C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{6422CA17-FA72-4B85-908A-20157EF2E374}"/>
   </bookViews>
@@ -2873,6 +2873,2673 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Projectile to hit X,Y</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13983145974677694"/>
+          <c:y val="0.17192748257461196"/>
+          <c:w val="0.82047462817147854"/>
+          <c:h val="0.6153546952464275"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]Sheet3!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y low ball</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>[1]Sheet3!$F$3:$F$103</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>560</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>570</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>610</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>670</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>690</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>710</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>740</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>770</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>790</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>810</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>820</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>830</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>840</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>870</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>880</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>890</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>910</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>920</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>930</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>940</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>960</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>970</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>990</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>[1]Sheet3!$G$3:$G$103</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.9228723013389413</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.786696677398309</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.591473128178098</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>23.337201653678321</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>29.023882253898961</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>34.651514928840029</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40.220099678501526</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45.729636502883444</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>51.180125401985791</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>56.571566375808558</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>61.903959424351754</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>67.177304547615364</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>72.391601745599417</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>77.546851018303897</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>82.643052365728792</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>87.680205787874115</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>92.658311284739867</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>97.577368856326032</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>102.43737850263264</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>107.23834022365966</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>111.9802540194071</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>116.66311988987498</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>121.28693783506327</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>125.85170785497201</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>130.35742994960114</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>134.80410411895073</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>139.19173036302072</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>143.52030868181117</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>147.78983907532202</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>152.0003215435533</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>156.151756086505</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>160.24414270417714</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>164.2774813965697</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>168.25177216368269</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>172.16701500551608</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>176.0232099220699</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>179.82035691334414</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>183.55845597933885</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>187.23750712005395</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>190.85751033548948</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>194.41846562564544</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>197.9203729905218</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>201.36323243011861</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>204.74704394443586</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>208.07180753347353</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>211.3375231972316</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>214.54419093571013</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>217.69181074890906</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>220.78038263682845</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>223.80990659946821</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>226.78038263682842</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>229.69181074890903</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>232.54419093571011</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>235.33752319723158</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>238.07180753347353</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>240.74704394443592</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>243.36323243011861</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>245.92037299052186</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>248.41846562564541</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>250.85751033548951</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>253.23750712005395</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>255.55845597933885</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>257.82035691334414</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>260.0232099220699</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>262.16701500551608</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>264.25177216368269</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>266.27748139656967</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>268.24414270417714</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>270.15175608650497</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>272.0003215435533</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>273.78983907532199</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>275.52030868181112</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>277.19173036302072</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>278.8041041189507</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>280.35742994960117</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>281.85170785497201</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>283.28693783506333</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>284.66311988987496</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>285.98025401940708</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>287.23834022365963</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>288.43737850263267</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>289.57736885632602</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>290.65831128473985</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>291.68020578787406</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>292.64305236572881</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>293.54685101830387</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>294.39160174559936</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>295.17730454761534</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>295.90395942435168</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>296.57156637580857</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>297.18012540198578</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>297.72963650288341</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>298.22009967850158</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>298.65151492884002</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>299.02388225389893</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>299.33720165367828</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>299.59147312817811</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>299.78669667739831</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>299.92287230133888</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>299.99999999999994</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7DF7-44AC-A0A5-8B3CD2631530}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]Sheet3!$H$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y high ball </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>[1]Sheet3!$F$3:$F$103</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>560</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>570</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>610</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>670</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>690</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>710</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>740</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>770</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>790</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>810</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>820</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>830</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>840</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>870</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>880</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>890</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>910</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>920</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>930</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>940</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>960</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>970</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>990</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>[1]Sheet3!$H$3:$H$103</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>39.549971735358291</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>78.361560203335614</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>116.43476540393195</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>153.76958733714733</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>190.3660260029817</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>226.22408140143511</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>261.34375353250755</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>295.72504239619906</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>329.36794799250953</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>362.27247032143902</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>394.43860938298758</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>425.8663651771551</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>456.5557377039417</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>486.50672696334726</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>515.71933295537201</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>544.19355568001561</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>571.92939513727833</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>598.92685132715997</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>625.18592424966073</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>650.7066139047804</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>675.48892029251931</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>699.53284341287713</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>722.83838326585396</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>745.4055398514497</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>767.23431316966457</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>788.32470322049846</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>808.67671000395148</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>828.2903335200233</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>847.16557376871447</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>865.30243075002454</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>882.70090446395329</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>899.36099491050163</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>915.28270208966842</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>930.46602600145468</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>944.91096664585984</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>958.61752402288403</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>971.58569813252711</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>983.81548897478933</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>995.30689654967057</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1006.0599208571707</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1016.0745618972901</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1025.3508196700286</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1033.8886941753856</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1041.6881854133621</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1048.7492933839574</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1055.0720180871717</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1060.6563595230054</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1065.5023176914576</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1069.6098925925291</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1072.9790842262196</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1075.6098925925291</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1077.5023176914574</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1078.6563595230052</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1079.072018087172</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1078.7492933839576</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1077.6881854133619</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1075.8886941753858</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1073.3508196700284</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1070.0745618972901</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1066.0599208571712</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1061.3068965496705</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1055.8154889747891</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1049.5856981325271</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1042.6175240228843</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1034.9109666458603</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1026.4660260014546</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1017.2827020896686</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1007.3609949105016</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>996.70090446395375</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>985.30243075002477</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>973.16557376871447</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>960.29033352002375</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>946.67671000395148</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>932.3247032204988</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>917.2343131696648</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>901.40553985145016</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>884.83838326585374</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>867.53284341287736</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>849.48892029251965</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>830.70661390478062</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>811.18592424966073</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>790.92685132716042</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>769.92939513727879</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>748.19355568001629</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>725.71933295537201</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>702.50672696334732</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>678.55573770394221</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>653.86636517715533</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>628.43860938298803</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>602.27247032143941</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>575.36794799250993</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>547.72504239619911</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>519.34375353250789</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>490.2240814014358</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>460.36602600298193</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>429.76958733714764</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>398.43476540393249</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>366.36156020333601</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>333.54997173535912</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7DF7-44AC-A0A5-8B3CD2631530}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]Sheet3!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y min u </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent3">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>[1]Sheet3!$F$3:$F$103</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>560</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>570</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>610</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>650</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>670</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>690</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>710</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>740</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>770</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>790</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>810</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>820</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>830</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>840</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>860</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>870</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>880</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>890</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>910</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>920</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>930</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>940</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>960</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>970</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>980</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>990</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>[1]Sheet3!$I$3:$I$103</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="101"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.335903443821445</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.46300075746468</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39.3812919409297</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>52.090776994216512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>64.591455917325121</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>76.883328710255498</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>88.966395373007686</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100.84065590558166</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>112.50611030797741</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>123.96275858019497</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>135.21060072223429</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>146.24963673409542</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>157.07986661577834</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>167.70129036728304</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>178.11390798860953</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>188.31771947975781</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>198.3127248407279</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>208.09892407151972</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>217.67631717213339</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>227.04490414256884</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>236.20468498282602</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>245.15565969290506</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>253.8978282728059</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>262.43119072252841</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>270.75574704207281</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>278.87149723143898</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>286.77844129062697</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>294.47657921963668</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>301.96591101846826</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>309.24643668712156</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>316.31815622559674</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>323.18106963389357</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>329.83517691201229</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>336.28047805995277</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>342.51697307771502</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>348.5446619652991</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>354.363544722705</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>359.97362134993261</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>365.37489184698205</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>370.56735621385326</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>375.55101445054618</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>380.32586655706098</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>384.8919125333976</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>389.24915237955599</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>393.39758609553616</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>397.33721368133814</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>401.0680351369619</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>404.59005046240731</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>407.90325965767465</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>411.00766272276377</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>413.90325965767465</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>416.59005046240736</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>419.06803513696184</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>421.33721368133814</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>423.3975860955361</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>425.24915237955594</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>426.8919125333976</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>428.32586655706103</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>429.55101445054623</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>430.56735621385326</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>431.37489184698205</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>431.97362134993267</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>432.36354472270494</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>432.5446619652991</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>432.51697307771502</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>432.28047805995277</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>431.83517691201234</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>431.18106963389363</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>430.31815622559674</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>429.24643668712156</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>427.9659110184682</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>426.47657921963673</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>424.77844129062703</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>422.87149723143909</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>420.75574704207293</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>418.43119072252853</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>415.89782827280578</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>413.15565969290515</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>410.20468498282605</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>407.04490414256895</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>403.67631717213339</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>400.09892407151972</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>396.31272484072792</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>392.31771947975778</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>388.11390798860964</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>383.70129036728304</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>379.07986661577843</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>374.24963673409547</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>369.21060072223418</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>363.96275858019499</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>358.50611030797734</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>352.8406559055818</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>346.96639537300769</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>340.88332871025568</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>334.59145591732511</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>328.09077699421641</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>321.38129194092971</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>314.46300075746467</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>307.33590344382151</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-7DF7-44AC-A0A5-8B3CD2631530}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>target</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent4">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:marker>
+              <c:symbol val="triangle"/>
+              <c:size val="8"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:srgbClr val="FFC000"/>
+                </a:solidFill>
+                <a:ln>
+                  <a:solidFill>
+                    <a:srgbClr val="FFC000"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst>
+                  <a:glow rad="63500">
+                    <a:schemeClr val="accent4">
+                      <a:satMod val="175000"/>
+                      <a:alpha val="25000"/>
+                    </a:schemeClr>
+                  </a:glow>
+                </a:effectLst>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-7DF7-44AC-A0A5-8B3CD2631530}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.3635855758993981E-3"/>
+                  <c:y val="-4.4805144970913792E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:r>
+                      <a:rPr lang="en-US"/>
+                      <a:t>X,</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> Y</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-7DF7-44AC-A0A5-8B3CD2631530}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>[1]Sheet3!$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>[1]Sheet3!$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-7DF7-44AC-A0A5-8B3CD2631530}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2003197247"/>
+        <c:axId val="2003198207"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2003197247"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>x/m</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:noFill/>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2003198207"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2003198207"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>y</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> above launch height/m</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2003197247"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18973812167709803"/>
+          <c:y val="9.0019641584537027E-2"/>
+          <c:w val="0.67410736393799819"/>
+          <c:h val="7.4503832716274712E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinearReversed" id="25">
   <a:schemeClr val="accent5"/>
@@ -2884,6 +5551,46 @@
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent3"/>
   <a:schemeClr val="accent5"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -3992,6 +6699,544 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -4078,6 +7323,49 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C51CC8B-809C-4B64-9525-C95DDF1E8104}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -7357,7 +10645,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Red Violet">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -7365,34 +10653,34 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="454551"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="D8D9DC"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="E32D91"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="C830CC"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="4EA6DC"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="4775E7"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="8971E1"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="D54773"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="6B9F25"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="8C8C8C"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -19422,5 +22710,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>